<commit_message>
Checkpoint before assistant change: Fix Excel export error by adjusting data row insertion
Replit-Commit-Author: Assistant
</commit_message>
<xml_diff>
--- a/src/template/template.xlsx
+++ b/src/template/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiennm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700B7B4B-A648-465A-B1AA-3DD653612EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F48235-4F43-4A2D-BDAC-CD3BB12D3CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01.Summary" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Số giờ làm thêm từ T2-T7</t>
   </si>
@@ -109,27 +109,14 @@
   <si>
     <t>Tổng số</t>
   </si>
-  <si>
-    <t>Người tổng hợp</t>
-  </si>
-  <si>
-    <t>Trưởng Bộ phận</t>
-  </si>
-  <si>
-    <t>TienNM</t>
-  </si>
-  <si>
-    <t>NghiaNH</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0_ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -143,33 +130,39 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000080"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -216,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -269,14 +262,42 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -284,23 +305,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -308,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -357,53 +378,44 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,10 +634,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:Z977"/>
+  <dimension ref="A1:Z849"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -675,17 +687,17 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="35"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="4"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -914,23 +926,23 @@
       <c r="Z7" s="19"/>
     </row>
     <row r="8" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
@@ -942,23 +954,52 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
+      <c r="A9" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31">
+        <f>SUM(G8:G8)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="31">
+        <f t="shared" ref="H9:M9" si="0">SUM(H8:H8)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="33">
+        <f>SUM(P8:P8)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="33">
+        <f>SUM(Q8:Q8)</f>
+        <v>0</v>
+      </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
@@ -969,24 +1010,24 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
+    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
@@ -997,24 +1038,24 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
+    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
@@ -1025,297 +1066,257 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="26">
-        <f t="shared" ref="G12:M12" si="0">SUM(G8:G11)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="27"/>
-      <c r="O12" s="24" t="str">
-        <f t="shared" ref="O8:O12" si="1">IF(LEN(N12)&gt;0,HYPERLINK("#'" &amp; N12 &amp; "'!A1","Link"),"")</f>
-        <v/>
-      </c>
-      <c r="P12" s="28">
-        <f t="shared" ref="P12:Q12" si="2">SUM(P8:P11)</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
+    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="11"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
     </row>
     <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
@@ -1376,11 +1377,11 @@
     <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="7"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="7"/>
+      <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -24529,3597 +24530,13 @@
       <c r="Y849" s="2"/>
       <c r="Z849" s="2"/>
     </row>
-    <row r="850" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A850" s="11"/>
-      <c r="B850" s="2"/>
-      <c r="C850" s="2"/>
-      <c r="D850" s="2"/>
-      <c r="E850" s="2"/>
-      <c r="F850" s="2"/>
-      <c r="G850" s="2"/>
-      <c r="H850" s="2"/>
-      <c r="I850" s="2"/>
-      <c r="J850" s="2"/>
-      <c r="K850" s="2"/>
-      <c r="L850" s="2"/>
-      <c r="M850" s="2"/>
-      <c r="N850" s="2"/>
-      <c r="O850" s="2"/>
-      <c r="P850" s="3"/>
-      <c r="Q850" s="3"/>
-      <c r="R850" s="2"/>
-      <c r="S850" s="2"/>
-      <c r="T850" s="2"/>
-      <c r="U850" s="2"/>
-      <c r="V850" s="2"/>
-      <c r="W850" s="2"/>
-      <c r="X850" s="2"/>
-      <c r="Y850" s="2"/>
-      <c r="Z850" s="2"/>
-    </row>
-    <row r="851" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A851" s="11"/>
-      <c r="B851" s="2"/>
-      <c r="C851" s="2"/>
-      <c r="D851" s="2"/>
-      <c r="E851" s="2"/>
-      <c r="F851" s="2"/>
-      <c r="G851" s="2"/>
-      <c r="H851" s="2"/>
-      <c r="I851" s="2"/>
-      <c r="J851" s="2"/>
-      <c r="K851" s="2"/>
-      <c r="L851" s="2"/>
-      <c r="M851" s="2"/>
-      <c r="N851" s="2"/>
-      <c r="O851" s="2"/>
-      <c r="P851" s="3"/>
-      <c r="Q851" s="3"/>
-      <c r="R851" s="2"/>
-      <c r="S851" s="2"/>
-      <c r="T851" s="2"/>
-      <c r="U851" s="2"/>
-      <c r="V851" s="2"/>
-      <c r="W851" s="2"/>
-      <c r="X851" s="2"/>
-      <c r="Y851" s="2"/>
-      <c r="Z851" s="2"/>
-    </row>
-    <row r="852" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A852" s="11"/>
-      <c r="B852" s="2"/>
-      <c r="C852" s="2"/>
-      <c r="D852" s="2"/>
-      <c r="E852" s="2"/>
-      <c r="F852" s="2"/>
-      <c r="G852" s="2"/>
-      <c r="H852" s="2"/>
-      <c r="I852" s="2"/>
-      <c r="J852" s="2"/>
-      <c r="K852" s="2"/>
-      <c r="L852" s="2"/>
-      <c r="M852" s="2"/>
-      <c r="N852" s="2"/>
-      <c r="O852" s="2"/>
-      <c r="P852" s="3"/>
-      <c r="Q852" s="3"/>
-      <c r="R852" s="2"/>
-      <c r="S852" s="2"/>
-      <c r="T852" s="2"/>
-      <c r="U852" s="2"/>
-      <c r="V852" s="2"/>
-      <c r="W852" s="2"/>
-      <c r="X852" s="2"/>
-      <c r="Y852" s="2"/>
-      <c r="Z852" s="2"/>
-    </row>
-    <row r="853" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A853" s="11"/>
-      <c r="B853" s="2"/>
-      <c r="C853" s="2"/>
-      <c r="D853" s="2"/>
-      <c r="E853" s="2"/>
-      <c r="F853" s="2"/>
-      <c r="G853" s="2"/>
-      <c r="H853" s="2"/>
-      <c r="I853" s="2"/>
-      <c r="J853" s="2"/>
-      <c r="K853" s="2"/>
-      <c r="L853" s="2"/>
-      <c r="M853" s="2"/>
-      <c r="N853" s="2"/>
-      <c r="O853" s="2"/>
-      <c r="P853" s="3"/>
-      <c r="Q853" s="3"/>
-      <c r="R853" s="2"/>
-      <c r="S853" s="2"/>
-      <c r="T853" s="2"/>
-      <c r="U853" s="2"/>
-      <c r="V853" s="2"/>
-      <c r="W853" s="2"/>
-      <c r="X853" s="2"/>
-      <c r="Y853" s="2"/>
-      <c r="Z853" s="2"/>
-    </row>
-    <row r="854" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A854" s="11"/>
-      <c r="B854" s="2"/>
-      <c r="C854" s="2"/>
-      <c r="D854" s="2"/>
-      <c r="E854" s="2"/>
-      <c r="F854" s="2"/>
-      <c r="G854" s="2"/>
-      <c r="H854" s="2"/>
-      <c r="I854" s="2"/>
-      <c r="J854" s="2"/>
-      <c r="K854" s="2"/>
-      <c r="L854" s="2"/>
-      <c r="M854" s="2"/>
-      <c r="N854" s="2"/>
-      <c r="O854" s="2"/>
-      <c r="P854" s="3"/>
-      <c r="Q854" s="3"/>
-      <c r="R854" s="2"/>
-      <c r="S854" s="2"/>
-      <c r="T854" s="2"/>
-      <c r="U854" s="2"/>
-      <c r="V854" s="2"/>
-      <c r="W854" s="2"/>
-      <c r="X854" s="2"/>
-      <c r="Y854" s="2"/>
-      <c r="Z854" s="2"/>
-    </row>
-    <row r="855" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A855" s="11"/>
-      <c r="B855" s="2"/>
-      <c r="C855" s="2"/>
-      <c r="D855" s="2"/>
-      <c r="E855" s="2"/>
-      <c r="F855" s="2"/>
-      <c r="G855" s="2"/>
-      <c r="H855" s="2"/>
-      <c r="I855" s="2"/>
-      <c r="J855" s="2"/>
-      <c r="K855" s="2"/>
-      <c r="L855" s="2"/>
-      <c r="M855" s="2"/>
-      <c r="N855" s="2"/>
-      <c r="O855" s="2"/>
-      <c r="P855" s="3"/>
-      <c r="Q855" s="3"/>
-      <c r="R855" s="2"/>
-      <c r="S855" s="2"/>
-      <c r="T855" s="2"/>
-      <c r="U855" s="2"/>
-      <c r="V855" s="2"/>
-      <c r="W855" s="2"/>
-      <c r="X855" s="2"/>
-      <c r="Y855" s="2"/>
-      <c r="Z855" s="2"/>
-    </row>
-    <row r="856" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A856" s="11"/>
-      <c r="B856" s="2"/>
-      <c r="C856" s="2"/>
-      <c r="D856" s="2"/>
-      <c r="E856" s="2"/>
-      <c r="F856" s="2"/>
-      <c r="G856" s="2"/>
-      <c r="H856" s="2"/>
-      <c r="I856" s="2"/>
-      <c r="J856" s="2"/>
-      <c r="K856" s="2"/>
-      <c r="L856" s="2"/>
-      <c r="M856" s="2"/>
-      <c r="N856" s="2"/>
-      <c r="O856" s="2"/>
-      <c r="P856" s="3"/>
-      <c r="Q856" s="3"/>
-      <c r="R856" s="2"/>
-      <c r="S856" s="2"/>
-      <c r="T856" s="2"/>
-      <c r="U856" s="2"/>
-      <c r="V856" s="2"/>
-      <c r="W856" s="2"/>
-      <c r="X856" s="2"/>
-      <c r="Y856" s="2"/>
-      <c r="Z856" s="2"/>
-    </row>
-    <row r="857" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A857" s="11"/>
-      <c r="B857" s="2"/>
-      <c r="C857" s="2"/>
-      <c r="D857" s="2"/>
-      <c r="E857" s="2"/>
-      <c r="F857" s="2"/>
-      <c r="G857" s="2"/>
-      <c r="H857" s="2"/>
-      <c r="I857" s="2"/>
-      <c r="J857" s="2"/>
-      <c r="K857" s="2"/>
-      <c r="L857" s="2"/>
-      <c r="M857" s="2"/>
-      <c r="N857" s="2"/>
-      <c r="O857" s="2"/>
-      <c r="P857" s="3"/>
-      <c r="Q857" s="3"/>
-      <c r="R857" s="2"/>
-      <c r="S857" s="2"/>
-      <c r="T857" s="2"/>
-      <c r="U857" s="2"/>
-      <c r="V857" s="2"/>
-      <c r="W857" s="2"/>
-      <c r="X857" s="2"/>
-      <c r="Y857" s="2"/>
-      <c r="Z857" s="2"/>
-    </row>
-    <row r="858" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A858" s="11"/>
-      <c r="B858" s="2"/>
-      <c r="C858" s="2"/>
-      <c r="D858" s="2"/>
-      <c r="E858" s="2"/>
-      <c r="F858" s="2"/>
-      <c r="G858" s="2"/>
-      <c r="H858" s="2"/>
-      <c r="I858" s="2"/>
-      <c r="J858" s="2"/>
-      <c r="K858" s="2"/>
-      <c r="L858" s="2"/>
-      <c r="M858" s="2"/>
-      <c r="N858" s="2"/>
-      <c r="O858" s="2"/>
-      <c r="P858" s="3"/>
-      <c r="Q858" s="3"/>
-      <c r="R858" s="2"/>
-      <c r="S858" s="2"/>
-      <c r="T858" s="2"/>
-      <c r="U858" s="2"/>
-      <c r="V858" s="2"/>
-      <c r="W858" s="2"/>
-      <c r="X858" s="2"/>
-      <c r="Y858" s="2"/>
-      <c r="Z858" s="2"/>
-    </row>
-    <row r="859" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A859" s="11"/>
-      <c r="B859" s="2"/>
-      <c r="C859" s="2"/>
-      <c r="D859" s="2"/>
-      <c r="E859" s="2"/>
-      <c r="F859" s="2"/>
-      <c r="G859" s="2"/>
-      <c r="H859" s="2"/>
-      <c r="I859" s="2"/>
-      <c r="J859" s="2"/>
-      <c r="K859" s="2"/>
-      <c r="L859" s="2"/>
-      <c r="M859" s="2"/>
-      <c r="N859" s="2"/>
-      <c r="O859" s="2"/>
-      <c r="P859" s="3"/>
-      <c r="Q859" s="3"/>
-      <c r="R859" s="2"/>
-      <c r="S859" s="2"/>
-      <c r="T859" s="2"/>
-      <c r="U859" s="2"/>
-      <c r="V859" s="2"/>
-      <c r="W859" s="2"/>
-      <c r="X859" s="2"/>
-      <c r="Y859" s="2"/>
-      <c r="Z859" s="2"/>
-    </row>
-    <row r="860" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A860" s="11"/>
-      <c r="B860" s="2"/>
-      <c r="C860" s="2"/>
-      <c r="D860" s="2"/>
-      <c r="E860" s="2"/>
-      <c r="F860" s="2"/>
-      <c r="G860" s="2"/>
-      <c r="H860" s="2"/>
-      <c r="I860" s="2"/>
-      <c r="J860" s="2"/>
-      <c r="K860" s="2"/>
-      <c r="L860" s="2"/>
-      <c r="M860" s="2"/>
-      <c r="N860" s="2"/>
-      <c r="O860" s="2"/>
-      <c r="P860" s="3"/>
-      <c r="Q860" s="3"/>
-      <c r="R860" s="2"/>
-      <c r="S860" s="2"/>
-      <c r="T860" s="2"/>
-      <c r="U860" s="2"/>
-      <c r="V860" s="2"/>
-      <c r="W860" s="2"/>
-      <c r="X860" s="2"/>
-      <c r="Y860" s="2"/>
-      <c r="Z860" s="2"/>
-    </row>
-    <row r="861" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A861" s="11"/>
-      <c r="B861" s="2"/>
-      <c r="C861" s="2"/>
-      <c r="D861" s="2"/>
-      <c r="E861" s="2"/>
-      <c r="F861" s="2"/>
-      <c r="G861" s="2"/>
-      <c r="H861" s="2"/>
-      <c r="I861" s="2"/>
-      <c r="J861" s="2"/>
-      <c r="K861" s="2"/>
-      <c r="L861" s="2"/>
-      <c r="M861" s="2"/>
-      <c r="N861" s="2"/>
-      <c r="O861" s="2"/>
-      <c r="P861" s="3"/>
-      <c r="Q861" s="3"/>
-      <c r="R861" s="2"/>
-      <c r="S861" s="2"/>
-      <c r="T861" s="2"/>
-      <c r="U861" s="2"/>
-      <c r="V861" s="2"/>
-      <c r="W861" s="2"/>
-      <c r="X861" s="2"/>
-      <c r="Y861" s="2"/>
-      <c r="Z861" s="2"/>
-    </row>
-    <row r="862" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A862" s="11"/>
-      <c r="B862" s="2"/>
-      <c r="C862" s="2"/>
-      <c r="D862" s="2"/>
-      <c r="E862" s="2"/>
-      <c r="F862" s="2"/>
-      <c r="G862" s="2"/>
-      <c r="H862" s="2"/>
-      <c r="I862" s="2"/>
-      <c r="J862" s="2"/>
-      <c r="K862" s="2"/>
-      <c r="L862" s="2"/>
-      <c r="M862" s="2"/>
-      <c r="N862" s="2"/>
-      <c r="O862" s="2"/>
-      <c r="P862" s="3"/>
-      <c r="Q862" s="3"/>
-      <c r="R862" s="2"/>
-      <c r="S862" s="2"/>
-      <c r="T862" s="2"/>
-      <c r="U862" s="2"/>
-      <c r="V862" s="2"/>
-      <c r="W862" s="2"/>
-      <c r="X862" s="2"/>
-      <c r="Y862" s="2"/>
-      <c r="Z862" s="2"/>
-    </row>
-    <row r="863" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A863" s="11"/>
-      <c r="B863" s="2"/>
-      <c r="C863" s="2"/>
-      <c r="D863" s="2"/>
-      <c r="E863" s="2"/>
-      <c r="F863" s="2"/>
-      <c r="G863" s="2"/>
-      <c r="H863" s="2"/>
-      <c r="I863" s="2"/>
-      <c r="J863" s="2"/>
-      <c r="K863" s="2"/>
-      <c r="L863" s="2"/>
-      <c r="M863" s="2"/>
-      <c r="N863" s="2"/>
-      <c r="O863" s="2"/>
-      <c r="P863" s="3"/>
-      <c r="Q863" s="3"/>
-      <c r="R863" s="2"/>
-      <c r="S863" s="2"/>
-      <c r="T863" s="2"/>
-      <c r="U863" s="2"/>
-      <c r="V863" s="2"/>
-      <c r="W863" s="2"/>
-      <c r="X863" s="2"/>
-      <c r="Y863" s="2"/>
-      <c r="Z863" s="2"/>
-    </row>
-    <row r="864" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A864" s="11"/>
-      <c r="B864" s="2"/>
-      <c r="C864" s="2"/>
-      <c r="D864" s="2"/>
-      <c r="E864" s="2"/>
-      <c r="F864" s="2"/>
-      <c r="G864" s="2"/>
-      <c r="H864" s="2"/>
-      <c r="I864" s="2"/>
-      <c r="J864" s="2"/>
-      <c r="K864" s="2"/>
-      <c r="L864" s="2"/>
-      <c r="M864" s="2"/>
-      <c r="N864" s="2"/>
-      <c r="O864" s="2"/>
-      <c r="P864" s="3"/>
-      <c r="Q864" s="3"/>
-      <c r="R864" s="2"/>
-      <c r="S864" s="2"/>
-      <c r="T864" s="2"/>
-      <c r="U864" s="2"/>
-      <c r="V864" s="2"/>
-      <c r="W864" s="2"/>
-      <c r="X864" s="2"/>
-      <c r="Y864" s="2"/>
-      <c r="Z864" s="2"/>
-    </row>
-    <row r="865" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A865" s="11"/>
-      <c r="B865" s="2"/>
-      <c r="C865" s="2"/>
-      <c r="D865" s="2"/>
-      <c r="E865" s="2"/>
-      <c r="F865" s="2"/>
-      <c r="G865" s="2"/>
-      <c r="H865" s="2"/>
-      <c r="I865" s="2"/>
-      <c r="J865" s="2"/>
-      <c r="K865" s="2"/>
-      <c r="L865" s="2"/>
-      <c r="M865" s="2"/>
-      <c r="N865" s="2"/>
-      <c r="O865" s="2"/>
-      <c r="P865" s="3"/>
-      <c r="Q865" s="3"/>
-      <c r="R865" s="2"/>
-      <c r="S865" s="2"/>
-      <c r="T865" s="2"/>
-      <c r="U865" s="2"/>
-      <c r="V865" s="2"/>
-      <c r="W865" s="2"/>
-      <c r="X865" s="2"/>
-      <c r="Y865" s="2"/>
-      <c r="Z865" s="2"/>
-    </row>
-    <row r="866" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A866" s="11"/>
-      <c r="B866" s="2"/>
-      <c r="C866" s="2"/>
-      <c r="D866" s="2"/>
-      <c r="E866" s="2"/>
-      <c r="F866" s="2"/>
-      <c r="G866" s="2"/>
-      <c r="H866" s="2"/>
-      <c r="I866" s="2"/>
-      <c r="J866" s="2"/>
-      <c r="K866" s="2"/>
-      <c r="L866" s="2"/>
-      <c r="M866" s="2"/>
-      <c r="N866" s="2"/>
-      <c r="O866" s="2"/>
-      <c r="P866" s="3"/>
-      <c r="Q866" s="3"/>
-      <c r="R866" s="2"/>
-      <c r="S866" s="2"/>
-      <c r="T866" s="2"/>
-      <c r="U866" s="2"/>
-      <c r="V866" s="2"/>
-      <c r="W866" s="2"/>
-      <c r="X866" s="2"/>
-      <c r="Y866" s="2"/>
-      <c r="Z866" s="2"/>
-    </row>
-    <row r="867" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A867" s="11"/>
-      <c r="B867" s="2"/>
-      <c r="C867" s="2"/>
-      <c r="D867" s="2"/>
-      <c r="E867" s="2"/>
-      <c r="F867" s="2"/>
-      <c r="G867" s="2"/>
-      <c r="H867" s="2"/>
-      <c r="I867" s="2"/>
-      <c r="J867" s="2"/>
-      <c r="K867" s="2"/>
-      <c r="L867" s="2"/>
-      <c r="M867" s="2"/>
-      <c r="N867" s="2"/>
-      <c r="O867" s="2"/>
-      <c r="P867" s="3"/>
-      <c r="Q867" s="3"/>
-      <c r="R867" s="2"/>
-      <c r="S867" s="2"/>
-      <c r="T867" s="2"/>
-      <c r="U867" s="2"/>
-      <c r="V867" s="2"/>
-      <c r="W867" s="2"/>
-      <c r="X867" s="2"/>
-      <c r="Y867" s="2"/>
-      <c r="Z867" s="2"/>
-    </row>
-    <row r="868" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A868" s="11"/>
-      <c r="B868" s="2"/>
-      <c r="C868" s="2"/>
-      <c r="D868" s="2"/>
-      <c r="E868" s="2"/>
-      <c r="F868" s="2"/>
-      <c r="G868" s="2"/>
-      <c r="H868" s="2"/>
-      <c r="I868" s="2"/>
-      <c r="J868" s="2"/>
-      <c r="K868" s="2"/>
-      <c r="L868" s="2"/>
-      <c r="M868" s="2"/>
-      <c r="N868" s="2"/>
-      <c r="O868" s="2"/>
-      <c r="P868" s="3"/>
-      <c r="Q868" s="3"/>
-      <c r="R868" s="2"/>
-      <c r="S868" s="2"/>
-      <c r="T868" s="2"/>
-      <c r="U868" s="2"/>
-      <c r="V868" s="2"/>
-      <c r="W868" s="2"/>
-      <c r="X868" s="2"/>
-      <c r="Y868" s="2"/>
-      <c r="Z868" s="2"/>
-    </row>
-    <row r="869" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A869" s="11"/>
-      <c r="B869" s="2"/>
-      <c r="C869" s="2"/>
-      <c r="D869" s="2"/>
-      <c r="E869" s="2"/>
-      <c r="F869" s="2"/>
-      <c r="G869" s="2"/>
-      <c r="H869" s="2"/>
-      <c r="I869" s="2"/>
-      <c r="J869" s="2"/>
-      <c r="K869" s="2"/>
-      <c r="L869" s="2"/>
-      <c r="M869" s="2"/>
-      <c r="N869" s="2"/>
-      <c r="O869" s="2"/>
-      <c r="P869" s="3"/>
-      <c r="Q869" s="3"/>
-      <c r="R869" s="2"/>
-      <c r="S869" s="2"/>
-      <c r="T869" s="2"/>
-      <c r="U869" s="2"/>
-      <c r="V869" s="2"/>
-      <c r="W869" s="2"/>
-      <c r="X869" s="2"/>
-      <c r="Y869" s="2"/>
-      <c r="Z869" s="2"/>
-    </row>
-    <row r="870" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A870" s="11"/>
-      <c r="B870" s="2"/>
-      <c r="C870" s="2"/>
-      <c r="D870" s="2"/>
-      <c r="E870" s="2"/>
-      <c r="F870" s="2"/>
-      <c r="G870" s="2"/>
-      <c r="H870" s="2"/>
-      <c r="I870" s="2"/>
-      <c r="J870" s="2"/>
-      <c r="K870" s="2"/>
-      <c r="L870" s="2"/>
-      <c r="M870" s="2"/>
-      <c r="N870" s="2"/>
-      <c r="O870" s="2"/>
-      <c r="P870" s="3"/>
-      <c r="Q870" s="3"/>
-      <c r="R870" s="2"/>
-      <c r="S870" s="2"/>
-      <c r="T870" s="2"/>
-      <c r="U870" s="2"/>
-      <c r="V870" s="2"/>
-      <c r="W870" s="2"/>
-      <c r="X870" s="2"/>
-      <c r="Y870" s="2"/>
-      <c r="Z870" s="2"/>
-    </row>
-    <row r="871" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A871" s="11"/>
-      <c r="B871" s="2"/>
-      <c r="C871" s="2"/>
-      <c r="D871" s="2"/>
-      <c r="E871" s="2"/>
-      <c r="F871" s="2"/>
-      <c r="G871" s="2"/>
-      <c r="H871" s="2"/>
-      <c r="I871" s="2"/>
-      <c r="J871" s="2"/>
-      <c r="K871" s="2"/>
-      <c r="L871" s="2"/>
-      <c r="M871" s="2"/>
-      <c r="N871" s="2"/>
-      <c r="O871" s="2"/>
-      <c r="P871" s="3"/>
-      <c r="Q871" s="3"/>
-      <c r="R871" s="2"/>
-      <c r="S871" s="2"/>
-      <c r="T871" s="2"/>
-      <c r="U871" s="2"/>
-      <c r="V871" s="2"/>
-      <c r="W871" s="2"/>
-      <c r="X871" s="2"/>
-      <c r="Y871" s="2"/>
-      <c r="Z871" s="2"/>
-    </row>
-    <row r="872" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A872" s="11"/>
-      <c r="B872" s="2"/>
-      <c r="C872" s="2"/>
-      <c r="D872" s="2"/>
-      <c r="E872" s="2"/>
-      <c r="F872" s="2"/>
-      <c r="G872" s="2"/>
-      <c r="H872" s="2"/>
-      <c r="I872" s="2"/>
-      <c r="J872" s="2"/>
-      <c r="K872" s="2"/>
-      <c r="L872" s="2"/>
-      <c r="M872" s="2"/>
-      <c r="N872" s="2"/>
-      <c r="O872" s="2"/>
-      <c r="P872" s="3"/>
-      <c r="Q872" s="3"/>
-      <c r="R872" s="2"/>
-      <c r="S872" s="2"/>
-      <c r="T872" s="2"/>
-      <c r="U872" s="2"/>
-      <c r="V872" s="2"/>
-      <c r="W872" s="2"/>
-      <c r="X872" s="2"/>
-      <c r="Y872" s="2"/>
-      <c r="Z872" s="2"/>
-    </row>
-    <row r="873" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A873" s="11"/>
-      <c r="B873" s="2"/>
-      <c r="C873" s="2"/>
-      <c r="D873" s="2"/>
-      <c r="E873" s="2"/>
-      <c r="F873" s="2"/>
-      <c r="G873" s="2"/>
-      <c r="H873" s="2"/>
-      <c r="I873" s="2"/>
-      <c r="J873" s="2"/>
-      <c r="K873" s="2"/>
-      <c r="L873" s="2"/>
-      <c r="M873" s="2"/>
-      <c r="N873" s="2"/>
-      <c r="O873" s="2"/>
-      <c r="P873" s="3"/>
-      <c r="Q873" s="3"/>
-      <c r="R873" s="2"/>
-      <c r="S873" s="2"/>
-      <c r="T873" s="2"/>
-      <c r="U873" s="2"/>
-      <c r="V873" s="2"/>
-      <c r="W873" s="2"/>
-      <c r="X873" s="2"/>
-      <c r="Y873" s="2"/>
-      <c r="Z873" s="2"/>
-    </row>
-    <row r="874" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A874" s="11"/>
-      <c r="B874" s="2"/>
-      <c r="C874" s="2"/>
-      <c r="D874" s="2"/>
-      <c r="E874" s="2"/>
-      <c r="F874" s="2"/>
-      <c r="G874" s="2"/>
-      <c r="H874" s="2"/>
-      <c r="I874" s="2"/>
-      <c r="J874" s="2"/>
-      <c r="K874" s="2"/>
-      <c r="L874" s="2"/>
-      <c r="M874" s="2"/>
-      <c r="N874" s="2"/>
-      <c r="O874" s="2"/>
-      <c r="P874" s="3"/>
-      <c r="Q874" s="3"/>
-      <c r="R874" s="2"/>
-      <c r="S874" s="2"/>
-      <c r="T874" s="2"/>
-      <c r="U874" s="2"/>
-      <c r="V874" s="2"/>
-      <c r="W874" s="2"/>
-      <c r="X874" s="2"/>
-      <c r="Y874" s="2"/>
-      <c r="Z874" s="2"/>
-    </row>
-    <row r="875" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A875" s="11"/>
-      <c r="B875" s="2"/>
-      <c r="C875" s="2"/>
-      <c r="D875" s="2"/>
-      <c r="E875" s="2"/>
-      <c r="F875" s="2"/>
-      <c r="G875" s="2"/>
-      <c r="H875" s="2"/>
-      <c r="I875" s="2"/>
-      <c r="J875" s="2"/>
-      <c r="K875" s="2"/>
-      <c r="L875" s="2"/>
-      <c r="M875" s="2"/>
-      <c r="N875" s="2"/>
-      <c r="O875" s="2"/>
-      <c r="P875" s="3"/>
-      <c r="Q875" s="3"/>
-      <c r="R875" s="2"/>
-      <c r="S875" s="2"/>
-      <c r="T875" s="2"/>
-      <c r="U875" s="2"/>
-      <c r="V875" s="2"/>
-      <c r="W875" s="2"/>
-      <c r="X875" s="2"/>
-      <c r="Y875" s="2"/>
-      <c r="Z875" s="2"/>
-    </row>
-    <row r="876" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A876" s="11"/>
-      <c r="B876" s="2"/>
-      <c r="C876" s="2"/>
-      <c r="D876" s="2"/>
-      <c r="E876" s="2"/>
-      <c r="F876" s="2"/>
-      <c r="G876" s="2"/>
-      <c r="H876" s="2"/>
-      <c r="I876" s="2"/>
-      <c r="J876" s="2"/>
-      <c r="K876" s="2"/>
-      <c r="L876" s="2"/>
-      <c r="M876" s="2"/>
-      <c r="N876" s="2"/>
-      <c r="O876" s="2"/>
-      <c r="P876" s="3"/>
-      <c r="Q876" s="3"/>
-      <c r="R876" s="2"/>
-      <c r="S876" s="2"/>
-      <c r="T876" s="2"/>
-      <c r="U876" s="2"/>
-      <c r="V876" s="2"/>
-      <c r="W876" s="2"/>
-      <c r="X876" s="2"/>
-      <c r="Y876" s="2"/>
-      <c r="Z876" s="2"/>
-    </row>
-    <row r="877" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A877" s="11"/>
-      <c r="B877" s="2"/>
-      <c r="C877" s="2"/>
-      <c r="D877" s="2"/>
-      <c r="E877" s="2"/>
-      <c r="F877" s="2"/>
-      <c r="G877" s="2"/>
-      <c r="H877" s="2"/>
-      <c r="I877" s="2"/>
-      <c r="J877" s="2"/>
-      <c r="K877" s="2"/>
-      <c r="L877" s="2"/>
-      <c r="M877" s="2"/>
-      <c r="N877" s="2"/>
-      <c r="O877" s="2"/>
-      <c r="P877" s="3"/>
-      <c r="Q877" s="3"/>
-      <c r="R877" s="2"/>
-      <c r="S877" s="2"/>
-      <c r="T877" s="2"/>
-      <c r="U877" s="2"/>
-      <c r="V877" s="2"/>
-      <c r="W877" s="2"/>
-      <c r="X877" s="2"/>
-      <c r="Y877" s="2"/>
-      <c r="Z877" s="2"/>
-    </row>
-    <row r="878" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A878" s="11"/>
-      <c r="B878" s="2"/>
-      <c r="C878" s="2"/>
-      <c r="D878" s="2"/>
-      <c r="E878" s="2"/>
-      <c r="F878" s="2"/>
-      <c r="G878" s="2"/>
-      <c r="H878" s="2"/>
-      <c r="I878" s="2"/>
-      <c r="J878" s="2"/>
-      <c r="K878" s="2"/>
-      <c r="L878" s="2"/>
-      <c r="M878" s="2"/>
-      <c r="N878" s="2"/>
-      <c r="O878" s="2"/>
-      <c r="P878" s="3"/>
-      <c r="Q878" s="3"/>
-      <c r="R878" s="2"/>
-      <c r="S878" s="2"/>
-      <c r="T878" s="2"/>
-      <c r="U878" s="2"/>
-      <c r="V878" s="2"/>
-      <c r="W878" s="2"/>
-      <c r="X878" s="2"/>
-      <c r="Y878" s="2"/>
-      <c r="Z878" s="2"/>
-    </row>
-    <row r="879" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A879" s="11"/>
-      <c r="B879" s="2"/>
-      <c r="C879" s="2"/>
-      <c r="D879" s="2"/>
-      <c r="E879" s="2"/>
-      <c r="F879" s="2"/>
-      <c r="G879" s="2"/>
-      <c r="H879" s="2"/>
-      <c r="I879" s="2"/>
-      <c r="J879" s="2"/>
-      <c r="K879" s="2"/>
-      <c r="L879" s="2"/>
-      <c r="M879" s="2"/>
-      <c r="N879" s="2"/>
-      <c r="O879" s="2"/>
-      <c r="P879" s="3"/>
-      <c r="Q879" s="3"/>
-      <c r="R879" s="2"/>
-      <c r="S879" s="2"/>
-      <c r="T879" s="2"/>
-      <c r="U879" s="2"/>
-      <c r="V879" s="2"/>
-      <c r="W879" s="2"/>
-      <c r="X879" s="2"/>
-      <c r="Y879" s="2"/>
-      <c r="Z879" s="2"/>
-    </row>
-    <row r="880" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A880" s="11"/>
-      <c r="B880" s="2"/>
-      <c r="C880" s="2"/>
-      <c r="D880" s="2"/>
-      <c r="E880" s="2"/>
-      <c r="F880" s="2"/>
-      <c r="G880" s="2"/>
-      <c r="H880" s="2"/>
-      <c r="I880" s="2"/>
-      <c r="J880" s="2"/>
-      <c r="K880" s="2"/>
-      <c r="L880" s="2"/>
-      <c r="M880" s="2"/>
-      <c r="N880" s="2"/>
-      <c r="O880" s="2"/>
-      <c r="P880" s="3"/>
-      <c r="Q880" s="3"/>
-      <c r="R880" s="2"/>
-      <c r="S880" s="2"/>
-      <c r="T880" s="2"/>
-      <c r="U880" s="2"/>
-      <c r="V880" s="2"/>
-      <c r="W880" s="2"/>
-      <c r="X880" s="2"/>
-      <c r="Y880" s="2"/>
-      <c r="Z880" s="2"/>
-    </row>
-    <row r="881" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A881" s="11"/>
-      <c r="B881" s="2"/>
-      <c r="C881" s="2"/>
-      <c r="D881" s="2"/>
-      <c r="E881" s="2"/>
-      <c r="F881" s="2"/>
-      <c r="G881" s="2"/>
-      <c r="H881" s="2"/>
-      <c r="I881" s="2"/>
-      <c r="J881" s="2"/>
-      <c r="K881" s="2"/>
-      <c r="L881" s="2"/>
-      <c r="M881" s="2"/>
-      <c r="N881" s="2"/>
-      <c r="O881" s="2"/>
-      <c r="P881" s="3"/>
-      <c r="Q881" s="3"/>
-      <c r="R881" s="2"/>
-      <c r="S881" s="2"/>
-      <c r="T881" s="2"/>
-      <c r="U881" s="2"/>
-      <c r="V881" s="2"/>
-      <c r="W881" s="2"/>
-      <c r="X881" s="2"/>
-      <c r="Y881" s="2"/>
-      <c r="Z881" s="2"/>
-    </row>
-    <row r="882" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A882" s="11"/>
-      <c r="B882" s="2"/>
-      <c r="C882" s="2"/>
-      <c r="D882" s="2"/>
-      <c r="E882" s="2"/>
-      <c r="F882" s="2"/>
-      <c r="G882" s="2"/>
-      <c r="H882" s="2"/>
-      <c r="I882" s="2"/>
-      <c r="J882" s="2"/>
-      <c r="K882" s="2"/>
-      <c r="L882" s="2"/>
-      <c r="M882" s="2"/>
-      <c r="N882" s="2"/>
-      <c r="O882" s="2"/>
-      <c r="P882" s="3"/>
-      <c r="Q882" s="3"/>
-      <c r="R882" s="2"/>
-      <c r="S882" s="2"/>
-      <c r="T882" s="2"/>
-      <c r="U882" s="2"/>
-      <c r="V882" s="2"/>
-      <c r="W882" s="2"/>
-      <c r="X882" s="2"/>
-      <c r="Y882" s="2"/>
-      <c r="Z882" s="2"/>
-    </row>
-    <row r="883" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A883" s="11"/>
-      <c r="B883" s="2"/>
-      <c r="C883" s="2"/>
-      <c r="D883" s="2"/>
-      <c r="E883" s="2"/>
-      <c r="F883" s="2"/>
-      <c r="G883" s="2"/>
-      <c r="H883" s="2"/>
-      <c r="I883" s="2"/>
-      <c r="J883" s="2"/>
-      <c r="K883" s="2"/>
-      <c r="L883" s="2"/>
-      <c r="M883" s="2"/>
-      <c r="N883" s="2"/>
-      <c r="O883" s="2"/>
-      <c r="P883" s="3"/>
-      <c r="Q883" s="3"/>
-      <c r="R883" s="2"/>
-      <c r="S883" s="2"/>
-      <c r="T883" s="2"/>
-      <c r="U883" s="2"/>
-      <c r="V883" s="2"/>
-      <c r="W883" s="2"/>
-      <c r="X883" s="2"/>
-      <c r="Y883" s="2"/>
-      <c r="Z883" s="2"/>
-    </row>
-    <row r="884" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A884" s="11"/>
-      <c r="B884" s="2"/>
-      <c r="C884" s="2"/>
-      <c r="D884" s="2"/>
-      <c r="E884" s="2"/>
-      <c r="F884" s="2"/>
-      <c r="G884" s="2"/>
-      <c r="H884" s="2"/>
-      <c r="I884" s="2"/>
-      <c r="J884" s="2"/>
-      <c r="K884" s="2"/>
-      <c r="L884" s="2"/>
-      <c r="M884" s="2"/>
-      <c r="N884" s="2"/>
-      <c r="O884" s="2"/>
-      <c r="P884" s="3"/>
-      <c r="Q884" s="3"/>
-      <c r="R884" s="2"/>
-      <c r="S884" s="2"/>
-      <c r="T884" s="2"/>
-      <c r="U884" s="2"/>
-      <c r="V884" s="2"/>
-      <c r="W884" s="2"/>
-      <c r="X884" s="2"/>
-      <c r="Y884" s="2"/>
-      <c r="Z884" s="2"/>
-    </row>
-    <row r="885" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A885" s="11"/>
-      <c r="B885" s="2"/>
-      <c r="C885" s="2"/>
-      <c r="D885" s="2"/>
-      <c r="E885" s="2"/>
-      <c r="F885" s="2"/>
-      <c r="G885" s="2"/>
-      <c r="H885" s="2"/>
-      <c r="I885" s="2"/>
-      <c r="J885" s="2"/>
-      <c r="K885" s="2"/>
-      <c r="L885" s="2"/>
-      <c r="M885" s="2"/>
-      <c r="N885" s="2"/>
-      <c r="O885" s="2"/>
-      <c r="P885" s="3"/>
-      <c r="Q885" s="3"/>
-      <c r="R885" s="2"/>
-      <c r="S885" s="2"/>
-      <c r="T885" s="2"/>
-      <c r="U885" s="2"/>
-      <c r="V885" s="2"/>
-      <c r="W885" s="2"/>
-      <c r="X885" s="2"/>
-      <c r="Y885" s="2"/>
-      <c r="Z885" s="2"/>
-    </row>
-    <row r="886" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A886" s="11"/>
-      <c r="B886" s="2"/>
-      <c r="C886" s="2"/>
-      <c r="D886" s="2"/>
-      <c r="E886" s="2"/>
-      <c r="F886" s="2"/>
-      <c r="G886" s="2"/>
-      <c r="H886" s="2"/>
-      <c r="I886" s="2"/>
-      <c r="J886" s="2"/>
-      <c r="K886" s="2"/>
-      <c r="L886" s="2"/>
-      <c r="M886" s="2"/>
-      <c r="N886" s="2"/>
-      <c r="O886" s="2"/>
-      <c r="P886" s="3"/>
-      <c r="Q886" s="3"/>
-      <c r="R886" s="2"/>
-      <c r="S886" s="2"/>
-      <c r="T886" s="2"/>
-      <c r="U886" s="2"/>
-      <c r="V886" s="2"/>
-      <c r="W886" s="2"/>
-      <c r="X886" s="2"/>
-      <c r="Y886" s="2"/>
-      <c r="Z886" s="2"/>
-    </row>
-    <row r="887" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A887" s="11"/>
-      <c r="B887" s="2"/>
-      <c r="C887" s="2"/>
-      <c r="D887" s="2"/>
-      <c r="E887" s="2"/>
-      <c r="F887" s="2"/>
-      <c r="G887" s="2"/>
-      <c r="H887" s="2"/>
-      <c r="I887" s="2"/>
-      <c r="J887" s="2"/>
-      <c r="K887" s="2"/>
-      <c r="L887" s="2"/>
-      <c r="M887" s="2"/>
-      <c r="N887" s="2"/>
-      <c r="O887" s="2"/>
-      <c r="P887" s="3"/>
-      <c r="Q887" s="3"/>
-      <c r="R887" s="2"/>
-      <c r="S887" s="2"/>
-      <c r="T887" s="2"/>
-      <c r="U887" s="2"/>
-      <c r="V887" s="2"/>
-      <c r="W887" s="2"/>
-      <c r="X887" s="2"/>
-      <c r="Y887" s="2"/>
-      <c r="Z887" s="2"/>
-    </row>
-    <row r="888" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A888" s="11"/>
-      <c r="B888" s="2"/>
-      <c r="C888" s="2"/>
-      <c r="D888" s="2"/>
-      <c r="E888" s="2"/>
-      <c r="F888" s="2"/>
-      <c r="G888" s="2"/>
-      <c r="H888" s="2"/>
-      <c r="I888" s="2"/>
-      <c r="J888" s="2"/>
-      <c r="K888" s="2"/>
-      <c r="L888" s="2"/>
-      <c r="M888" s="2"/>
-      <c r="N888" s="2"/>
-      <c r="O888" s="2"/>
-      <c r="P888" s="3"/>
-      <c r="Q888" s="3"/>
-      <c r="R888" s="2"/>
-      <c r="S888" s="2"/>
-      <c r="T888" s="2"/>
-      <c r="U888" s="2"/>
-      <c r="V888" s="2"/>
-      <c r="W888" s="2"/>
-      <c r="X888" s="2"/>
-      <c r="Y888" s="2"/>
-      <c r="Z888" s="2"/>
-    </row>
-    <row r="889" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A889" s="11"/>
-      <c r="B889" s="2"/>
-      <c r="C889" s="2"/>
-      <c r="D889" s="2"/>
-      <c r="E889" s="2"/>
-      <c r="F889" s="2"/>
-      <c r="G889" s="2"/>
-      <c r="H889" s="2"/>
-      <c r="I889" s="2"/>
-      <c r="J889" s="2"/>
-      <c r="K889" s="2"/>
-      <c r="L889" s="2"/>
-      <c r="M889" s="2"/>
-      <c r="N889" s="2"/>
-      <c r="O889" s="2"/>
-      <c r="P889" s="3"/>
-      <c r="Q889" s="3"/>
-      <c r="R889" s="2"/>
-      <c r="S889" s="2"/>
-      <c r="T889" s="2"/>
-      <c r="U889" s="2"/>
-      <c r="V889" s="2"/>
-      <c r="W889" s="2"/>
-      <c r="X889" s="2"/>
-      <c r="Y889" s="2"/>
-      <c r="Z889" s="2"/>
-    </row>
-    <row r="890" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A890" s="11"/>
-      <c r="B890" s="2"/>
-      <c r="C890" s="2"/>
-      <c r="D890" s="2"/>
-      <c r="E890" s="2"/>
-      <c r="F890" s="2"/>
-      <c r="G890" s="2"/>
-      <c r="H890" s="2"/>
-      <c r="I890" s="2"/>
-      <c r="J890" s="2"/>
-      <c r="K890" s="2"/>
-      <c r="L890" s="2"/>
-      <c r="M890" s="2"/>
-      <c r="N890" s="2"/>
-      <c r="O890" s="2"/>
-      <c r="P890" s="3"/>
-      <c r="Q890" s="3"/>
-      <c r="R890" s="2"/>
-      <c r="S890" s="2"/>
-      <c r="T890" s="2"/>
-      <c r="U890" s="2"/>
-      <c r="V890" s="2"/>
-      <c r="W890" s="2"/>
-      <c r="X890" s="2"/>
-      <c r="Y890" s="2"/>
-      <c r="Z890" s="2"/>
-    </row>
-    <row r="891" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A891" s="11"/>
-      <c r="B891" s="2"/>
-      <c r="C891" s="2"/>
-      <c r="D891" s="2"/>
-      <c r="E891" s="2"/>
-      <c r="F891" s="2"/>
-      <c r="G891" s="2"/>
-      <c r="H891" s="2"/>
-      <c r="I891" s="2"/>
-      <c r="J891" s="2"/>
-      <c r="K891" s="2"/>
-      <c r="L891" s="2"/>
-      <c r="M891" s="2"/>
-      <c r="N891" s="2"/>
-      <c r="O891" s="2"/>
-      <c r="P891" s="3"/>
-      <c r="Q891" s="3"/>
-      <c r="R891" s="2"/>
-      <c r="S891" s="2"/>
-      <c r="T891" s="2"/>
-      <c r="U891" s="2"/>
-      <c r="V891" s="2"/>
-      <c r="W891" s="2"/>
-      <c r="X891" s="2"/>
-      <c r="Y891" s="2"/>
-      <c r="Z891" s="2"/>
-    </row>
-    <row r="892" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A892" s="11"/>
-      <c r="B892" s="2"/>
-      <c r="C892" s="2"/>
-      <c r="D892" s="2"/>
-      <c r="E892" s="2"/>
-      <c r="F892" s="2"/>
-      <c r="G892" s="2"/>
-      <c r="H892" s="2"/>
-      <c r="I892" s="2"/>
-      <c r="J892" s="2"/>
-      <c r="K892" s="2"/>
-      <c r="L892" s="2"/>
-      <c r="M892" s="2"/>
-      <c r="N892" s="2"/>
-      <c r="O892" s="2"/>
-      <c r="P892" s="3"/>
-      <c r="Q892" s="3"/>
-      <c r="R892" s="2"/>
-      <c r="S892" s="2"/>
-      <c r="T892" s="2"/>
-      <c r="U892" s="2"/>
-      <c r="V892" s="2"/>
-      <c r="W892" s="2"/>
-      <c r="X892" s="2"/>
-      <c r="Y892" s="2"/>
-      <c r="Z892" s="2"/>
-    </row>
-    <row r="893" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A893" s="11"/>
-      <c r="B893" s="2"/>
-      <c r="C893" s="2"/>
-      <c r="D893" s="2"/>
-      <c r="E893" s="2"/>
-      <c r="F893" s="2"/>
-      <c r="G893" s="2"/>
-      <c r="H893" s="2"/>
-      <c r="I893" s="2"/>
-      <c r="J893" s="2"/>
-      <c r="K893" s="2"/>
-      <c r="L893" s="2"/>
-      <c r="M893" s="2"/>
-      <c r="N893" s="2"/>
-      <c r="O893" s="2"/>
-      <c r="P893" s="3"/>
-      <c r="Q893" s="3"/>
-      <c r="R893" s="2"/>
-      <c r="S893" s="2"/>
-      <c r="T893" s="2"/>
-      <c r="U893" s="2"/>
-      <c r="V893" s="2"/>
-      <c r="W893" s="2"/>
-      <c r="X893" s="2"/>
-      <c r="Y893" s="2"/>
-      <c r="Z893" s="2"/>
-    </row>
-    <row r="894" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A894" s="11"/>
-      <c r="B894" s="2"/>
-      <c r="C894" s="2"/>
-      <c r="D894" s="2"/>
-      <c r="E894" s="2"/>
-      <c r="F894" s="2"/>
-      <c r="G894" s="2"/>
-      <c r="H894" s="2"/>
-      <c r="I894" s="2"/>
-      <c r="J894" s="2"/>
-      <c r="K894" s="2"/>
-      <c r="L894" s="2"/>
-      <c r="M894" s="2"/>
-      <c r="N894" s="2"/>
-      <c r="O894" s="2"/>
-      <c r="P894" s="3"/>
-      <c r="Q894" s="3"/>
-      <c r="R894" s="2"/>
-      <c r="S894" s="2"/>
-      <c r="T894" s="2"/>
-      <c r="U894" s="2"/>
-      <c r="V894" s="2"/>
-      <c r="W894" s="2"/>
-      <c r="X894" s="2"/>
-      <c r="Y894" s="2"/>
-      <c r="Z894" s="2"/>
-    </row>
-    <row r="895" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A895" s="11"/>
-      <c r="B895" s="2"/>
-      <c r="C895" s="2"/>
-      <c r="D895" s="2"/>
-      <c r="E895" s="2"/>
-      <c r="F895" s="2"/>
-      <c r="G895" s="2"/>
-      <c r="H895" s="2"/>
-      <c r="I895" s="2"/>
-      <c r="J895" s="2"/>
-      <c r="K895" s="2"/>
-      <c r="L895" s="2"/>
-      <c r="M895" s="2"/>
-      <c r="N895" s="2"/>
-      <c r="O895" s="2"/>
-      <c r="P895" s="3"/>
-      <c r="Q895" s="3"/>
-      <c r="R895" s="2"/>
-      <c r="S895" s="2"/>
-      <c r="T895" s="2"/>
-      <c r="U895" s="2"/>
-      <c r="V895" s="2"/>
-      <c r="W895" s="2"/>
-      <c r="X895" s="2"/>
-      <c r="Y895" s="2"/>
-      <c r="Z895" s="2"/>
-    </row>
-    <row r="896" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A896" s="11"/>
-      <c r="B896" s="2"/>
-      <c r="C896" s="2"/>
-      <c r="D896" s="2"/>
-      <c r="E896" s="2"/>
-      <c r="F896" s="2"/>
-      <c r="G896" s="2"/>
-      <c r="H896" s="2"/>
-      <c r="I896" s="2"/>
-      <c r="J896" s="2"/>
-      <c r="K896" s="2"/>
-      <c r="L896" s="2"/>
-      <c r="M896" s="2"/>
-      <c r="N896" s="2"/>
-      <c r="O896" s="2"/>
-      <c r="P896" s="3"/>
-      <c r="Q896" s="3"/>
-      <c r="R896" s="2"/>
-      <c r="S896" s="2"/>
-      <c r="T896" s="2"/>
-      <c r="U896" s="2"/>
-      <c r="V896" s="2"/>
-      <c r="W896" s="2"/>
-      <c r="X896" s="2"/>
-      <c r="Y896" s="2"/>
-      <c r="Z896" s="2"/>
-    </row>
-    <row r="897" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A897" s="11"/>
-      <c r="B897" s="2"/>
-      <c r="C897" s="2"/>
-      <c r="D897" s="2"/>
-      <c r="E897" s="2"/>
-      <c r="F897" s="2"/>
-      <c r="G897" s="2"/>
-      <c r="H897" s="2"/>
-      <c r="I897" s="2"/>
-      <c r="J897" s="2"/>
-      <c r="K897" s="2"/>
-      <c r="L897" s="2"/>
-      <c r="M897" s="2"/>
-      <c r="N897" s="2"/>
-      <c r="O897" s="2"/>
-      <c r="P897" s="3"/>
-      <c r="Q897" s="3"/>
-      <c r="R897" s="2"/>
-      <c r="S897" s="2"/>
-      <c r="T897" s="2"/>
-      <c r="U897" s="2"/>
-      <c r="V897" s="2"/>
-      <c r="W897" s="2"/>
-      <c r="X897" s="2"/>
-      <c r="Y897" s="2"/>
-      <c r="Z897" s="2"/>
-    </row>
-    <row r="898" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A898" s="11"/>
-      <c r="B898" s="2"/>
-      <c r="C898" s="2"/>
-      <c r="D898" s="2"/>
-      <c r="E898" s="2"/>
-      <c r="F898" s="2"/>
-      <c r="G898" s="2"/>
-      <c r="H898" s="2"/>
-      <c r="I898" s="2"/>
-      <c r="J898" s="2"/>
-      <c r="K898" s="2"/>
-      <c r="L898" s="2"/>
-      <c r="M898" s="2"/>
-      <c r="N898" s="2"/>
-      <c r="O898" s="2"/>
-      <c r="P898" s="3"/>
-      <c r="Q898" s="3"/>
-      <c r="R898" s="2"/>
-      <c r="S898" s="2"/>
-      <c r="T898" s="2"/>
-      <c r="U898" s="2"/>
-      <c r="V898" s="2"/>
-      <c r="W898" s="2"/>
-      <c r="X898" s="2"/>
-      <c r="Y898" s="2"/>
-      <c r="Z898" s="2"/>
-    </row>
-    <row r="899" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A899" s="11"/>
-      <c r="B899" s="2"/>
-      <c r="C899" s="2"/>
-      <c r="D899" s="2"/>
-      <c r="E899" s="2"/>
-      <c r="F899" s="2"/>
-      <c r="G899" s="2"/>
-      <c r="H899" s="2"/>
-      <c r="I899" s="2"/>
-      <c r="J899" s="2"/>
-      <c r="K899" s="2"/>
-      <c r="L899" s="2"/>
-      <c r="M899" s="2"/>
-      <c r="N899" s="2"/>
-      <c r="O899" s="2"/>
-      <c r="P899" s="3"/>
-      <c r="Q899" s="3"/>
-      <c r="R899" s="2"/>
-      <c r="S899" s="2"/>
-      <c r="T899" s="2"/>
-      <c r="U899" s="2"/>
-      <c r="V899" s="2"/>
-      <c r="W899" s="2"/>
-      <c r="X899" s="2"/>
-      <c r="Y899" s="2"/>
-      <c r="Z899" s="2"/>
-    </row>
-    <row r="900" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A900" s="11"/>
-      <c r="B900" s="2"/>
-      <c r="C900" s="2"/>
-      <c r="D900" s="2"/>
-      <c r="E900" s="2"/>
-      <c r="F900" s="2"/>
-      <c r="G900" s="2"/>
-      <c r="H900" s="2"/>
-      <c r="I900" s="2"/>
-      <c r="J900" s="2"/>
-      <c r="K900" s="2"/>
-      <c r="L900" s="2"/>
-      <c r="M900" s="2"/>
-      <c r="N900" s="2"/>
-      <c r="O900" s="2"/>
-      <c r="P900" s="3"/>
-      <c r="Q900" s="3"/>
-      <c r="R900" s="2"/>
-      <c r="S900" s="2"/>
-      <c r="T900" s="2"/>
-      <c r="U900" s="2"/>
-      <c r="V900" s="2"/>
-      <c r="W900" s="2"/>
-      <c r="X900" s="2"/>
-      <c r="Y900" s="2"/>
-      <c r="Z900" s="2"/>
-    </row>
-    <row r="901" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A901" s="11"/>
-      <c r="B901" s="2"/>
-      <c r="C901" s="2"/>
-      <c r="D901" s="2"/>
-      <c r="E901" s="2"/>
-      <c r="F901" s="2"/>
-      <c r="G901" s="2"/>
-      <c r="H901" s="2"/>
-      <c r="I901" s="2"/>
-      <c r="J901" s="2"/>
-      <c r="K901" s="2"/>
-      <c r="L901" s="2"/>
-      <c r="M901" s="2"/>
-      <c r="N901" s="2"/>
-      <c r="O901" s="2"/>
-      <c r="P901" s="3"/>
-      <c r="Q901" s="3"/>
-      <c r="R901" s="2"/>
-      <c r="S901" s="2"/>
-      <c r="T901" s="2"/>
-      <c r="U901" s="2"/>
-      <c r="V901" s="2"/>
-      <c r="W901" s="2"/>
-      <c r="X901" s="2"/>
-      <c r="Y901" s="2"/>
-      <c r="Z901" s="2"/>
-    </row>
-    <row r="902" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A902" s="11"/>
-      <c r="B902" s="2"/>
-      <c r="C902" s="2"/>
-      <c r="D902" s="2"/>
-      <c r="E902" s="2"/>
-      <c r="F902" s="2"/>
-      <c r="G902" s="2"/>
-      <c r="H902" s="2"/>
-      <c r="I902" s="2"/>
-      <c r="J902" s="2"/>
-      <c r="K902" s="2"/>
-      <c r="L902" s="2"/>
-      <c r="M902" s="2"/>
-      <c r="N902" s="2"/>
-      <c r="O902" s="2"/>
-      <c r="P902" s="3"/>
-      <c r="Q902" s="3"/>
-      <c r="R902" s="2"/>
-      <c r="S902" s="2"/>
-      <c r="T902" s="2"/>
-      <c r="U902" s="2"/>
-      <c r="V902" s="2"/>
-      <c r="W902" s="2"/>
-      <c r="X902" s="2"/>
-      <c r="Y902" s="2"/>
-      <c r="Z902" s="2"/>
-    </row>
-    <row r="903" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A903" s="11"/>
-      <c r="B903" s="2"/>
-      <c r="C903" s="2"/>
-      <c r="D903" s="2"/>
-      <c r="E903" s="2"/>
-      <c r="F903" s="2"/>
-      <c r="G903" s="2"/>
-      <c r="H903" s="2"/>
-      <c r="I903" s="2"/>
-      <c r="J903" s="2"/>
-      <c r="K903" s="2"/>
-      <c r="L903" s="2"/>
-      <c r="M903" s="2"/>
-      <c r="N903" s="2"/>
-      <c r="O903" s="2"/>
-      <c r="P903" s="3"/>
-      <c r="Q903" s="3"/>
-      <c r="R903" s="2"/>
-      <c r="S903" s="2"/>
-      <c r="T903" s="2"/>
-      <c r="U903" s="2"/>
-      <c r="V903" s="2"/>
-      <c r="W903" s="2"/>
-      <c r="X903" s="2"/>
-      <c r="Y903" s="2"/>
-      <c r="Z903" s="2"/>
-    </row>
-    <row r="904" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A904" s="11"/>
-      <c r="B904" s="2"/>
-      <c r="C904" s="2"/>
-      <c r="D904" s="2"/>
-      <c r="E904" s="2"/>
-      <c r="F904" s="2"/>
-      <c r="G904" s="2"/>
-      <c r="H904" s="2"/>
-      <c r="I904" s="2"/>
-      <c r="J904" s="2"/>
-      <c r="K904" s="2"/>
-      <c r="L904" s="2"/>
-      <c r="M904" s="2"/>
-      <c r="N904" s="2"/>
-      <c r="O904" s="2"/>
-      <c r="P904" s="3"/>
-      <c r="Q904" s="3"/>
-      <c r="R904" s="2"/>
-      <c r="S904" s="2"/>
-      <c r="T904" s="2"/>
-      <c r="U904" s="2"/>
-      <c r="V904" s="2"/>
-      <c r="W904" s="2"/>
-      <c r="X904" s="2"/>
-      <c r="Y904" s="2"/>
-      <c r="Z904" s="2"/>
-    </row>
-    <row r="905" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A905" s="11"/>
-      <c r="B905" s="2"/>
-      <c r="C905" s="2"/>
-      <c r="D905" s="2"/>
-      <c r="E905" s="2"/>
-      <c r="F905" s="2"/>
-      <c r="G905" s="2"/>
-      <c r="H905" s="2"/>
-      <c r="I905" s="2"/>
-      <c r="J905" s="2"/>
-      <c r="K905" s="2"/>
-      <c r="L905" s="2"/>
-      <c r="M905" s="2"/>
-      <c r="N905" s="2"/>
-      <c r="O905" s="2"/>
-      <c r="P905" s="3"/>
-      <c r="Q905" s="3"/>
-      <c r="R905" s="2"/>
-      <c r="S905" s="2"/>
-      <c r="T905" s="2"/>
-      <c r="U905" s="2"/>
-      <c r="V905" s="2"/>
-      <c r="W905" s="2"/>
-      <c r="X905" s="2"/>
-      <c r="Y905" s="2"/>
-      <c r="Z905" s="2"/>
-    </row>
-    <row r="906" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A906" s="11"/>
-      <c r="B906" s="2"/>
-      <c r="C906" s="2"/>
-      <c r="D906" s="2"/>
-      <c r="E906" s="2"/>
-      <c r="F906" s="2"/>
-      <c r="G906" s="2"/>
-      <c r="H906" s="2"/>
-      <c r="I906" s="2"/>
-      <c r="J906" s="2"/>
-      <c r="K906" s="2"/>
-      <c r="L906" s="2"/>
-      <c r="M906" s="2"/>
-      <c r="N906" s="2"/>
-      <c r="O906" s="2"/>
-      <c r="P906" s="3"/>
-      <c r="Q906" s="3"/>
-      <c r="R906" s="2"/>
-      <c r="S906" s="2"/>
-      <c r="T906" s="2"/>
-      <c r="U906" s="2"/>
-      <c r="V906" s="2"/>
-      <c r="W906" s="2"/>
-      <c r="X906" s="2"/>
-      <c r="Y906" s="2"/>
-      <c r="Z906" s="2"/>
-    </row>
-    <row r="907" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A907" s="11"/>
-      <c r="B907" s="2"/>
-      <c r="C907" s="2"/>
-      <c r="D907" s="2"/>
-      <c r="E907" s="2"/>
-      <c r="F907" s="2"/>
-      <c r="G907" s="2"/>
-      <c r="H907" s="2"/>
-      <c r="I907" s="2"/>
-      <c r="J907" s="2"/>
-      <c r="K907" s="2"/>
-      <c r="L907" s="2"/>
-      <c r="M907" s="2"/>
-      <c r="N907" s="2"/>
-      <c r="O907" s="2"/>
-      <c r="P907" s="3"/>
-      <c r="Q907" s="3"/>
-      <c r="R907" s="2"/>
-      <c r="S907" s="2"/>
-      <c r="T907" s="2"/>
-      <c r="U907" s="2"/>
-      <c r="V907" s="2"/>
-      <c r="W907" s="2"/>
-      <c r="X907" s="2"/>
-      <c r="Y907" s="2"/>
-      <c r="Z907" s="2"/>
-    </row>
-    <row r="908" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A908" s="11"/>
-      <c r="B908" s="2"/>
-      <c r="C908" s="2"/>
-      <c r="D908" s="2"/>
-      <c r="E908" s="2"/>
-      <c r="F908" s="2"/>
-      <c r="G908" s="2"/>
-      <c r="H908" s="2"/>
-      <c r="I908" s="2"/>
-      <c r="J908" s="2"/>
-      <c r="K908" s="2"/>
-      <c r="L908" s="2"/>
-      <c r="M908" s="2"/>
-      <c r="N908" s="2"/>
-      <c r="O908" s="2"/>
-      <c r="P908" s="3"/>
-      <c r="Q908" s="3"/>
-      <c r="R908" s="2"/>
-      <c r="S908" s="2"/>
-      <c r="T908" s="2"/>
-      <c r="U908" s="2"/>
-      <c r="V908" s="2"/>
-      <c r="W908" s="2"/>
-      <c r="X908" s="2"/>
-      <c r="Y908" s="2"/>
-      <c r="Z908" s="2"/>
-    </row>
-    <row r="909" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A909" s="11"/>
-      <c r="B909" s="2"/>
-      <c r="C909" s="2"/>
-      <c r="D909" s="2"/>
-      <c r="E909" s="2"/>
-      <c r="F909" s="2"/>
-      <c r="G909" s="2"/>
-      <c r="H909" s="2"/>
-      <c r="I909" s="2"/>
-      <c r="J909" s="2"/>
-      <c r="K909" s="2"/>
-      <c r="L909" s="2"/>
-      <c r="M909" s="2"/>
-      <c r="N909" s="2"/>
-      <c r="O909" s="2"/>
-      <c r="P909" s="3"/>
-      <c r="Q909" s="3"/>
-      <c r="R909" s="2"/>
-      <c r="S909" s="2"/>
-      <c r="T909" s="2"/>
-      <c r="U909" s="2"/>
-      <c r="V909" s="2"/>
-      <c r="W909" s="2"/>
-      <c r="X909" s="2"/>
-      <c r="Y909" s="2"/>
-      <c r="Z909" s="2"/>
-    </row>
-    <row r="910" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A910" s="11"/>
-      <c r="B910" s="2"/>
-      <c r="C910" s="2"/>
-      <c r="D910" s="2"/>
-      <c r="E910" s="2"/>
-      <c r="F910" s="2"/>
-      <c r="G910" s="2"/>
-      <c r="H910" s="2"/>
-      <c r="I910" s="2"/>
-      <c r="J910" s="2"/>
-      <c r="K910" s="2"/>
-      <c r="L910" s="2"/>
-      <c r="M910" s="2"/>
-      <c r="N910" s="2"/>
-      <c r="O910" s="2"/>
-      <c r="P910" s="3"/>
-      <c r="Q910" s="3"/>
-      <c r="R910" s="2"/>
-      <c r="S910" s="2"/>
-      <c r="T910" s="2"/>
-      <c r="U910" s="2"/>
-      <c r="V910" s="2"/>
-      <c r="W910" s="2"/>
-      <c r="X910" s="2"/>
-      <c r="Y910" s="2"/>
-      <c r="Z910" s="2"/>
-    </row>
-    <row r="911" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A911" s="11"/>
-      <c r="B911" s="2"/>
-      <c r="C911" s="2"/>
-      <c r="D911" s="2"/>
-      <c r="E911" s="2"/>
-      <c r="F911" s="2"/>
-      <c r="G911" s="2"/>
-      <c r="H911" s="2"/>
-      <c r="I911" s="2"/>
-      <c r="J911" s="2"/>
-      <c r="K911" s="2"/>
-      <c r="L911" s="2"/>
-      <c r="M911" s="2"/>
-      <c r="N911" s="2"/>
-      <c r="O911" s="2"/>
-      <c r="P911" s="3"/>
-      <c r="Q911" s="3"/>
-      <c r="R911" s="2"/>
-      <c r="S911" s="2"/>
-      <c r="T911" s="2"/>
-      <c r="U911" s="2"/>
-      <c r="V911" s="2"/>
-      <c r="W911" s="2"/>
-      <c r="X911" s="2"/>
-      <c r="Y911" s="2"/>
-      <c r="Z911" s="2"/>
-    </row>
-    <row r="912" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A912" s="11"/>
-      <c r="B912" s="2"/>
-      <c r="C912" s="2"/>
-      <c r="D912" s="2"/>
-      <c r="E912" s="2"/>
-      <c r="F912" s="2"/>
-      <c r="G912" s="2"/>
-      <c r="H912" s="2"/>
-      <c r="I912" s="2"/>
-      <c r="J912" s="2"/>
-      <c r="K912" s="2"/>
-      <c r="L912" s="2"/>
-      <c r="M912" s="2"/>
-      <c r="N912" s="2"/>
-      <c r="O912" s="2"/>
-      <c r="P912" s="3"/>
-      <c r="Q912" s="3"/>
-      <c r="R912" s="2"/>
-      <c r="S912" s="2"/>
-      <c r="T912" s="2"/>
-      <c r="U912" s="2"/>
-      <c r="V912" s="2"/>
-      <c r="W912" s="2"/>
-      <c r="X912" s="2"/>
-      <c r="Y912" s="2"/>
-      <c r="Z912" s="2"/>
-    </row>
-    <row r="913" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A913" s="11"/>
-      <c r="B913" s="2"/>
-      <c r="C913" s="2"/>
-      <c r="D913" s="2"/>
-      <c r="E913" s="2"/>
-      <c r="F913" s="2"/>
-      <c r="G913" s="2"/>
-      <c r="H913" s="2"/>
-      <c r="I913" s="2"/>
-      <c r="J913" s="2"/>
-      <c r="K913" s="2"/>
-      <c r="L913" s="2"/>
-      <c r="M913" s="2"/>
-      <c r="N913" s="2"/>
-      <c r="O913" s="2"/>
-      <c r="P913" s="3"/>
-      <c r="Q913" s="3"/>
-      <c r="R913" s="2"/>
-      <c r="S913" s="2"/>
-      <c r="T913" s="2"/>
-      <c r="U913" s="2"/>
-      <c r="V913" s="2"/>
-      <c r="W913" s="2"/>
-      <c r="X913" s="2"/>
-      <c r="Y913" s="2"/>
-      <c r="Z913" s="2"/>
-    </row>
-    <row r="914" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A914" s="11"/>
-      <c r="B914" s="2"/>
-      <c r="C914" s="2"/>
-      <c r="D914" s="2"/>
-      <c r="E914" s="2"/>
-      <c r="F914" s="2"/>
-      <c r="G914" s="2"/>
-      <c r="H914" s="2"/>
-      <c r="I914" s="2"/>
-      <c r="J914" s="2"/>
-      <c r="K914" s="2"/>
-      <c r="L914" s="2"/>
-      <c r="M914" s="2"/>
-      <c r="N914" s="2"/>
-      <c r="O914" s="2"/>
-      <c r="P914" s="3"/>
-      <c r="Q914" s="3"/>
-      <c r="R914" s="2"/>
-      <c r="S914" s="2"/>
-      <c r="T914" s="2"/>
-      <c r="U914" s="2"/>
-      <c r="V914" s="2"/>
-      <c r="W914" s="2"/>
-      <c r="X914" s="2"/>
-      <c r="Y914" s="2"/>
-      <c r="Z914" s="2"/>
-    </row>
-    <row r="915" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A915" s="11"/>
-      <c r="B915" s="2"/>
-      <c r="C915" s="2"/>
-      <c r="D915" s="2"/>
-      <c r="E915" s="2"/>
-      <c r="F915" s="2"/>
-      <c r="G915" s="2"/>
-      <c r="H915" s="2"/>
-      <c r="I915" s="2"/>
-      <c r="J915" s="2"/>
-      <c r="K915" s="2"/>
-      <c r="L915" s="2"/>
-      <c r="M915" s="2"/>
-      <c r="N915" s="2"/>
-      <c r="O915" s="2"/>
-      <c r="P915" s="3"/>
-      <c r="Q915" s="3"/>
-      <c r="R915" s="2"/>
-      <c r="S915" s="2"/>
-      <c r="T915" s="2"/>
-      <c r="U915" s="2"/>
-      <c r="V915" s="2"/>
-      <c r="W915" s="2"/>
-      <c r="X915" s="2"/>
-      <c r="Y915" s="2"/>
-      <c r="Z915" s="2"/>
-    </row>
-    <row r="916" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A916" s="11"/>
-      <c r="B916" s="2"/>
-      <c r="C916" s="2"/>
-      <c r="D916" s="2"/>
-      <c r="E916" s="2"/>
-      <c r="F916" s="2"/>
-      <c r="G916" s="2"/>
-      <c r="H916" s="2"/>
-      <c r="I916" s="2"/>
-      <c r="J916" s="2"/>
-      <c r="K916" s="2"/>
-      <c r="L916" s="2"/>
-      <c r="M916" s="2"/>
-      <c r="N916" s="2"/>
-      <c r="O916" s="2"/>
-      <c r="P916" s="3"/>
-      <c r="Q916" s="3"/>
-      <c r="R916" s="2"/>
-      <c r="S916" s="2"/>
-      <c r="T916" s="2"/>
-      <c r="U916" s="2"/>
-      <c r="V916" s="2"/>
-      <c r="W916" s="2"/>
-      <c r="X916" s="2"/>
-      <c r="Y916" s="2"/>
-      <c r="Z916" s="2"/>
-    </row>
-    <row r="917" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A917" s="11"/>
-      <c r="B917" s="2"/>
-      <c r="C917" s="2"/>
-      <c r="D917" s="2"/>
-      <c r="E917" s="2"/>
-      <c r="F917" s="2"/>
-      <c r="G917" s="2"/>
-      <c r="H917" s="2"/>
-      <c r="I917" s="2"/>
-      <c r="J917" s="2"/>
-      <c r="K917" s="2"/>
-      <c r="L917" s="2"/>
-      <c r="M917" s="2"/>
-      <c r="N917" s="2"/>
-      <c r="O917" s="2"/>
-      <c r="P917" s="3"/>
-      <c r="Q917" s="3"/>
-      <c r="R917" s="2"/>
-      <c r="S917" s="2"/>
-      <c r="T917" s="2"/>
-      <c r="U917" s="2"/>
-      <c r="V917" s="2"/>
-      <c r="W917" s="2"/>
-      <c r="X917" s="2"/>
-      <c r="Y917" s="2"/>
-      <c r="Z917" s="2"/>
-    </row>
-    <row r="918" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A918" s="11"/>
-      <c r="B918" s="2"/>
-      <c r="C918" s="2"/>
-      <c r="D918" s="2"/>
-      <c r="E918" s="2"/>
-      <c r="F918" s="2"/>
-      <c r="G918" s="2"/>
-      <c r="H918" s="2"/>
-      <c r="I918" s="2"/>
-      <c r="J918" s="2"/>
-      <c r="K918" s="2"/>
-      <c r="L918" s="2"/>
-      <c r="M918" s="2"/>
-      <c r="N918" s="2"/>
-      <c r="O918" s="2"/>
-      <c r="P918" s="3"/>
-      <c r="Q918" s="3"/>
-      <c r="R918" s="2"/>
-      <c r="S918" s="2"/>
-      <c r="T918" s="2"/>
-      <c r="U918" s="2"/>
-      <c r="V918" s="2"/>
-      <c r="W918" s="2"/>
-      <c r="X918" s="2"/>
-      <c r="Y918" s="2"/>
-      <c r="Z918" s="2"/>
-    </row>
-    <row r="919" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A919" s="11"/>
-      <c r="B919" s="2"/>
-      <c r="C919" s="2"/>
-      <c r="D919" s="2"/>
-      <c r="E919" s="2"/>
-      <c r="F919" s="2"/>
-      <c r="G919" s="2"/>
-      <c r="H919" s="2"/>
-      <c r="I919" s="2"/>
-      <c r="J919" s="2"/>
-      <c r="K919" s="2"/>
-      <c r="L919" s="2"/>
-      <c r="M919" s="2"/>
-      <c r="N919" s="2"/>
-      <c r="O919" s="2"/>
-      <c r="P919" s="3"/>
-      <c r="Q919" s="3"/>
-      <c r="R919" s="2"/>
-      <c r="S919" s="2"/>
-      <c r="T919" s="2"/>
-      <c r="U919" s="2"/>
-      <c r="V919" s="2"/>
-      <c r="W919" s="2"/>
-      <c r="X919" s="2"/>
-      <c r="Y919" s="2"/>
-      <c r="Z919" s="2"/>
-    </row>
-    <row r="920" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A920" s="11"/>
-      <c r="B920" s="2"/>
-      <c r="C920" s="2"/>
-      <c r="D920" s="2"/>
-      <c r="E920" s="2"/>
-      <c r="F920" s="2"/>
-      <c r="G920" s="2"/>
-      <c r="H920" s="2"/>
-      <c r="I920" s="2"/>
-      <c r="J920" s="2"/>
-      <c r="K920" s="2"/>
-      <c r="L920" s="2"/>
-      <c r="M920" s="2"/>
-      <c r="N920" s="2"/>
-      <c r="O920" s="2"/>
-      <c r="P920" s="3"/>
-      <c r="Q920" s="3"/>
-      <c r="R920" s="2"/>
-      <c r="S920" s="2"/>
-      <c r="T920" s="2"/>
-      <c r="U920" s="2"/>
-      <c r="V920" s="2"/>
-      <c r="W920" s="2"/>
-      <c r="X920" s="2"/>
-      <c r="Y920" s="2"/>
-      <c r="Z920" s="2"/>
-    </row>
-    <row r="921" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A921" s="11"/>
-      <c r="B921" s="2"/>
-      <c r="C921" s="2"/>
-      <c r="D921" s="2"/>
-      <c r="E921" s="2"/>
-      <c r="F921" s="2"/>
-      <c r="G921" s="2"/>
-      <c r="H921" s="2"/>
-      <c r="I921" s="2"/>
-      <c r="J921" s="2"/>
-      <c r="K921" s="2"/>
-      <c r="L921" s="2"/>
-      <c r="M921" s="2"/>
-      <c r="N921" s="2"/>
-      <c r="O921" s="2"/>
-      <c r="P921" s="3"/>
-      <c r="Q921" s="3"/>
-      <c r="R921" s="2"/>
-      <c r="S921" s="2"/>
-      <c r="T921" s="2"/>
-      <c r="U921" s="2"/>
-      <c r="V921" s="2"/>
-      <c r="W921" s="2"/>
-      <c r="X921" s="2"/>
-      <c r="Y921" s="2"/>
-      <c r="Z921" s="2"/>
-    </row>
-    <row r="922" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A922" s="11"/>
-      <c r="B922" s="2"/>
-      <c r="C922" s="2"/>
-      <c r="D922" s="2"/>
-      <c r="E922" s="2"/>
-      <c r="F922" s="2"/>
-      <c r="G922" s="2"/>
-      <c r="H922" s="2"/>
-      <c r="I922" s="2"/>
-      <c r="J922" s="2"/>
-      <c r="K922" s="2"/>
-      <c r="L922" s="2"/>
-      <c r="M922" s="2"/>
-      <c r="N922" s="2"/>
-      <c r="O922" s="2"/>
-      <c r="P922" s="3"/>
-      <c r="Q922" s="3"/>
-      <c r="R922" s="2"/>
-      <c r="S922" s="2"/>
-      <c r="T922" s="2"/>
-      <c r="U922" s="2"/>
-      <c r="V922" s="2"/>
-      <c r="W922" s="2"/>
-      <c r="X922" s="2"/>
-      <c r="Y922" s="2"/>
-      <c r="Z922" s="2"/>
-    </row>
-    <row r="923" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A923" s="11"/>
-      <c r="B923" s="2"/>
-      <c r="C923" s="2"/>
-      <c r="D923" s="2"/>
-      <c r="E923" s="2"/>
-      <c r="F923" s="2"/>
-      <c r="G923" s="2"/>
-      <c r="H923" s="2"/>
-      <c r="I923" s="2"/>
-      <c r="J923" s="2"/>
-      <c r="K923" s="2"/>
-      <c r="L923" s="2"/>
-      <c r="M923" s="2"/>
-      <c r="N923" s="2"/>
-      <c r="O923" s="2"/>
-      <c r="P923" s="3"/>
-      <c r="Q923" s="3"/>
-      <c r="R923" s="2"/>
-      <c r="S923" s="2"/>
-      <c r="T923" s="2"/>
-      <c r="U923" s="2"/>
-      <c r="V923" s="2"/>
-      <c r="W923" s="2"/>
-      <c r="X923" s="2"/>
-      <c r="Y923" s="2"/>
-      <c r="Z923" s="2"/>
-    </row>
-    <row r="924" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A924" s="11"/>
-      <c r="B924" s="2"/>
-      <c r="C924" s="2"/>
-      <c r="D924" s="2"/>
-      <c r="E924" s="2"/>
-      <c r="F924" s="2"/>
-      <c r="G924" s="2"/>
-      <c r="H924" s="2"/>
-      <c r="I924" s="2"/>
-      <c r="J924" s="2"/>
-      <c r="K924" s="2"/>
-      <c r="L924" s="2"/>
-      <c r="M924" s="2"/>
-      <c r="N924" s="2"/>
-      <c r="O924" s="2"/>
-      <c r="P924" s="3"/>
-      <c r="Q924" s="3"/>
-      <c r="R924" s="2"/>
-      <c r="S924" s="2"/>
-      <c r="T924" s="2"/>
-      <c r="U924" s="2"/>
-      <c r="V924" s="2"/>
-      <c r="W924" s="2"/>
-      <c r="X924" s="2"/>
-      <c r="Y924" s="2"/>
-      <c r="Z924" s="2"/>
-    </row>
-    <row r="925" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A925" s="11"/>
-      <c r="B925" s="2"/>
-      <c r="C925" s="2"/>
-      <c r="D925" s="2"/>
-      <c r="E925" s="2"/>
-      <c r="F925" s="2"/>
-      <c r="G925" s="2"/>
-      <c r="H925" s="2"/>
-      <c r="I925" s="2"/>
-      <c r="J925" s="2"/>
-      <c r="K925" s="2"/>
-      <c r="L925" s="2"/>
-      <c r="M925" s="2"/>
-      <c r="N925" s="2"/>
-      <c r="O925" s="2"/>
-      <c r="P925" s="3"/>
-      <c r="Q925" s="3"/>
-      <c r="R925" s="2"/>
-      <c r="S925" s="2"/>
-      <c r="T925" s="2"/>
-      <c r="U925" s="2"/>
-      <c r="V925" s="2"/>
-      <c r="W925" s="2"/>
-      <c r="X925" s="2"/>
-      <c r="Y925" s="2"/>
-      <c r="Z925" s="2"/>
-    </row>
-    <row r="926" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A926" s="11"/>
-      <c r="B926" s="2"/>
-      <c r="C926" s="2"/>
-      <c r="D926" s="2"/>
-      <c r="E926" s="2"/>
-      <c r="F926" s="2"/>
-      <c r="G926" s="2"/>
-      <c r="H926" s="2"/>
-      <c r="I926" s="2"/>
-      <c r="J926" s="2"/>
-      <c r="K926" s="2"/>
-      <c r="L926" s="2"/>
-      <c r="M926" s="2"/>
-      <c r="N926" s="2"/>
-      <c r="O926" s="2"/>
-      <c r="P926" s="3"/>
-      <c r="Q926" s="3"/>
-      <c r="R926" s="2"/>
-      <c r="S926" s="2"/>
-      <c r="T926" s="2"/>
-      <c r="U926" s="2"/>
-      <c r="V926" s="2"/>
-      <c r="W926" s="2"/>
-      <c r="X926" s="2"/>
-      <c r="Y926" s="2"/>
-      <c r="Z926" s="2"/>
-    </row>
-    <row r="927" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A927" s="11"/>
-      <c r="B927" s="2"/>
-      <c r="C927" s="2"/>
-      <c r="D927" s="2"/>
-      <c r="E927" s="2"/>
-      <c r="F927" s="2"/>
-      <c r="G927" s="2"/>
-      <c r="H927" s="2"/>
-      <c r="I927" s="2"/>
-      <c r="J927" s="2"/>
-      <c r="K927" s="2"/>
-      <c r="L927" s="2"/>
-      <c r="M927" s="2"/>
-      <c r="N927" s="2"/>
-      <c r="O927" s="2"/>
-      <c r="P927" s="3"/>
-      <c r="Q927" s="3"/>
-      <c r="R927" s="2"/>
-      <c r="S927" s="2"/>
-      <c r="T927" s="2"/>
-      <c r="U927" s="2"/>
-      <c r="V927" s="2"/>
-      <c r="W927" s="2"/>
-      <c r="X927" s="2"/>
-      <c r="Y927" s="2"/>
-      <c r="Z927" s="2"/>
-    </row>
-    <row r="928" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A928" s="11"/>
-      <c r="B928" s="2"/>
-      <c r="C928" s="2"/>
-      <c r="D928" s="2"/>
-      <c r="E928" s="2"/>
-      <c r="F928" s="2"/>
-      <c r="G928" s="2"/>
-      <c r="H928" s="2"/>
-      <c r="I928" s="2"/>
-      <c r="J928" s="2"/>
-      <c r="K928" s="2"/>
-      <c r="L928" s="2"/>
-      <c r="M928" s="2"/>
-      <c r="N928" s="2"/>
-      <c r="O928" s="2"/>
-      <c r="P928" s="3"/>
-      <c r="Q928" s="3"/>
-      <c r="R928" s="2"/>
-      <c r="S928" s="2"/>
-      <c r="T928" s="2"/>
-      <c r="U928" s="2"/>
-      <c r="V928" s="2"/>
-      <c r="W928" s="2"/>
-      <c r="X928" s="2"/>
-      <c r="Y928" s="2"/>
-      <c r="Z928" s="2"/>
-    </row>
-    <row r="929" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A929" s="11"/>
-      <c r="B929" s="2"/>
-      <c r="C929" s="2"/>
-      <c r="D929" s="2"/>
-      <c r="E929" s="2"/>
-      <c r="F929" s="2"/>
-      <c r="G929" s="2"/>
-      <c r="H929" s="2"/>
-      <c r="I929" s="2"/>
-      <c r="J929" s="2"/>
-      <c r="K929" s="2"/>
-      <c r="L929" s="2"/>
-      <c r="M929" s="2"/>
-      <c r="N929" s="2"/>
-      <c r="O929" s="2"/>
-      <c r="P929" s="3"/>
-      <c r="Q929" s="3"/>
-      <c r="R929" s="2"/>
-      <c r="S929" s="2"/>
-      <c r="T929" s="2"/>
-      <c r="U929" s="2"/>
-      <c r="V929" s="2"/>
-      <c r="W929" s="2"/>
-      <c r="X929" s="2"/>
-      <c r="Y929" s="2"/>
-      <c r="Z929" s="2"/>
-    </row>
-    <row r="930" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A930" s="11"/>
-      <c r="B930" s="2"/>
-      <c r="C930" s="2"/>
-      <c r="D930" s="2"/>
-      <c r="E930" s="2"/>
-      <c r="F930" s="2"/>
-      <c r="G930" s="2"/>
-      <c r="H930" s="2"/>
-      <c r="I930" s="2"/>
-      <c r="J930" s="2"/>
-      <c r="K930" s="2"/>
-      <c r="L930" s="2"/>
-      <c r="M930" s="2"/>
-      <c r="N930" s="2"/>
-      <c r="O930" s="2"/>
-      <c r="P930" s="3"/>
-      <c r="Q930" s="3"/>
-      <c r="R930" s="2"/>
-      <c r="S930" s="2"/>
-      <c r="T930" s="2"/>
-      <c r="U930" s="2"/>
-      <c r="V930" s="2"/>
-      <c r="W930" s="2"/>
-      <c r="X930" s="2"/>
-      <c r="Y930" s="2"/>
-      <c r="Z930" s="2"/>
-    </row>
-    <row r="931" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A931" s="11"/>
-      <c r="B931" s="2"/>
-      <c r="C931" s="2"/>
-      <c r="D931" s="2"/>
-      <c r="E931" s="2"/>
-      <c r="F931" s="2"/>
-      <c r="G931" s="2"/>
-      <c r="H931" s="2"/>
-      <c r="I931" s="2"/>
-      <c r="J931" s="2"/>
-      <c r="K931" s="2"/>
-      <c r="L931" s="2"/>
-      <c r="M931" s="2"/>
-      <c r="N931" s="2"/>
-      <c r="O931" s="2"/>
-      <c r="P931" s="3"/>
-      <c r="Q931" s="3"/>
-      <c r="R931" s="2"/>
-      <c r="S931" s="2"/>
-      <c r="T931" s="2"/>
-      <c r="U931" s="2"/>
-      <c r="V931" s="2"/>
-      <c r="W931" s="2"/>
-      <c r="X931" s="2"/>
-      <c r="Y931" s="2"/>
-      <c r="Z931" s="2"/>
-    </row>
-    <row r="932" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A932" s="11"/>
-      <c r="B932" s="2"/>
-      <c r="C932" s="2"/>
-      <c r="D932" s="2"/>
-      <c r="E932" s="2"/>
-      <c r="F932" s="2"/>
-      <c r="G932" s="2"/>
-      <c r="H932" s="2"/>
-      <c r="I932" s="2"/>
-      <c r="J932" s="2"/>
-      <c r="K932" s="2"/>
-      <c r="L932" s="2"/>
-      <c r="M932" s="2"/>
-      <c r="N932" s="2"/>
-      <c r="O932" s="2"/>
-      <c r="P932" s="3"/>
-      <c r="Q932" s="3"/>
-      <c r="R932" s="2"/>
-      <c r="S932" s="2"/>
-      <c r="T932" s="2"/>
-      <c r="U932" s="2"/>
-      <c r="V932" s="2"/>
-      <c r="W932" s="2"/>
-      <c r="X932" s="2"/>
-      <c r="Y932" s="2"/>
-      <c r="Z932" s="2"/>
-    </row>
-    <row r="933" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A933" s="11"/>
-      <c r="B933" s="2"/>
-      <c r="C933" s="2"/>
-      <c r="D933" s="2"/>
-      <c r="E933" s="2"/>
-      <c r="F933" s="2"/>
-      <c r="G933" s="2"/>
-      <c r="H933" s="2"/>
-      <c r="I933" s="2"/>
-      <c r="J933" s="2"/>
-      <c r="K933" s="2"/>
-      <c r="L933" s="2"/>
-      <c r="M933" s="2"/>
-      <c r="N933" s="2"/>
-      <c r="O933" s="2"/>
-      <c r="P933" s="3"/>
-      <c r="Q933" s="3"/>
-      <c r="R933" s="2"/>
-      <c r="S933" s="2"/>
-      <c r="T933" s="2"/>
-      <c r="U933" s="2"/>
-      <c r="V933" s="2"/>
-      <c r="W933" s="2"/>
-      <c r="X933" s="2"/>
-      <c r="Y933" s="2"/>
-      <c r="Z933" s="2"/>
-    </row>
-    <row r="934" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A934" s="11"/>
-      <c r="B934" s="2"/>
-      <c r="C934" s="2"/>
-      <c r="D934" s="2"/>
-      <c r="E934" s="2"/>
-      <c r="F934" s="2"/>
-      <c r="G934" s="2"/>
-      <c r="H934" s="2"/>
-      <c r="I934" s="2"/>
-      <c r="J934" s="2"/>
-      <c r="K934" s="2"/>
-      <c r="L934" s="2"/>
-      <c r="M934" s="2"/>
-      <c r="N934" s="2"/>
-      <c r="O934" s="2"/>
-      <c r="P934" s="3"/>
-      <c r="Q934" s="3"/>
-      <c r="R934" s="2"/>
-      <c r="S934" s="2"/>
-      <c r="T934" s="2"/>
-      <c r="U934" s="2"/>
-      <c r="V934" s="2"/>
-      <c r="W934" s="2"/>
-      <c r="X934" s="2"/>
-      <c r="Y934" s="2"/>
-      <c r="Z934" s="2"/>
-    </row>
-    <row r="935" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A935" s="11"/>
-      <c r="B935" s="2"/>
-      <c r="C935" s="2"/>
-      <c r="D935" s="2"/>
-      <c r="E935" s="2"/>
-      <c r="F935" s="2"/>
-      <c r="G935" s="2"/>
-      <c r="H935" s="2"/>
-      <c r="I935" s="2"/>
-      <c r="J935" s="2"/>
-      <c r="K935" s="2"/>
-      <c r="L935" s="2"/>
-      <c r="M935" s="2"/>
-      <c r="N935" s="2"/>
-      <c r="O935" s="2"/>
-      <c r="P935" s="3"/>
-      <c r="Q935" s="3"/>
-      <c r="R935" s="2"/>
-      <c r="S935" s="2"/>
-      <c r="T935" s="2"/>
-      <c r="U935" s="2"/>
-      <c r="V935" s="2"/>
-      <c r="W935" s="2"/>
-      <c r="X935" s="2"/>
-      <c r="Y935" s="2"/>
-      <c r="Z935" s="2"/>
-    </row>
-    <row r="936" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A936" s="11"/>
-      <c r="B936" s="2"/>
-      <c r="C936" s="2"/>
-      <c r="D936" s="2"/>
-      <c r="E936" s="2"/>
-      <c r="F936" s="2"/>
-      <c r="G936" s="2"/>
-      <c r="H936" s="2"/>
-      <c r="I936" s="2"/>
-      <c r="J936" s="2"/>
-      <c r="K936" s="2"/>
-      <c r="L936" s="2"/>
-      <c r="M936" s="2"/>
-      <c r="N936" s="2"/>
-      <c r="O936" s="2"/>
-      <c r="P936" s="3"/>
-      <c r="Q936" s="3"/>
-      <c r="R936" s="2"/>
-      <c r="S936" s="2"/>
-      <c r="T936" s="2"/>
-      <c r="U936" s="2"/>
-      <c r="V936" s="2"/>
-      <c r="W936" s="2"/>
-      <c r="X936" s="2"/>
-      <c r="Y936" s="2"/>
-      <c r="Z936" s="2"/>
-    </row>
-    <row r="937" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A937" s="11"/>
-      <c r="B937" s="2"/>
-      <c r="C937" s="2"/>
-      <c r="D937" s="2"/>
-      <c r="E937" s="2"/>
-      <c r="F937" s="2"/>
-      <c r="G937" s="2"/>
-      <c r="H937" s="2"/>
-      <c r="I937" s="2"/>
-      <c r="J937" s="2"/>
-      <c r="K937" s="2"/>
-      <c r="L937" s="2"/>
-      <c r="M937" s="2"/>
-      <c r="N937" s="2"/>
-      <c r="O937" s="2"/>
-      <c r="P937" s="3"/>
-      <c r="Q937" s="3"/>
-      <c r="R937" s="2"/>
-      <c r="S937" s="2"/>
-      <c r="T937" s="2"/>
-      <c r="U937" s="2"/>
-      <c r="V937" s="2"/>
-      <c r="W937" s="2"/>
-      <c r="X937" s="2"/>
-      <c r="Y937" s="2"/>
-      <c r="Z937" s="2"/>
-    </row>
-    <row r="938" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A938" s="11"/>
-      <c r="B938" s="2"/>
-      <c r="C938" s="2"/>
-      <c r="D938" s="2"/>
-      <c r="E938" s="2"/>
-      <c r="F938" s="2"/>
-      <c r="G938" s="2"/>
-      <c r="H938" s="2"/>
-      <c r="I938" s="2"/>
-      <c r="J938" s="2"/>
-      <c r="K938" s="2"/>
-      <c r="L938" s="2"/>
-      <c r="M938" s="2"/>
-      <c r="N938" s="2"/>
-      <c r="O938" s="2"/>
-      <c r="P938" s="3"/>
-      <c r="Q938" s="3"/>
-      <c r="R938" s="2"/>
-      <c r="S938" s="2"/>
-      <c r="T938" s="2"/>
-      <c r="U938" s="2"/>
-      <c r="V938" s="2"/>
-      <c r="W938" s="2"/>
-      <c r="X938" s="2"/>
-      <c r="Y938" s="2"/>
-      <c r="Z938" s="2"/>
-    </row>
-    <row r="939" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A939" s="11"/>
-      <c r="B939" s="2"/>
-      <c r="C939" s="2"/>
-      <c r="D939" s="2"/>
-      <c r="E939" s="2"/>
-      <c r="F939" s="2"/>
-      <c r="G939" s="2"/>
-      <c r="H939" s="2"/>
-      <c r="I939" s="2"/>
-      <c r="J939" s="2"/>
-      <c r="K939" s="2"/>
-      <c r="L939" s="2"/>
-      <c r="M939" s="2"/>
-      <c r="N939" s="2"/>
-      <c r="O939" s="2"/>
-      <c r="P939" s="3"/>
-      <c r="Q939" s="3"/>
-      <c r="R939" s="2"/>
-      <c r="S939" s="2"/>
-      <c r="T939" s="2"/>
-      <c r="U939" s="2"/>
-      <c r="V939" s="2"/>
-      <c r="W939" s="2"/>
-      <c r="X939" s="2"/>
-      <c r="Y939" s="2"/>
-      <c r="Z939" s="2"/>
-    </row>
-    <row r="940" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A940" s="11"/>
-      <c r="B940" s="2"/>
-      <c r="C940" s="2"/>
-      <c r="D940" s="2"/>
-      <c r="E940" s="2"/>
-      <c r="F940" s="2"/>
-      <c r="G940" s="2"/>
-      <c r="H940" s="2"/>
-      <c r="I940" s="2"/>
-      <c r="J940" s="2"/>
-      <c r="K940" s="2"/>
-      <c r="L940" s="2"/>
-      <c r="M940" s="2"/>
-      <c r="N940" s="2"/>
-      <c r="O940" s="2"/>
-      <c r="P940" s="3"/>
-      <c r="Q940" s="3"/>
-      <c r="R940" s="2"/>
-      <c r="S940" s="2"/>
-      <c r="T940" s="2"/>
-      <c r="U940" s="2"/>
-      <c r="V940" s="2"/>
-      <c r="W940" s="2"/>
-      <c r="X940" s="2"/>
-      <c r="Y940" s="2"/>
-      <c r="Z940" s="2"/>
-    </row>
-    <row r="941" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A941" s="11"/>
-      <c r="B941" s="2"/>
-      <c r="C941" s="2"/>
-      <c r="D941" s="2"/>
-      <c r="E941" s="2"/>
-      <c r="F941" s="2"/>
-      <c r="G941" s="2"/>
-      <c r="H941" s="2"/>
-      <c r="I941" s="2"/>
-      <c r="J941" s="2"/>
-      <c r="K941" s="2"/>
-      <c r="L941" s="2"/>
-      <c r="M941" s="2"/>
-      <c r="N941" s="2"/>
-      <c r="O941" s="2"/>
-      <c r="P941" s="3"/>
-      <c r="Q941" s="3"/>
-      <c r="R941" s="2"/>
-      <c r="S941" s="2"/>
-      <c r="T941" s="2"/>
-      <c r="U941" s="2"/>
-      <c r="V941" s="2"/>
-      <c r="W941" s="2"/>
-      <c r="X941" s="2"/>
-      <c r="Y941" s="2"/>
-      <c r="Z941" s="2"/>
-    </row>
-    <row r="942" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A942" s="11"/>
-      <c r="B942" s="2"/>
-      <c r="C942" s="2"/>
-      <c r="D942" s="2"/>
-      <c r="E942" s="2"/>
-      <c r="F942" s="2"/>
-      <c r="G942" s="2"/>
-      <c r="H942" s="2"/>
-      <c r="I942" s="2"/>
-      <c r="J942" s="2"/>
-      <c r="K942" s="2"/>
-      <c r="L942" s="2"/>
-      <c r="M942" s="2"/>
-      <c r="N942" s="2"/>
-      <c r="O942" s="2"/>
-      <c r="P942" s="3"/>
-      <c r="Q942" s="3"/>
-      <c r="R942" s="2"/>
-      <c r="S942" s="2"/>
-      <c r="T942" s="2"/>
-      <c r="U942" s="2"/>
-      <c r="V942" s="2"/>
-      <c r="W942" s="2"/>
-      <c r="X942" s="2"/>
-      <c r="Y942" s="2"/>
-      <c r="Z942" s="2"/>
-    </row>
-    <row r="943" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A943" s="11"/>
-      <c r="B943" s="2"/>
-      <c r="C943" s="2"/>
-      <c r="D943" s="2"/>
-      <c r="E943" s="2"/>
-      <c r="F943" s="2"/>
-      <c r="G943" s="2"/>
-      <c r="H943" s="2"/>
-      <c r="I943" s="2"/>
-      <c r="J943" s="2"/>
-      <c r="K943" s="2"/>
-      <c r="L943" s="2"/>
-      <c r="M943" s="2"/>
-      <c r="N943" s="2"/>
-      <c r="O943" s="2"/>
-      <c r="P943" s="3"/>
-      <c r="Q943" s="3"/>
-      <c r="R943" s="2"/>
-      <c r="S943" s="2"/>
-      <c r="T943" s="2"/>
-      <c r="U943" s="2"/>
-      <c r="V943" s="2"/>
-      <c r="W943" s="2"/>
-      <c r="X943" s="2"/>
-      <c r="Y943" s="2"/>
-      <c r="Z943" s="2"/>
-    </row>
-    <row r="944" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A944" s="11"/>
-      <c r="B944" s="2"/>
-      <c r="C944" s="2"/>
-      <c r="D944" s="2"/>
-      <c r="E944" s="2"/>
-      <c r="F944" s="2"/>
-      <c r="G944" s="2"/>
-      <c r="H944" s="2"/>
-      <c r="I944" s="2"/>
-      <c r="J944" s="2"/>
-      <c r="K944" s="2"/>
-      <c r="L944" s="2"/>
-      <c r="M944" s="2"/>
-      <c r="N944" s="2"/>
-      <c r="O944" s="2"/>
-      <c r="P944" s="3"/>
-      <c r="Q944" s="3"/>
-      <c r="R944" s="2"/>
-      <c r="S944" s="2"/>
-      <c r="T944" s="2"/>
-      <c r="U944" s="2"/>
-      <c r="V944" s="2"/>
-      <c r="W944" s="2"/>
-      <c r="X944" s="2"/>
-      <c r="Y944" s="2"/>
-      <c r="Z944" s="2"/>
-    </row>
-    <row r="945" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A945" s="11"/>
-      <c r="B945" s="2"/>
-      <c r="C945" s="2"/>
-      <c r="D945" s="2"/>
-      <c r="E945" s="2"/>
-      <c r="F945" s="2"/>
-      <c r="G945" s="2"/>
-      <c r="H945" s="2"/>
-      <c r="I945" s="2"/>
-      <c r="J945" s="2"/>
-      <c r="K945" s="2"/>
-      <c r="L945" s="2"/>
-      <c r="M945" s="2"/>
-      <c r="N945" s="2"/>
-      <c r="O945" s="2"/>
-      <c r="P945" s="3"/>
-      <c r="Q945" s="3"/>
-      <c r="R945" s="2"/>
-      <c r="S945" s="2"/>
-      <c r="T945" s="2"/>
-      <c r="U945" s="2"/>
-      <c r="V945" s="2"/>
-      <c r="W945" s="2"/>
-      <c r="X945" s="2"/>
-      <c r="Y945" s="2"/>
-      <c r="Z945" s="2"/>
-    </row>
-    <row r="946" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A946" s="11"/>
-      <c r="B946" s="2"/>
-      <c r="C946" s="2"/>
-      <c r="D946" s="2"/>
-      <c r="E946" s="2"/>
-      <c r="F946" s="2"/>
-      <c r="G946" s="2"/>
-      <c r="H946" s="2"/>
-      <c r="I946" s="2"/>
-      <c r="J946" s="2"/>
-      <c r="K946" s="2"/>
-      <c r="L946" s="2"/>
-      <c r="M946" s="2"/>
-      <c r="N946" s="2"/>
-      <c r="O946" s="2"/>
-      <c r="P946" s="3"/>
-      <c r="Q946" s="3"/>
-      <c r="R946" s="2"/>
-      <c r="S946" s="2"/>
-      <c r="T946" s="2"/>
-      <c r="U946" s="2"/>
-      <c r="V946" s="2"/>
-      <c r="W946" s="2"/>
-      <c r="X946" s="2"/>
-      <c r="Y946" s="2"/>
-      <c r="Z946" s="2"/>
-    </row>
-    <row r="947" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A947" s="11"/>
-      <c r="B947" s="2"/>
-      <c r="C947" s="2"/>
-      <c r="D947" s="2"/>
-      <c r="E947" s="2"/>
-      <c r="F947" s="2"/>
-      <c r="G947" s="2"/>
-      <c r="H947" s="2"/>
-      <c r="I947" s="2"/>
-      <c r="J947" s="2"/>
-      <c r="K947" s="2"/>
-      <c r="L947" s="2"/>
-      <c r="M947" s="2"/>
-      <c r="N947" s="2"/>
-      <c r="O947" s="2"/>
-      <c r="P947" s="3"/>
-      <c r="Q947" s="3"/>
-      <c r="R947" s="2"/>
-      <c r="S947" s="2"/>
-      <c r="T947" s="2"/>
-      <c r="U947" s="2"/>
-      <c r="V947" s="2"/>
-      <c r="W947" s="2"/>
-      <c r="X947" s="2"/>
-      <c r="Y947" s="2"/>
-      <c r="Z947" s="2"/>
-    </row>
-    <row r="948" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A948" s="11"/>
-      <c r="B948" s="2"/>
-      <c r="C948" s="2"/>
-      <c r="D948" s="2"/>
-      <c r="E948" s="2"/>
-      <c r="F948" s="2"/>
-      <c r="G948" s="2"/>
-      <c r="H948" s="2"/>
-      <c r="I948" s="2"/>
-      <c r="J948" s="2"/>
-      <c r="K948" s="2"/>
-      <c r="L948" s="2"/>
-      <c r="M948" s="2"/>
-      <c r="N948" s="2"/>
-      <c r="O948" s="2"/>
-      <c r="P948" s="3"/>
-      <c r="Q948" s="3"/>
-      <c r="R948" s="2"/>
-      <c r="S948" s="2"/>
-      <c r="T948" s="2"/>
-      <c r="U948" s="2"/>
-      <c r="V948" s="2"/>
-      <c r="W948" s="2"/>
-      <c r="X948" s="2"/>
-      <c r="Y948" s="2"/>
-      <c r="Z948" s="2"/>
-    </row>
-    <row r="949" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A949" s="11"/>
-      <c r="B949" s="2"/>
-      <c r="C949" s="2"/>
-      <c r="D949" s="2"/>
-      <c r="E949" s="2"/>
-      <c r="F949" s="2"/>
-      <c r="G949" s="2"/>
-      <c r="H949" s="2"/>
-      <c r="I949" s="2"/>
-      <c r="J949" s="2"/>
-      <c r="K949" s="2"/>
-      <c r="L949" s="2"/>
-      <c r="M949" s="2"/>
-      <c r="N949" s="2"/>
-      <c r="O949" s="2"/>
-      <c r="P949" s="3"/>
-      <c r="Q949" s="3"/>
-      <c r="R949" s="2"/>
-      <c r="S949" s="2"/>
-      <c r="T949" s="2"/>
-      <c r="U949" s="2"/>
-      <c r="V949" s="2"/>
-      <c r="W949" s="2"/>
-      <c r="X949" s="2"/>
-      <c r="Y949" s="2"/>
-      <c r="Z949" s="2"/>
-    </row>
-    <row r="950" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A950" s="11"/>
-      <c r="B950" s="2"/>
-      <c r="C950" s="2"/>
-      <c r="D950" s="2"/>
-      <c r="E950" s="2"/>
-      <c r="F950" s="2"/>
-      <c r="G950" s="2"/>
-      <c r="H950" s="2"/>
-      <c r="I950" s="2"/>
-      <c r="J950" s="2"/>
-      <c r="K950" s="2"/>
-      <c r="L950" s="2"/>
-      <c r="M950" s="2"/>
-      <c r="N950" s="2"/>
-      <c r="O950" s="2"/>
-      <c r="P950" s="3"/>
-      <c r="Q950" s="3"/>
-      <c r="R950" s="2"/>
-      <c r="S950" s="2"/>
-      <c r="T950" s="2"/>
-      <c r="U950" s="2"/>
-      <c r="V950" s="2"/>
-      <c r="W950" s="2"/>
-      <c r="X950" s="2"/>
-      <c r="Y950" s="2"/>
-      <c r="Z950" s="2"/>
-    </row>
-    <row r="951" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A951" s="11"/>
-      <c r="B951" s="2"/>
-      <c r="C951" s="2"/>
-      <c r="D951" s="2"/>
-      <c r="E951" s="2"/>
-      <c r="F951" s="2"/>
-      <c r="G951" s="2"/>
-      <c r="H951" s="2"/>
-      <c r="I951" s="2"/>
-      <c r="J951" s="2"/>
-      <c r="K951" s="2"/>
-      <c r="L951" s="2"/>
-      <c r="M951" s="2"/>
-      <c r="N951" s="2"/>
-      <c r="O951" s="2"/>
-      <c r="P951" s="3"/>
-      <c r="Q951" s="3"/>
-      <c r="R951" s="2"/>
-      <c r="S951" s="2"/>
-      <c r="T951" s="2"/>
-      <c r="U951" s="2"/>
-      <c r="V951" s="2"/>
-      <c r="W951" s="2"/>
-      <c r="X951" s="2"/>
-      <c r="Y951" s="2"/>
-      <c r="Z951" s="2"/>
-    </row>
-    <row r="952" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A952" s="11"/>
-      <c r="B952" s="2"/>
-      <c r="C952" s="2"/>
-      <c r="D952" s="2"/>
-      <c r="E952" s="2"/>
-      <c r="F952" s="2"/>
-      <c r="G952" s="2"/>
-      <c r="H952" s="2"/>
-      <c r="I952" s="2"/>
-      <c r="J952" s="2"/>
-      <c r="K952" s="2"/>
-      <c r="L952" s="2"/>
-      <c r="M952" s="2"/>
-      <c r="N952" s="2"/>
-      <c r="O952" s="2"/>
-      <c r="P952" s="3"/>
-      <c r="Q952" s="3"/>
-      <c r="R952" s="2"/>
-      <c r="S952" s="2"/>
-      <c r="T952" s="2"/>
-      <c r="U952" s="2"/>
-      <c r="V952" s="2"/>
-      <c r="W952" s="2"/>
-      <c r="X952" s="2"/>
-      <c r="Y952" s="2"/>
-      <c r="Z952" s="2"/>
-    </row>
-    <row r="953" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A953" s="11"/>
-      <c r="B953" s="2"/>
-      <c r="C953" s="2"/>
-      <c r="D953" s="2"/>
-      <c r="E953" s="2"/>
-      <c r="F953" s="2"/>
-      <c r="G953" s="2"/>
-      <c r="H953" s="2"/>
-      <c r="I953" s="2"/>
-      <c r="J953" s="2"/>
-      <c r="K953" s="2"/>
-      <c r="L953" s="2"/>
-      <c r="M953" s="2"/>
-      <c r="N953" s="2"/>
-      <c r="O953" s="2"/>
-      <c r="P953" s="3"/>
-      <c r="Q953" s="3"/>
-      <c r="R953" s="2"/>
-      <c r="S953" s="2"/>
-      <c r="T953" s="2"/>
-      <c r="U953" s="2"/>
-      <c r="V953" s="2"/>
-      <c r="W953" s="2"/>
-      <c r="X953" s="2"/>
-      <c r="Y953" s="2"/>
-      <c r="Z953" s="2"/>
-    </row>
-    <row r="954" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A954" s="11"/>
-      <c r="B954" s="2"/>
-      <c r="C954" s="2"/>
-      <c r="D954" s="2"/>
-      <c r="E954" s="2"/>
-      <c r="F954" s="2"/>
-      <c r="G954" s="2"/>
-      <c r="H954" s="2"/>
-      <c r="I954" s="2"/>
-      <c r="J954" s="2"/>
-      <c r="K954" s="2"/>
-      <c r="L954" s="2"/>
-      <c r="M954" s="2"/>
-      <c r="N954" s="2"/>
-      <c r="O954" s="2"/>
-      <c r="P954" s="3"/>
-      <c r="Q954" s="3"/>
-      <c r="R954" s="2"/>
-      <c r="S954" s="2"/>
-      <c r="T954" s="2"/>
-      <c r="U954" s="2"/>
-      <c r="V954" s="2"/>
-      <c r="W954" s="2"/>
-      <c r="X954" s="2"/>
-      <c r="Y954" s="2"/>
-      <c r="Z954" s="2"/>
-    </row>
-    <row r="955" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A955" s="11"/>
-      <c r="B955" s="2"/>
-      <c r="C955" s="2"/>
-      <c r="D955" s="2"/>
-      <c r="E955" s="2"/>
-      <c r="F955" s="2"/>
-      <c r="G955" s="2"/>
-      <c r="H955" s="2"/>
-      <c r="I955" s="2"/>
-      <c r="J955" s="2"/>
-      <c r="K955" s="2"/>
-      <c r="L955" s="2"/>
-      <c r="M955" s="2"/>
-      <c r="N955" s="2"/>
-      <c r="O955" s="2"/>
-      <c r="P955" s="3"/>
-      <c r="Q955" s="3"/>
-      <c r="R955" s="2"/>
-      <c r="S955" s="2"/>
-      <c r="T955" s="2"/>
-      <c r="U955" s="2"/>
-      <c r="V955" s="2"/>
-      <c r="W955" s="2"/>
-      <c r="X955" s="2"/>
-      <c r="Y955" s="2"/>
-      <c r="Z955" s="2"/>
-    </row>
-    <row r="956" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A956" s="11"/>
-      <c r="B956" s="2"/>
-      <c r="C956" s="2"/>
-      <c r="D956" s="2"/>
-      <c r="E956" s="2"/>
-      <c r="F956" s="2"/>
-      <c r="G956" s="2"/>
-      <c r="H956" s="2"/>
-      <c r="I956" s="2"/>
-      <c r="J956" s="2"/>
-      <c r="K956" s="2"/>
-      <c r="L956" s="2"/>
-      <c r="M956" s="2"/>
-      <c r="N956" s="2"/>
-      <c r="O956" s="2"/>
-      <c r="P956" s="3"/>
-      <c r="Q956" s="3"/>
-      <c r="R956" s="2"/>
-      <c r="S956" s="2"/>
-      <c r="T956" s="2"/>
-      <c r="U956" s="2"/>
-      <c r="V956" s="2"/>
-      <c r="W956" s="2"/>
-      <c r="X956" s="2"/>
-      <c r="Y956" s="2"/>
-      <c r="Z956" s="2"/>
-    </row>
-    <row r="957" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A957" s="11"/>
-      <c r="B957" s="2"/>
-      <c r="C957" s="2"/>
-      <c r="D957" s="2"/>
-      <c r="E957" s="2"/>
-      <c r="F957" s="2"/>
-      <c r="G957" s="2"/>
-      <c r="H957" s="2"/>
-      <c r="I957" s="2"/>
-      <c r="J957" s="2"/>
-      <c r="K957" s="2"/>
-      <c r="L957" s="2"/>
-      <c r="M957" s="2"/>
-      <c r="N957" s="2"/>
-      <c r="O957" s="2"/>
-      <c r="P957" s="3"/>
-      <c r="Q957" s="3"/>
-      <c r="R957" s="2"/>
-      <c r="S957" s="2"/>
-      <c r="T957" s="2"/>
-      <c r="U957" s="2"/>
-      <c r="V957" s="2"/>
-      <c r="W957" s="2"/>
-      <c r="X957" s="2"/>
-      <c r="Y957" s="2"/>
-      <c r="Z957" s="2"/>
-    </row>
-    <row r="958" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A958" s="11"/>
-      <c r="B958" s="2"/>
-      <c r="C958" s="2"/>
-      <c r="D958" s="2"/>
-      <c r="E958" s="2"/>
-      <c r="F958" s="2"/>
-      <c r="G958" s="2"/>
-      <c r="H958" s="2"/>
-      <c r="I958" s="2"/>
-      <c r="J958" s="2"/>
-      <c r="K958" s="2"/>
-      <c r="L958" s="2"/>
-      <c r="M958" s="2"/>
-      <c r="N958" s="2"/>
-      <c r="O958" s="2"/>
-      <c r="P958" s="3"/>
-      <c r="Q958" s="3"/>
-      <c r="R958" s="2"/>
-      <c r="S958" s="2"/>
-      <c r="T958" s="2"/>
-      <c r="U958" s="2"/>
-      <c r="V958" s="2"/>
-      <c r="W958" s="2"/>
-      <c r="X958" s="2"/>
-      <c r="Y958" s="2"/>
-      <c r="Z958" s="2"/>
-    </row>
-    <row r="959" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A959" s="11"/>
-      <c r="B959" s="2"/>
-      <c r="C959" s="2"/>
-      <c r="D959" s="2"/>
-      <c r="E959" s="2"/>
-      <c r="F959" s="2"/>
-      <c r="G959" s="2"/>
-      <c r="H959" s="2"/>
-      <c r="I959" s="2"/>
-      <c r="J959" s="2"/>
-      <c r="K959" s="2"/>
-      <c r="L959" s="2"/>
-      <c r="M959" s="2"/>
-      <c r="N959" s="2"/>
-      <c r="O959" s="2"/>
-      <c r="P959" s="3"/>
-      <c r="Q959" s="3"/>
-      <c r="R959" s="2"/>
-      <c r="S959" s="2"/>
-      <c r="T959" s="2"/>
-      <c r="U959" s="2"/>
-      <c r="V959" s="2"/>
-      <c r="W959" s="2"/>
-      <c r="X959" s="2"/>
-      <c r="Y959" s="2"/>
-      <c r="Z959" s="2"/>
-    </row>
-    <row r="960" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A960" s="11"/>
-      <c r="B960" s="2"/>
-      <c r="C960" s="2"/>
-      <c r="D960" s="2"/>
-      <c r="E960" s="2"/>
-      <c r="F960" s="2"/>
-      <c r="G960" s="2"/>
-      <c r="H960" s="2"/>
-      <c r="I960" s="2"/>
-      <c r="J960" s="2"/>
-      <c r="K960" s="2"/>
-      <c r="L960" s="2"/>
-      <c r="M960" s="2"/>
-      <c r="N960" s="2"/>
-      <c r="O960" s="2"/>
-      <c r="P960" s="3"/>
-      <c r="Q960" s="3"/>
-      <c r="R960" s="2"/>
-      <c r="S960" s="2"/>
-      <c r="T960" s="2"/>
-      <c r="U960" s="2"/>
-      <c r="V960" s="2"/>
-      <c r="W960" s="2"/>
-      <c r="X960" s="2"/>
-      <c r="Y960" s="2"/>
-      <c r="Z960" s="2"/>
-    </row>
-    <row r="961" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A961" s="11"/>
-      <c r="B961" s="2"/>
-      <c r="C961" s="2"/>
-      <c r="D961" s="2"/>
-      <c r="E961" s="2"/>
-      <c r="F961" s="2"/>
-      <c r="G961" s="2"/>
-      <c r="H961" s="2"/>
-      <c r="I961" s="2"/>
-      <c r="J961" s="2"/>
-      <c r="K961" s="2"/>
-      <c r="L961" s="2"/>
-      <c r="M961" s="2"/>
-      <c r="N961" s="2"/>
-      <c r="O961" s="2"/>
-      <c r="P961" s="3"/>
-      <c r="Q961" s="3"/>
-      <c r="R961" s="2"/>
-      <c r="S961" s="2"/>
-      <c r="T961" s="2"/>
-      <c r="U961" s="2"/>
-      <c r="V961" s="2"/>
-      <c r="W961" s="2"/>
-      <c r="X961" s="2"/>
-      <c r="Y961" s="2"/>
-      <c r="Z961" s="2"/>
-    </row>
-    <row r="962" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A962" s="11"/>
-      <c r="B962" s="2"/>
-      <c r="C962" s="2"/>
-      <c r="D962" s="2"/>
-      <c r="E962" s="2"/>
-      <c r="F962" s="2"/>
-      <c r="G962" s="2"/>
-      <c r="H962" s="2"/>
-      <c r="I962" s="2"/>
-      <c r="J962" s="2"/>
-      <c r="K962" s="2"/>
-      <c r="L962" s="2"/>
-      <c r="M962" s="2"/>
-      <c r="N962" s="2"/>
-      <c r="O962" s="2"/>
-      <c r="P962" s="3"/>
-      <c r="Q962" s="3"/>
-      <c r="R962" s="2"/>
-      <c r="S962" s="2"/>
-      <c r="T962" s="2"/>
-      <c r="U962" s="2"/>
-      <c r="V962" s="2"/>
-      <c r="W962" s="2"/>
-      <c r="X962" s="2"/>
-      <c r="Y962" s="2"/>
-      <c r="Z962" s="2"/>
-    </row>
-    <row r="963" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A963" s="11"/>
-      <c r="B963" s="2"/>
-      <c r="C963" s="2"/>
-      <c r="D963" s="2"/>
-      <c r="E963" s="2"/>
-      <c r="F963" s="2"/>
-      <c r="G963" s="2"/>
-      <c r="H963" s="2"/>
-      <c r="I963" s="2"/>
-      <c r="J963" s="2"/>
-      <c r="K963" s="2"/>
-      <c r="L963" s="2"/>
-      <c r="M963" s="2"/>
-      <c r="N963" s="2"/>
-      <c r="O963" s="2"/>
-      <c r="P963" s="3"/>
-      <c r="Q963" s="3"/>
-      <c r="R963" s="2"/>
-      <c r="S963" s="2"/>
-      <c r="T963" s="2"/>
-      <c r="U963" s="2"/>
-      <c r="V963" s="2"/>
-      <c r="W963" s="2"/>
-      <c r="X963" s="2"/>
-      <c r="Y963" s="2"/>
-      <c r="Z963" s="2"/>
-    </row>
-    <row r="964" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A964" s="11"/>
-      <c r="B964" s="2"/>
-      <c r="C964" s="2"/>
-      <c r="D964" s="2"/>
-      <c r="E964" s="2"/>
-      <c r="F964" s="2"/>
-      <c r="G964" s="2"/>
-      <c r="H964" s="2"/>
-      <c r="I964" s="2"/>
-      <c r="J964" s="2"/>
-      <c r="K964" s="2"/>
-      <c r="L964" s="2"/>
-      <c r="M964" s="2"/>
-      <c r="N964" s="2"/>
-      <c r="O964" s="2"/>
-      <c r="P964" s="3"/>
-      <c r="Q964" s="3"/>
-      <c r="R964" s="2"/>
-      <c r="S964" s="2"/>
-      <c r="T964" s="2"/>
-      <c r="U964" s="2"/>
-      <c r="V964" s="2"/>
-      <c r="W964" s="2"/>
-      <c r="X964" s="2"/>
-      <c r="Y964" s="2"/>
-      <c r="Z964" s="2"/>
-    </row>
-    <row r="965" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A965" s="11"/>
-      <c r="B965" s="2"/>
-      <c r="C965" s="2"/>
-      <c r="D965" s="2"/>
-      <c r="E965" s="2"/>
-      <c r="F965" s="2"/>
-      <c r="G965" s="2"/>
-      <c r="H965" s="2"/>
-      <c r="I965" s="2"/>
-      <c r="J965" s="2"/>
-      <c r="K965" s="2"/>
-      <c r="L965" s="2"/>
-      <c r="M965" s="2"/>
-      <c r="N965" s="2"/>
-      <c r="O965" s="2"/>
-      <c r="P965" s="3"/>
-      <c r="Q965" s="3"/>
-      <c r="R965" s="2"/>
-      <c r="S965" s="2"/>
-      <c r="T965" s="2"/>
-      <c r="U965" s="2"/>
-      <c r="V965" s="2"/>
-      <c r="W965" s="2"/>
-      <c r="X965" s="2"/>
-      <c r="Y965" s="2"/>
-      <c r="Z965" s="2"/>
-    </row>
-    <row r="966" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A966" s="11"/>
-      <c r="B966" s="2"/>
-      <c r="C966" s="2"/>
-      <c r="D966" s="2"/>
-      <c r="E966" s="2"/>
-      <c r="F966" s="2"/>
-      <c r="G966" s="2"/>
-      <c r="H966" s="2"/>
-      <c r="I966" s="2"/>
-      <c r="J966" s="2"/>
-      <c r="K966" s="2"/>
-      <c r="L966" s="2"/>
-      <c r="M966" s="2"/>
-      <c r="N966" s="2"/>
-      <c r="O966" s="2"/>
-      <c r="P966" s="3"/>
-      <c r="Q966" s="3"/>
-      <c r="R966" s="2"/>
-      <c r="S966" s="2"/>
-      <c r="T966" s="2"/>
-      <c r="U966" s="2"/>
-      <c r="V966" s="2"/>
-      <c r="W966" s="2"/>
-      <c r="X966" s="2"/>
-      <c r="Y966" s="2"/>
-      <c r="Z966" s="2"/>
-    </row>
-    <row r="967" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A967" s="11"/>
-      <c r="B967" s="2"/>
-      <c r="C967" s="2"/>
-      <c r="D967" s="2"/>
-      <c r="E967" s="2"/>
-      <c r="F967" s="2"/>
-      <c r="G967" s="2"/>
-      <c r="H967" s="2"/>
-      <c r="I967" s="2"/>
-      <c r="J967" s="2"/>
-      <c r="K967" s="2"/>
-      <c r="L967" s="2"/>
-      <c r="M967" s="2"/>
-      <c r="N967" s="2"/>
-      <c r="O967" s="2"/>
-      <c r="P967" s="3"/>
-      <c r="Q967" s="3"/>
-      <c r="R967" s="2"/>
-      <c r="S967" s="2"/>
-      <c r="T967" s="2"/>
-      <c r="U967" s="2"/>
-      <c r="V967" s="2"/>
-      <c r="W967" s="2"/>
-      <c r="X967" s="2"/>
-      <c r="Y967" s="2"/>
-      <c r="Z967" s="2"/>
-    </row>
-    <row r="968" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A968" s="11"/>
-      <c r="B968" s="2"/>
-      <c r="C968" s="2"/>
-      <c r="D968" s="2"/>
-      <c r="E968" s="2"/>
-      <c r="F968" s="2"/>
-      <c r="G968" s="2"/>
-      <c r="H968" s="2"/>
-      <c r="I968" s="2"/>
-      <c r="J968" s="2"/>
-      <c r="K968" s="2"/>
-      <c r="L968" s="2"/>
-      <c r="M968" s="2"/>
-      <c r="N968" s="2"/>
-      <c r="O968" s="2"/>
-      <c r="P968" s="3"/>
-      <c r="Q968" s="3"/>
-      <c r="R968" s="2"/>
-      <c r="S968" s="2"/>
-      <c r="T968" s="2"/>
-      <c r="U968" s="2"/>
-      <c r="V968" s="2"/>
-      <c r="W968" s="2"/>
-      <c r="X968" s="2"/>
-      <c r="Y968" s="2"/>
-      <c r="Z968" s="2"/>
-    </row>
-    <row r="969" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A969" s="11"/>
-      <c r="B969" s="2"/>
-      <c r="C969" s="2"/>
-      <c r="D969" s="2"/>
-      <c r="E969" s="2"/>
-      <c r="F969" s="2"/>
-      <c r="G969" s="2"/>
-      <c r="H969" s="2"/>
-      <c r="I969" s="2"/>
-      <c r="J969" s="2"/>
-      <c r="K969" s="2"/>
-      <c r="L969" s="2"/>
-      <c r="M969" s="2"/>
-      <c r="N969" s="2"/>
-      <c r="O969" s="2"/>
-      <c r="P969" s="3"/>
-      <c r="Q969" s="3"/>
-      <c r="R969" s="2"/>
-      <c r="S969" s="2"/>
-      <c r="T969" s="2"/>
-      <c r="U969" s="2"/>
-      <c r="V969" s="2"/>
-      <c r="W969" s="2"/>
-      <c r="X969" s="2"/>
-      <c r="Y969" s="2"/>
-      <c r="Z969" s="2"/>
-    </row>
-    <row r="970" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A970" s="11"/>
-      <c r="B970" s="2"/>
-      <c r="C970" s="2"/>
-      <c r="D970" s="2"/>
-      <c r="E970" s="2"/>
-      <c r="F970" s="2"/>
-      <c r="G970" s="2"/>
-      <c r="H970" s="2"/>
-      <c r="I970" s="2"/>
-      <c r="J970" s="2"/>
-      <c r="K970" s="2"/>
-      <c r="L970" s="2"/>
-      <c r="M970" s="2"/>
-      <c r="N970" s="2"/>
-      <c r="O970" s="2"/>
-      <c r="P970" s="3"/>
-      <c r="Q970" s="3"/>
-      <c r="R970" s="2"/>
-      <c r="S970" s="2"/>
-      <c r="T970" s="2"/>
-      <c r="U970" s="2"/>
-      <c r="V970" s="2"/>
-      <c r="W970" s="2"/>
-      <c r="X970" s="2"/>
-      <c r="Y970" s="2"/>
-      <c r="Z970" s="2"/>
-    </row>
-    <row r="971" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A971" s="11"/>
-      <c r="B971" s="2"/>
-      <c r="C971" s="2"/>
-      <c r="D971" s="2"/>
-      <c r="E971" s="2"/>
-      <c r="F971" s="2"/>
-      <c r="G971" s="2"/>
-      <c r="H971" s="2"/>
-      <c r="I971" s="2"/>
-      <c r="J971" s="2"/>
-      <c r="K971" s="2"/>
-      <c r="L971" s="2"/>
-      <c r="M971" s="2"/>
-      <c r="N971" s="2"/>
-      <c r="O971" s="2"/>
-      <c r="P971" s="3"/>
-      <c r="Q971" s="3"/>
-      <c r="R971" s="2"/>
-      <c r="S971" s="2"/>
-      <c r="T971" s="2"/>
-      <c r="U971" s="2"/>
-      <c r="V971" s="2"/>
-      <c r="W971" s="2"/>
-      <c r="X971" s="2"/>
-      <c r="Y971" s="2"/>
-      <c r="Z971" s="2"/>
-    </row>
-    <row r="972" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A972" s="11"/>
-      <c r="B972" s="2"/>
-      <c r="C972" s="2"/>
-      <c r="D972" s="2"/>
-      <c r="E972" s="2"/>
-      <c r="F972" s="2"/>
-      <c r="G972" s="2"/>
-      <c r="H972" s="2"/>
-      <c r="I972" s="2"/>
-      <c r="J972" s="2"/>
-      <c r="K972" s="2"/>
-      <c r="L972" s="2"/>
-      <c r="M972" s="2"/>
-      <c r="N972" s="2"/>
-      <c r="O972" s="2"/>
-      <c r="P972" s="3"/>
-      <c r="Q972" s="3"/>
-      <c r="R972" s="2"/>
-      <c r="S972" s="2"/>
-      <c r="T972" s="2"/>
-      <c r="U972" s="2"/>
-      <c r="V972" s="2"/>
-      <c r="W972" s="2"/>
-      <c r="X972" s="2"/>
-      <c r="Y972" s="2"/>
-      <c r="Z972" s="2"/>
-    </row>
-    <row r="973" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A973" s="11"/>
-      <c r="B973" s="2"/>
-      <c r="C973" s="2"/>
-      <c r="D973" s="2"/>
-      <c r="E973" s="2"/>
-      <c r="F973" s="2"/>
-      <c r="G973" s="2"/>
-      <c r="H973" s="2"/>
-      <c r="I973" s="2"/>
-      <c r="J973" s="2"/>
-      <c r="K973" s="2"/>
-      <c r="L973" s="2"/>
-      <c r="M973" s="2"/>
-      <c r="N973" s="2"/>
-      <c r="O973" s="2"/>
-      <c r="P973" s="3"/>
-      <c r="Q973" s="3"/>
-      <c r="R973" s="2"/>
-      <c r="S973" s="2"/>
-      <c r="T973" s="2"/>
-      <c r="U973" s="2"/>
-      <c r="V973" s="2"/>
-      <c r="W973" s="2"/>
-      <c r="X973" s="2"/>
-      <c r="Y973" s="2"/>
-      <c r="Z973" s="2"/>
-    </row>
-    <row r="974" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A974" s="11"/>
-      <c r="B974" s="2"/>
-      <c r="C974" s="2"/>
-      <c r="D974" s="2"/>
-      <c r="E974" s="2"/>
-      <c r="F974" s="2"/>
-      <c r="G974" s="2"/>
-      <c r="H974" s="2"/>
-      <c r="I974" s="2"/>
-      <c r="J974" s="2"/>
-      <c r="K974" s="2"/>
-      <c r="L974" s="2"/>
-      <c r="M974" s="2"/>
-      <c r="N974" s="2"/>
-      <c r="O974" s="2"/>
-      <c r="P974" s="3"/>
-      <c r="Q974" s="3"/>
-      <c r="R974" s="2"/>
-      <c r="S974" s="2"/>
-      <c r="T974" s="2"/>
-      <c r="U974" s="2"/>
-      <c r="V974" s="2"/>
-      <c r="W974" s="2"/>
-      <c r="X974" s="2"/>
-      <c r="Y974" s="2"/>
-      <c r="Z974" s="2"/>
-    </row>
-    <row r="975" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A975" s="11"/>
-      <c r="B975" s="2"/>
-      <c r="C975" s="2"/>
-      <c r="D975" s="2"/>
-      <c r="E975" s="2"/>
-      <c r="F975" s="2"/>
-      <c r="G975" s="2"/>
-      <c r="H975" s="2"/>
-      <c r="I975" s="2"/>
-      <c r="J975" s="2"/>
-      <c r="K975" s="2"/>
-      <c r="L975" s="2"/>
-      <c r="M975" s="2"/>
-      <c r="N975" s="2"/>
-      <c r="O975" s="2"/>
-      <c r="P975" s="3"/>
-      <c r="Q975" s="3"/>
-      <c r="R975" s="2"/>
-      <c r="S975" s="2"/>
-      <c r="T975" s="2"/>
-      <c r="U975" s="2"/>
-      <c r="V975" s="2"/>
-      <c r="W975" s="2"/>
-      <c r="X975" s="2"/>
-      <c r="Y975" s="2"/>
-      <c r="Z975" s="2"/>
-    </row>
-    <row r="976" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A976" s="11"/>
-      <c r="B976" s="2"/>
-      <c r="C976" s="2"/>
-      <c r="D976" s="2"/>
-      <c r="E976" s="2"/>
-      <c r="F976" s="2"/>
-      <c r="G976" s="2"/>
-      <c r="H976" s="2"/>
-      <c r="I976" s="2"/>
-      <c r="J976" s="2"/>
-      <c r="K976" s="2"/>
-      <c r="L976" s="2"/>
-      <c r="M976" s="2"/>
-      <c r="N976" s="2"/>
-      <c r="O976" s="2"/>
-      <c r="P976" s="3"/>
-      <c r="Q976" s="3"/>
-      <c r="R976" s="2"/>
-      <c r="S976" s="2"/>
-      <c r="T976" s="2"/>
-      <c r="U976" s="2"/>
-      <c r="V976" s="2"/>
-      <c r="W976" s="2"/>
-      <c r="X976" s="2"/>
-      <c r="Y976" s="2"/>
-      <c r="Z976" s="2"/>
-    </row>
-    <row r="977" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A977" s="11"/>
-      <c r="B977" s="2"/>
-      <c r="C977" s="2"/>
-      <c r="D977" s="2"/>
-      <c r="E977" s="2"/>
-      <c r="F977" s="2"/>
-      <c r="G977" s="2"/>
-      <c r="H977" s="2"/>
-      <c r="I977" s="2"/>
-      <c r="J977" s="2"/>
-      <c r="K977" s="2"/>
-      <c r="L977" s="2"/>
-      <c r="M977" s="2"/>
-      <c r="N977" s="2"/>
-      <c r="O977" s="2"/>
-      <c r="P977" s="3"/>
-      <c r="Q977" s="3"/>
-      <c r="R977" s="2"/>
-      <c r="S977" s="2"/>
-      <c r="T977" s="2"/>
-      <c r="U977" s="2"/>
-      <c r="V977" s="2"/>
-      <c r="W977" s="2"/>
-      <c r="X977" s="2"/>
-      <c r="Y977" s="2"/>
-      <c r="Z977" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A9:F9"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D8:D11" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D8" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Fixed Price,OSDC,Bodyshop,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Checkpoint before assistant change: Improve Excel export API by using row duplication instead of insertion for better performance.
Replit-Commit-Author: Assistant
</commit_message>
<xml_diff>
--- a/src/template/template.xlsx
+++ b/src/template/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiennm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F48235-4F43-4A2D-BDAC-CD3BB12D3CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6B8534-3890-4455-AADD-2F01ED0CAD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01.Summary" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Số giờ làm thêm từ T2-T7</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>Hyperlink</t>
-  </si>
-  <si>
-    <t>Tổng số</t>
   </si>
 </sst>
 </file>
@@ -209,27 +206,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -288,132 +270,77 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -634,10 +561,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:Z849"/>
+  <dimension ref="A1:Z847"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -687,17 +614,17 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="16"/>
       <c r="J2" s="4"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -864,66 +791,66 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="17" t="s">
+      <c r="O7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="18" t="s">
+      <c r="P7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="19"/>
-      <c r="X7" s="19"/>
-      <c r="Y7" s="19"/>
-      <c r="Z7" s="19"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
     </row>
     <row r="8" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
@@ -953,53 +880,24 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="31">
-        <f>SUM(G8:G8)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="31">
-        <f t="shared" ref="H9:M9" si="0">SUM(H8:H8)</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="33">
-        <f>SUM(P8:P8)</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="33">
-        <f>SUM(Q8:Q8)</f>
-        <v>0</v>
-      </c>
+    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
@@ -24474,66 +24372,9 @@
       <c r="Y847" s="2"/>
       <c r="Z847" s="2"/>
     </row>
-    <row r="848" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A848" s="11"/>
-      <c r="B848" s="2"/>
-      <c r="C848" s="2"/>
-      <c r="D848" s="2"/>
-      <c r="E848" s="2"/>
-      <c r="F848" s="2"/>
-      <c r="G848" s="2"/>
-      <c r="H848" s="2"/>
-      <c r="I848" s="2"/>
-      <c r="J848" s="2"/>
-      <c r="K848" s="2"/>
-      <c r="L848" s="2"/>
-      <c r="M848" s="2"/>
-      <c r="N848" s="2"/>
-      <c r="O848" s="2"/>
-      <c r="P848" s="3"/>
-      <c r="Q848" s="3"/>
-      <c r="R848" s="2"/>
-      <c r="S848" s="2"/>
-      <c r="T848" s="2"/>
-      <c r="U848" s="2"/>
-      <c r="V848" s="2"/>
-      <c r="W848" s="2"/>
-      <c r="X848" s="2"/>
-      <c r="Y848" s="2"/>
-      <c r="Z848" s="2"/>
-    </row>
-    <row r="849" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A849" s="11"/>
-      <c r="B849" s="2"/>
-      <c r="C849" s="2"/>
-      <c r="D849" s="2"/>
-      <c r="E849" s="2"/>
-      <c r="F849" s="2"/>
-      <c r="G849" s="2"/>
-      <c r="H849" s="2"/>
-      <c r="I849" s="2"/>
-      <c r="J849" s="2"/>
-      <c r="K849" s="2"/>
-      <c r="L849" s="2"/>
-      <c r="M849" s="2"/>
-      <c r="N849" s="2"/>
-      <c r="O849" s="2"/>
-      <c r="P849" s="3"/>
-      <c r="Q849" s="3"/>
-      <c r="R849" s="2"/>
-      <c r="S849" s="2"/>
-      <c r="T849" s="2"/>
-      <c r="U849" s="2"/>
-      <c r="V849" s="2"/>
-      <c r="W849" s="2"/>
-      <c r="X849" s="2"/>
-      <c r="Y849" s="2"/>
-      <c r="Z849" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A9:F9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D8" xr:uid="{00000000-0002-0000-0200-000000000000}">

</xml_diff>

<commit_message>
Checkpoint before assistant change: Improve Excel export logic:  Data is now written directly to the sheet without unnecessary row duplication.
Replit-Commit-Author: Assistant
</commit_message>
<xml_diff>
--- a/src/template/template.xlsx
+++ b/src/template/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiennm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6B8534-3890-4455-AADD-2F01ED0CAD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700B7B4B-A648-465A-B1AA-3DD653612EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Số giờ làm thêm từ T2-T7</t>
   </si>
@@ -106,14 +106,30 @@
   <si>
     <t>Hyperlink</t>
   </si>
+  <si>
+    <t>Tổng số</t>
+  </si>
+  <si>
+    <t>Người tổng hợp</t>
+  </si>
+  <si>
+    <t>Trưởng Bộ phận</t>
+  </si>
+  <si>
+    <t>TienNM</t>
+  </si>
+  <si>
+    <t>NghiaNH</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0_ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -127,39 +143,33 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000080"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -206,12 +216,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -244,105 +269,141 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
         <color rgb="FF000000"/>
-      </left>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,10 +622,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:Z847"/>
+  <dimension ref="A1:Z977"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -614,17 +675,17 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="4"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -791,85 +852,85 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="21" t="s">
+      <c r="O7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="P7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="22" t="s">
+      <c r="Q7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
     </row>
     <row r="8" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
@@ -880,24 +941,24 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
+    <row r="9" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
@@ -908,24 +969,24 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+    <row r="10" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
@@ -936,24 +997,24 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+    <row r="11" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
@@ -964,257 +1025,297 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
+    <row r="12" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="26">
+        <f t="shared" ref="G12:M12" si="0">SUM(G8:G11)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="27"/>
+      <c r="O12" s="24" t="str">
+        <f t="shared" ref="O8:O12" si="1">IF(LEN(N12)&gt;0,HYPERLINK("#'" &amp; N12 &amp; "'!A1","Link"),"")</f>
+        <v/>
+      </c>
+      <c r="P12" s="28">
+        <f t="shared" ref="P12:Q12" si="2">SUM(P8:P11)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
     </row>
     <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
     </row>
     <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
     </row>
     <row r="16" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
     </row>
     <row r="17" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="2"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
     </row>
     <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
     </row>
     <row r="19" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="2"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
     </row>
     <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
     </row>
     <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
@@ -1275,11 +1376,11 @@
     <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="C23" s="7"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="7"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -24372,12 +24473,3653 @@
       <c r="Y847" s="2"/>
       <c r="Z847" s="2"/>
     </row>
+    <row r="848" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A848" s="11"/>
+      <c r="B848" s="2"/>
+      <c r="C848" s="2"/>
+      <c r="D848" s="2"/>
+      <c r="E848" s="2"/>
+      <c r="F848" s="2"/>
+      <c r="G848" s="2"/>
+      <c r="H848" s="2"/>
+      <c r="I848" s="2"/>
+      <c r="J848" s="2"/>
+      <c r="K848" s="2"/>
+      <c r="L848" s="2"/>
+      <c r="M848" s="2"/>
+      <c r="N848" s="2"/>
+      <c r="O848" s="2"/>
+      <c r="P848" s="3"/>
+      <c r="Q848" s="3"/>
+      <c r="R848" s="2"/>
+      <c r="S848" s="2"/>
+      <c r="T848" s="2"/>
+      <c r="U848" s="2"/>
+      <c r="V848" s="2"/>
+      <c r="W848" s="2"/>
+      <c r="X848" s="2"/>
+      <c r="Y848" s="2"/>
+      <c r="Z848" s="2"/>
+    </row>
+    <row r="849" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A849" s="11"/>
+      <c r="B849" s="2"/>
+      <c r="C849" s="2"/>
+      <c r="D849" s="2"/>
+      <c r="E849" s="2"/>
+      <c r="F849" s="2"/>
+      <c r="G849" s="2"/>
+      <c r="H849" s="2"/>
+      <c r="I849" s="2"/>
+      <c r="J849" s="2"/>
+      <c r="K849" s="2"/>
+      <c r="L849" s="2"/>
+      <c r="M849" s="2"/>
+      <c r="N849" s="2"/>
+      <c r="O849" s="2"/>
+      <c r="P849" s="3"/>
+      <c r="Q849" s="3"/>
+      <c r="R849" s="2"/>
+      <c r="S849" s="2"/>
+      <c r="T849" s="2"/>
+      <c r="U849" s="2"/>
+      <c r="V849" s="2"/>
+      <c r="W849" s="2"/>
+      <c r="X849" s="2"/>
+      <c r="Y849" s="2"/>
+      <c r="Z849" s="2"/>
+    </row>
+    <row r="850" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A850" s="11"/>
+      <c r="B850" s="2"/>
+      <c r="C850" s="2"/>
+      <c r="D850" s="2"/>
+      <c r="E850" s="2"/>
+      <c r="F850" s="2"/>
+      <c r="G850" s="2"/>
+      <c r="H850" s="2"/>
+      <c r="I850" s="2"/>
+      <c r="J850" s="2"/>
+      <c r="K850" s="2"/>
+      <c r="L850" s="2"/>
+      <c r="M850" s="2"/>
+      <c r="N850" s="2"/>
+      <c r="O850" s="2"/>
+      <c r="P850" s="3"/>
+      <c r="Q850" s="3"/>
+      <c r="R850" s="2"/>
+      <c r="S850" s="2"/>
+      <c r="T850" s="2"/>
+      <c r="U850" s="2"/>
+      <c r="V850" s="2"/>
+      <c r="W850" s="2"/>
+      <c r="X850" s="2"/>
+      <c r="Y850" s="2"/>
+      <c r="Z850" s="2"/>
+    </row>
+    <row r="851" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A851" s="11"/>
+      <c r="B851" s="2"/>
+      <c r="C851" s="2"/>
+      <c r="D851" s="2"/>
+      <c r="E851" s="2"/>
+      <c r="F851" s="2"/>
+      <c r="G851" s="2"/>
+      <c r="H851" s="2"/>
+      <c r="I851" s="2"/>
+      <c r="J851" s="2"/>
+      <c r="K851" s="2"/>
+      <c r="L851" s="2"/>
+      <c r="M851" s="2"/>
+      <c r="N851" s="2"/>
+      <c r="O851" s="2"/>
+      <c r="P851" s="3"/>
+      <c r="Q851" s="3"/>
+      <c r="R851" s="2"/>
+      <c r="S851" s="2"/>
+      <c r="T851" s="2"/>
+      <c r="U851" s="2"/>
+      <c r="V851" s="2"/>
+      <c r="W851" s="2"/>
+      <c r="X851" s="2"/>
+      <c r="Y851" s="2"/>
+      <c r="Z851" s="2"/>
+    </row>
+    <row r="852" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A852" s="11"/>
+      <c r="B852" s="2"/>
+      <c r="C852" s="2"/>
+      <c r="D852" s="2"/>
+      <c r="E852" s="2"/>
+      <c r="F852" s="2"/>
+      <c r="G852" s="2"/>
+      <c r="H852" s="2"/>
+      <c r="I852" s="2"/>
+      <c r="J852" s="2"/>
+      <c r="K852" s="2"/>
+      <c r="L852" s="2"/>
+      <c r="M852" s="2"/>
+      <c r="N852" s="2"/>
+      <c r="O852" s="2"/>
+      <c r="P852" s="3"/>
+      <c r="Q852" s="3"/>
+      <c r="R852" s="2"/>
+      <c r="S852" s="2"/>
+      <c r="T852" s="2"/>
+      <c r="U852" s="2"/>
+      <c r="V852" s="2"/>
+      <c r="W852" s="2"/>
+      <c r="X852" s="2"/>
+      <c r="Y852" s="2"/>
+      <c r="Z852" s="2"/>
+    </row>
+    <row r="853" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A853" s="11"/>
+      <c r="B853" s="2"/>
+      <c r="C853" s="2"/>
+      <c r="D853" s="2"/>
+      <c r="E853" s="2"/>
+      <c r="F853" s="2"/>
+      <c r="G853" s="2"/>
+      <c r="H853" s="2"/>
+      <c r="I853" s="2"/>
+      <c r="J853" s="2"/>
+      <c r="K853" s="2"/>
+      <c r="L853" s="2"/>
+      <c r="M853" s="2"/>
+      <c r="N853" s="2"/>
+      <c r="O853" s="2"/>
+      <c r="P853" s="3"/>
+      <c r="Q853" s="3"/>
+      <c r="R853" s="2"/>
+      <c r="S853" s="2"/>
+      <c r="T853" s="2"/>
+      <c r="U853" s="2"/>
+      <c r="V853" s="2"/>
+      <c r="W853" s="2"/>
+      <c r="X853" s="2"/>
+      <c r="Y853" s="2"/>
+      <c r="Z853" s="2"/>
+    </row>
+    <row r="854" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A854" s="11"/>
+      <c r="B854" s="2"/>
+      <c r="C854" s="2"/>
+      <c r="D854" s="2"/>
+      <c r="E854" s="2"/>
+      <c r="F854" s="2"/>
+      <c r="G854" s="2"/>
+      <c r="H854" s="2"/>
+      <c r="I854" s="2"/>
+      <c r="J854" s="2"/>
+      <c r="K854" s="2"/>
+      <c r="L854" s="2"/>
+      <c r="M854" s="2"/>
+      <c r="N854" s="2"/>
+      <c r="O854" s="2"/>
+      <c r="P854" s="3"/>
+      <c r="Q854" s="3"/>
+      <c r="R854" s="2"/>
+      <c r="S854" s="2"/>
+      <c r="T854" s="2"/>
+      <c r="U854" s="2"/>
+      <c r="V854" s="2"/>
+      <c r="W854" s="2"/>
+      <c r="X854" s="2"/>
+      <c r="Y854" s="2"/>
+      <c r="Z854" s="2"/>
+    </row>
+    <row r="855" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A855" s="11"/>
+      <c r="B855" s="2"/>
+      <c r="C855" s="2"/>
+      <c r="D855" s="2"/>
+      <c r="E855" s="2"/>
+      <c r="F855" s="2"/>
+      <c r="G855" s="2"/>
+      <c r="H855" s="2"/>
+      <c r="I855" s="2"/>
+      <c r="J855" s="2"/>
+      <c r="K855" s="2"/>
+      <c r="L855" s="2"/>
+      <c r="M855" s="2"/>
+      <c r="N855" s="2"/>
+      <c r="O855" s="2"/>
+      <c r="P855" s="3"/>
+      <c r="Q855" s="3"/>
+      <c r="R855" s="2"/>
+      <c r="S855" s="2"/>
+      <c r="T855" s="2"/>
+      <c r="U855" s="2"/>
+      <c r="V855" s="2"/>
+      <c r="W855" s="2"/>
+      <c r="X855" s="2"/>
+      <c r="Y855" s="2"/>
+      <c r="Z855" s="2"/>
+    </row>
+    <row r="856" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A856" s="11"/>
+      <c r="B856" s="2"/>
+      <c r="C856" s="2"/>
+      <c r="D856" s="2"/>
+      <c r="E856" s="2"/>
+      <c r="F856" s="2"/>
+      <c r="G856" s="2"/>
+      <c r="H856" s="2"/>
+      <c r="I856" s="2"/>
+      <c r="J856" s="2"/>
+      <c r="K856" s="2"/>
+      <c r="L856" s="2"/>
+      <c r="M856" s="2"/>
+      <c r="N856" s="2"/>
+      <c r="O856" s="2"/>
+      <c r="P856" s="3"/>
+      <c r="Q856" s="3"/>
+      <c r="R856" s="2"/>
+      <c r="S856" s="2"/>
+      <c r="T856" s="2"/>
+      <c r="U856" s="2"/>
+      <c r="V856" s="2"/>
+      <c r="W856" s="2"/>
+      <c r="X856" s="2"/>
+      <c r="Y856" s="2"/>
+      <c r="Z856" s="2"/>
+    </row>
+    <row r="857" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A857" s="11"/>
+      <c r="B857" s="2"/>
+      <c r="C857" s="2"/>
+      <c r="D857" s="2"/>
+      <c r="E857" s="2"/>
+      <c r="F857" s="2"/>
+      <c r="G857" s="2"/>
+      <c r="H857" s="2"/>
+      <c r="I857" s="2"/>
+      <c r="J857" s="2"/>
+      <c r="K857" s="2"/>
+      <c r="L857" s="2"/>
+      <c r="M857" s="2"/>
+      <c r="N857" s="2"/>
+      <c r="O857" s="2"/>
+      <c r="P857" s="3"/>
+      <c r="Q857" s="3"/>
+      <c r="R857" s="2"/>
+      <c r="S857" s="2"/>
+      <c r="T857" s="2"/>
+      <c r="U857" s="2"/>
+      <c r="V857" s="2"/>
+      <c r="W857" s="2"/>
+      <c r="X857" s="2"/>
+      <c r="Y857" s="2"/>
+      <c r="Z857" s="2"/>
+    </row>
+    <row r="858" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A858" s="11"/>
+      <c r="B858" s="2"/>
+      <c r="C858" s="2"/>
+      <c r="D858" s="2"/>
+      <c r="E858" s="2"/>
+      <c r="F858" s="2"/>
+      <c r="G858" s="2"/>
+      <c r="H858" s="2"/>
+      <c r="I858" s="2"/>
+      <c r="J858" s="2"/>
+      <c r="K858" s="2"/>
+      <c r="L858" s="2"/>
+      <c r="M858" s="2"/>
+      <c r="N858" s="2"/>
+      <c r="O858" s="2"/>
+      <c r="P858" s="3"/>
+      <c r="Q858" s="3"/>
+      <c r="R858" s="2"/>
+      <c r="S858" s="2"/>
+      <c r="T858" s="2"/>
+      <c r="U858" s="2"/>
+      <c r="V858" s="2"/>
+      <c r="W858" s="2"/>
+      <c r="X858" s="2"/>
+      <c r="Y858" s="2"/>
+      <c r="Z858" s="2"/>
+    </row>
+    <row r="859" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A859" s="11"/>
+      <c r="B859" s="2"/>
+      <c r="C859" s="2"/>
+      <c r="D859" s="2"/>
+      <c r="E859" s="2"/>
+      <c r="F859" s="2"/>
+      <c r="G859" s="2"/>
+      <c r="H859" s="2"/>
+      <c r="I859" s="2"/>
+      <c r="J859" s="2"/>
+      <c r="K859" s="2"/>
+      <c r="L859" s="2"/>
+      <c r="M859" s="2"/>
+      <c r="N859" s="2"/>
+      <c r="O859" s="2"/>
+      <c r="P859" s="3"/>
+      <c r="Q859" s="3"/>
+      <c r="R859" s="2"/>
+      <c r="S859" s="2"/>
+      <c r="T859" s="2"/>
+      <c r="U859" s="2"/>
+      <c r="V859" s="2"/>
+      <c r="W859" s="2"/>
+      <c r="X859" s="2"/>
+      <c r="Y859" s="2"/>
+      <c r="Z859" s="2"/>
+    </row>
+    <row r="860" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A860" s="11"/>
+      <c r="B860" s="2"/>
+      <c r="C860" s="2"/>
+      <c r="D860" s="2"/>
+      <c r="E860" s="2"/>
+      <c r="F860" s="2"/>
+      <c r="G860" s="2"/>
+      <c r="H860" s="2"/>
+      <c r="I860" s="2"/>
+      <c r="J860" s="2"/>
+      <c r="K860" s="2"/>
+      <c r="L860" s="2"/>
+      <c r="M860" s="2"/>
+      <c r="N860" s="2"/>
+      <c r="O860" s="2"/>
+      <c r="P860" s="3"/>
+      <c r="Q860" s="3"/>
+      <c r="R860" s="2"/>
+      <c r="S860" s="2"/>
+      <c r="T860" s="2"/>
+      <c r="U860" s="2"/>
+      <c r="V860" s="2"/>
+      <c r="W860" s="2"/>
+      <c r="X860" s="2"/>
+      <c r="Y860" s="2"/>
+      <c r="Z860" s="2"/>
+    </row>
+    <row r="861" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A861" s="11"/>
+      <c r="B861" s="2"/>
+      <c r="C861" s="2"/>
+      <c r="D861" s="2"/>
+      <c r="E861" s="2"/>
+      <c r="F861" s="2"/>
+      <c r="G861" s="2"/>
+      <c r="H861" s="2"/>
+      <c r="I861" s="2"/>
+      <c r="J861" s="2"/>
+      <c r="K861" s="2"/>
+      <c r="L861" s="2"/>
+      <c r="M861" s="2"/>
+      <c r="N861" s="2"/>
+      <c r="O861" s="2"/>
+      <c r="P861" s="3"/>
+      <c r="Q861" s="3"/>
+      <c r="R861" s="2"/>
+      <c r="S861" s="2"/>
+      <c r="T861" s="2"/>
+      <c r="U861" s="2"/>
+      <c r="V861" s="2"/>
+      <c r="W861" s="2"/>
+      <c r="X861" s="2"/>
+      <c r="Y861" s="2"/>
+      <c r="Z861" s="2"/>
+    </row>
+    <row r="862" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A862" s="11"/>
+      <c r="B862" s="2"/>
+      <c r="C862" s="2"/>
+      <c r="D862" s="2"/>
+      <c r="E862" s="2"/>
+      <c r="F862" s="2"/>
+      <c r="G862" s="2"/>
+      <c r="H862" s="2"/>
+      <c r="I862" s="2"/>
+      <c r="J862" s="2"/>
+      <c r="K862" s="2"/>
+      <c r="L862" s="2"/>
+      <c r="M862" s="2"/>
+      <c r="N862" s="2"/>
+      <c r="O862" s="2"/>
+      <c r="P862" s="3"/>
+      <c r="Q862" s="3"/>
+      <c r="R862" s="2"/>
+      <c r="S862" s="2"/>
+      <c r="T862" s="2"/>
+      <c r="U862" s="2"/>
+      <c r="V862" s="2"/>
+      <c r="W862" s="2"/>
+      <c r="X862" s="2"/>
+      <c r="Y862" s="2"/>
+      <c r="Z862" s="2"/>
+    </row>
+    <row r="863" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A863" s="11"/>
+      <c r="B863" s="2"/>
+      <c r="C863" s="2"/>
+      <c r="D863" s="2"/>
+      <c r="E863" s="2"/>
+      <c r="F863" s="2"/>
+      <c r="G863" s="2"/>
+      <c r="H863" s="2"/>
+      <c r="I863" s="2"/>
+      <c r="J863" s="2"/>
+      <c r="K863" s="2"/>
+      <c r="L863" s="2"/>
+      <c r="M863" s="2"/>
+      <c r="N863" s="2"/>
+      <c r="O863" s="2"/>
+      <c r="P863" s="3"/>
+      <c r="Q863" s="3"/>
+      <c r="R863" s="2"/>
+      <c r="S863" s="2"/>
+      <c r="T863" s="2"/>
+      <c r="U863" s="2"/>
+      <c r="V863" s="2"/>
+      <c r="W863" s="2"/>
+      <c r="X863" s="2"/>
+      <c r="Y863" s="2"/>
+      <c r="Z863" s="2"/>
+    </row>
+    <row r="864" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A864" s="11"/>
+      <c r="B864" s="2"/>
+      <c r="C864" s="2"/>
+      <c r="D864" s="2"/>
+      <c r="E864" s="2"/>
+      <c r="F864" s="2"/>
+      <c r="G864" s="2"/>
+      <c r="H864" s="2"/>
+      <c r="I864" s="2"/>
+      <c r="J864" s="2"/>
+      <c r="K864" s="2"/>
+      <c r="L864" s="2"/>
+      <c r="M864" s="2"/>
+      <c r="N864" s="2"/>
+      <c r="O864" s="2"/>
+      <c r="P864" s="3"/>
+      <c r="Q864" s="3"/>
+      <c r="R864" s="2"/>
+      <c r="S864" s="2"/>
+      <c r="T864" s="2"/>
+      <c r="U864" s="2"/>
+      <c r="V864" s="2"/>
+      <c r="W864" s="2"/>
+      <c r="X864" s="2"/>
+      <c r="Y864" s="2"/>
+      <c r="Z864" s="2"/>
+    </row>
+    <row r="865" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A865" s="11"/>
+      <c r="B865" s="2"/>
+      <c r="C865" s="2"/>
+      <c r="D865" s="2"/>
+      <c r="E865" s="2"/>
+      <c r="F865" s="2"/>
+      <c r="G865" s="2"/>
+      <c r="H865" s="2"/>
+      <c r="I865" s="2"/>
+      <c r="J865" s="2"/>
+      <c r="K865" s="2"/>
+      <c r="L865" s="2"/>
+      <c r="M865" s="2"/>
+      <c r="N865" s="2"/>
+      <c r="O865" s="2"/>
+      <c r="P865" s="3"/>
+      <c r="Q865" s="3"/>
+      <c r="R865" s="2"/>
+      <c r="S865" s="2"/>
+      <c r="T865" s="2"/>
+      <c r="U865" s="2"/>
+      <c r="V865" s="2"/>
+      <c r="W865" s="2"/>
+      <c r="X865" s="2"/>
+      <c r="Y865" s="2"/>
+      <c r="Z865" s="2"/>
+    </row>
+    <row r="866" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A866" s="11"/>
+      <c r="B866" s="2"/>
+      <c r="C866" s="2"/>
+      <c r="D866" s="2"/>
+      <c r="E866" s="2"/>
+      <c r="F866" s="2"/>
+      <c r="G866" s="2"/>
+      <c r="H866" s="2"/>
+      <c r="I866" s="2"/>
+      <c r="J866" s="2"/>
+      <c r="K866" s="2"/>
+      <c r="L866" s="2"/>
+      <c r="M866" s="2"/>
+      <c r="N866" s="2"/>
+      <c r="O866" s="2"/>
+      <c r="P866" s="3"/>
+      <c r="Q866" s="3"/>
+      <c r="R866" s="2"/>
+      <c r="S866" s="2"/>
+      <c r="T866" s="2"/>
+      <c r="U866" s="2"/>
+      <c r="V866" s="2"/>
+      <c r="W866" s="2"/>
+      <c r="X866" s="2"/>
+      <c r="Y866" s="2"/>
+      <c r="Z866" s="2"/>
+    </row>
+    <row r="867" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A867" s="11"/>
+      <c r="B867" s="2"/>
+      <c r="C867" s="2"/>
+      <c r="D867" s="2"/>
+      <c r="E867" s="2"/>
+      <c r="F867" s="2"/>
+      <c r="G867" s="2"/>
+      <c r="H867" s="2"/>
+      <c r="I867" s="2"/>
+      <c r="J867" s="2"/>
+      <c r="K867" s="2"/>
+      <c r="L867" s="2"/>
+      <c r="M867" s="2"/>
+      <c r="N867" s="2"/>
+      <c r="O867" s="2"/>
+      <c r="P867" s="3"/>
+      <c r="Q867" s="3"/>
+      <c r="R867" s="2"/>
+      <c r="S867" s="2"/>
+      <c r="T867" s="2"/>
+      <c r="U867" s="2"/>
+      <c r="V867" s="2"/>
+      <c r="W867" s="2"/>
+      <c r="X867" s="2"/>
+      <c r="Y867" s="2"/>
+      <c r="Z867" s="2"/>
+    </row>
+    <row r="868" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A868" s="11"/>
+      <c r="B868" s="2"/>
+      <c r="C868" s="2"/>
+      <c r="D868" s="2"/>
+      <c r="E868" s="2"/>
+      <c r="F868" s="2"/>
+      <c r="G868" s="2"/>
+      <c r="H868" s="2"/>
+      <c r="I868" s="2"/>
+      <c r="J868" s="2"/>
+      <c r="K868" s="2"/>
+      <c r="L868" s="2"/>
+      <c r="M868" s="2"/>
+      <c r="N868" s="2"/>
+      <c r="O868" s="2"/>
+      <c r="P868" s="3"/>
+      <c r="Q868" s="3"/>
+      <c r="R868" s="2"/>
+      <c r="S868" s="2"/>
+      <c r="T868" s="2"/>
+      <c r="U868" s="2"/>
+      <c r="V868" s="2"/>
+      <c r="W868" s="2"/>
+      <c r="X868" s="2"/>
+      <c r="Y868" s="2"/>
+      <c r="Z868" s="2"/>
+    </row>
+    <row r="869" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A869" s="11"/>
+      <c r="B869" s="2"/>
+      <c r="C869" s="2"/>
+      <c r="D869" s="2"/>
+      <c r="E869" s="2"/>
+      <c r="F869" s="2"/>
+      <c r="G869" s="2"/>
+      <c r="H869" s="2"/>
+      <c r="I869" s="2"/>
+      <c r="J869" s="2"/>
+      <c r="K869" s="2"/>
+      <c r="L869" s="2"/>
+      <c r="M869" s="2"/>
+      <c r="N869" s="2"/>
+      <c r="O869" s="2"/>
+      <c r="P869" s="3"/>
+      <c r="Q869" s="3"/>
+      <c r="R869" s="2"/>
+      <c r="S869" s="2"/>
+      <c r="T869" s="2"/>
+      <c r="U869" s="2"/>
+      <c r="V869" s="2"/>
+      <c r="W869" s="2"/>
+      <c r="X869" s="2"/>
+      <c r="Y869" s="2"/>
+      <c r="Z869" s="2"/>
+    </row>
+    <row r="870" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A870" s="11"/>
+      <c r="B870" s="2"/>
+      <c r="C870" s="2"/>
+      <c r="D870" s="2"/>
+      <c r="E870" s="2"/>
+      <c r="F870" s="2"/>
+      <c r="G870" s="2"/>
+      <c r="H870" s="2"/>
+      <c r="I870" s="2"/>
+      <c r="J870" s="2"/>
+      <c r="K870" s="2"/>
+      <c r="L870" s="2"/>
+      <c r="M870" s="2"/>
+      <c r="N870" s="2"/>
+      <c r="O870" s="2"/>
+      <c r="P870" s="3"/>
+      <c r="Q870" s="3"/>
+      <c r="R870" s="2"/>
+      <c r="S870" s="2"/>
+      <c r="T870" s="2"/>
+      <c r="U870" s="2"/>
+      <c r="V870" s="2"/>
+      <c r="W870" s="2"/>
+      <c r="X870" s="2"/>
+      <c r="Y870" s="2"/>
+      <c r="Z870" s="2"/>
+    </row>
+    <row r="871" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A871" s="11"/>
+      <c r="B871" s="2"/>
+      <c r="C871" s="2"/>
+      <c r="D871" s="2"/>
+      <c r="E871" s="2"/>
+      <c r="F871" s="2"/>
+      <c r="G871" s="2"/>
+      <c r="H871" s="2"/>
+      <c r="I871" s="2"/>
+      <c r="J871" s="2"/>
+      <c r="K871" s="2"/>
+      <c r="L871" s="2"/>
+      <c r="M871" s="2"/>
+      <c r="N871" s="2"/>
+      <c r="O871" s="2"/>
+      <c r="P871" s="3"/>
+      <c r="Q871" s="3"/>
+      <c r="R871" s="2"/>
+      <c r="S871" s="2"/>
+      <c r="T871" s="2"/>
+      <c r="U871" s="2"/>
+      <c r="V871" s="2"/>
+      <c r="W871" s="2"/>
+      <c r="X871" s="2"/>
+      <c r="Y871" s="2"/>
+      <c r="Z871" s="2"/>
+    </row>
+    <row r="872" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A872" s="11"/>
+      <c r="B872" s="2"/>
+      <c r="C872" s="2"/>
+      <c r="D872" s="2"/>
+      <c r="E872" s="2"/>
+      <c r="F872" s="2"/>
+      <c r="G872" s="2"/>
+      <c r="H872" s="2"/>
+      <c r="I872" s="2"/>
+      <c r="J872" s="2"/>
+      <c r="K872" s="2"/>
+      <c r="L872" s="2"/>
+      <c r="M872" s="2"/>
+      <c r="N872" s="2"/>
+      <c r="O872" s="2"/>
+      <c r="P872" s="3"/>
+      <c r="Q872" s="3"/>
+      <c r="R872" s="2"/>
+      <c r="S872" s="2"/>
+      <c r="T872" s="2"/>
+      <c r="U872" s="2"/>
+      <c r="V872" s="2"/>
+      <c r="W872" s="2"/>
+      <c r="X872" s="2"/>
+      <c r="Y872" s="2"/>
+      <c r="Z872" s="2"/>
+    </row>
+    <row r="873" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A873" s="11"/>
+      <c r="B873" s="2"/>
+      <c r="C873" s="2"/>
+      <c r="D873" s="2"/>
+      <c r="E873" s="2"/>
+      <c r="F873" s="2"/>
+      <c r="G873" s="2"/>
+      <c r="H873" s="2"/>
+      <c r="I873" s="2"/>
+      <c r="J873" s="2"/>
+      <c r="K873" s="2"/>
+      <c r="L873" s="2"/>
+      <c r="M873" s="2"/>
+      <c r="N873" s="2"/>
+      <c r="O873" s="2"/>
+      <c r="P873" s="3"/>
+      <c r="Q873" s="3"/>
+      <c r="R873" s="2"/>
+      <c r="S873" s="2"/>
+      <c r="T873" s="2"/>
+      <c r="U873" s="2"/>
+      <c r="V873" s="2"/>
+      <c r="W873" s="2"/>
+      <c r="X873" s="2"/>
+      <c r="Y873" s="2"/>
+      <c r="Z873" s="2"/>
+    </row>
+    <row r="874" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A874" s="11"/>
+      <c r="B874" s="2"/>
+      <c r="C874" s="2"/>
+      <c r="D874" s="2"/>
+      <c r="E874" s="2"/>
+      <c r="F874" s="2"/>
+      <c r="G874" s="2"/>
+      <c r="H874" s="2"/>
+      <c r="I874" s="2"/>
+      <c r="J874" s="2"/>
+      <c r="K874" s="2"/>
+      <c r="L874" s="2"/>
+      <c r="M874" s="2"/>
+      <c r="N874" s="2"/>
+      <c r="O874" s="2"/>
+      <c r="P874" s="3"/>
+      <c r="Q874" s="3"/>
+      <c r="R874" s="2"/>
+      <c r="S874" s="2"/>
+      <c r="T874" s="2"/>
+      <c r="U874" s="2"/>
+      <c r="V874" s="2"/>
+      <c r="W874" s="2"/>
+      <c r="X874" s="2"/>
+      <c r="Y874" s="2"/>
+      <c r="Z874" s="2"/>
+    </row>
+    <row r="875" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A875" s="11"/>
+      <c r="B875" s="2"/>
+      <c r="C875" s="2"/>
+      <c r="D875" s="2"/>
+      <c r="E875" s="2"/>
+      <c r="F875" s="2"/>
+      <c r="G875" s="2"/>
+      <c r="H875" s="2"/>
+      <c r="I875" s="2"/>
+      <c r="J875" s="2"/>
+      <c r="K875" s="2"/>
+      <c r="L875" s="2"/>
+      <c r="M875" s="2"/>
+      <c r="N875" s="2"/>
+      <c r="O875" s="2"/>
+      <c r="P875" s="3"/>
+      <c r="Q875" s="3"/>
+      <c r="R875" s="2"/>
+      <c r="S875" s="2"/>
+      <c r="T875" s="2"/>
+      <c r="U875" s="2"/>
+      <c r="V875" s="2"/>
+      <c r="W875" s="2"/>
+      <c r="X875" s="2"/>
+      <c r="Y875" s="2"/>
+      <c r="Z875" s="2"/>
+    </row>
+    <row r="876" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A876" s="11"/>
+      <c r="B876" s="2"/>
+      <c r="C876" s="2"/>
+      <c r="D876" s="2"/>
+      <c r="E876" s="2"/>
+      <c r="F876" s="2"/>
+      <c r="G876" s="2"/>
+      <c r="H876" s="2"/>
+      <c r="I876" s="2"/>
+      <c r="J876" s="2"/>
+      <c r="K876" s="2"/>
+      <c r="L876" s="2"/>
+      <c r="M876" s="2"/>
+      <c r="N876" s="2"/>
+      <c r="O876" s="2"/>
+      <c r="P876" s="3"/>
+      <c r="Q876" s="3"/>
+      <c r="R876" s="2"/>
+      <c r="S876" s="2"/>
+      <c r="T876" s="2"/>
+      <c r="U876" s="2"/>
+      <c r="V876" s="2"/>
+      <c r="W876" s="2"/>
+      <c r="X876" s="2"/>
+      <c r="Y876" s="2"/>
+      <c r="Z876" s="2"/>
+    </row>
+    <row r="877" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A877" s="11"/>
+      <c r="B877" s="2"/>
+      <c r="C877" s="2"/>
+      <c r="D877" s="2"/>
+      <c r="E877" s="2"/>
+      <c r="F877" s="2"/>
+      <c r="G877" s="2"/>
+      <c r="H877" s="2"/>
+      <c r="I877" s="2"/>
+      <c r="J877" s="2"/>
+      <c r="K877" s="2"/>
+      <c r="L877" s="2"/>
+      <c r="M877" s="2"/>
+      <c r="N877" s="2"/>
+      <c r="O877" s="2"/>
+      <c r="P877" s="3"/>
+      <c r="Q877" s="3"/>
+      <c r="R877" s="2"/>
+      <c r="S877" s="2"/>
+      <c r="T877" s="2"/>
+      <c r="U877" s="2"/>
+      <c r="V877" s="2"/>
+      <c r="W877" s="2"/>
+      <c r="X877" s="2"/>
+      <c r="Y877" s="2"/>
+      <c r="Z877" s="2"/>
+    </row>
+    <row r="878" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A878" s="11"/>
+      <c r="B878" s="2"/>
+      <c r="C878" s="2"/>
+      <c r="D878" s="2"/>
+      <c r="E878" s="2"/>
+      <c r="F878" s="2"/>
+      <c r="G878" s="2"/>
+      <c r="H878" s="2"/>
+      <c r="I878" s="2"/>
+      <c r="J878" s="2"/>
+      <c r="K878" s="2"/>
+      <c r="L878" s="2"/>
+      <c r="M878" s="2"/>
+      <c r="N878" s="2"/>
+      <c r="O878" s="2"/>
+      <c r="P878" s="3"/>
+      <c r="Q878" s="3"/>
+      <c r="R878" s="2"/>
+      <c r="S878" s="2"/>
+      <c r="T878" s="2"/>
+      <c r="U878" s="2"/>
+      <c r="V878" s="2"/>
+      <c r="W878" s="2"/>
+      <c r="X878" s="2"/>
+      <c r="Y878" s="2"/>
+      <c r="Z878" s="2"/>
+    </row>
+    <row r="879" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A879" s="11"/>
+      <c r="B879" s="2"/>
+      <c r="C879" s="2"/>
+      <c r="D879" s="2"/>
+      <c r="E879" s="2"/>
+      <c r="F879" s="2"/>
+      <c r="G879" s="2"/>
+      <c r="H879" s="2"/>
+      <c r="I879" s="2"/>
+      <c r="J879" s="2"/>
+      <c r="K879" s="2"/>
+      <c r="L879" s="2"/>
+      <c r="M879" s="2"/>
+      <c r="N879" s="2"/>
+      <c r="O879" s="2"/>
+      <c r="P879" s="3"/>
+      <c r="Q879" s="3"/>
+      <c r="R879" s="2"/>
+      <c r="S879" s="2"/>
+      <c r="T879" s="2"/>
+      <c r="U879" s="2"/>
+      <c r="V879" s="2"/>
+      <c r="W879" s="2"/>
+      <c r="X879" s="2"/>
+      <c r="Y879" s="2"/>
+      <c r="Z879" s="2"/>
+    </row>
+    <row r="880" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A880" s="11"/>
+      <c r="B880" s="2"/>
+      <c r="C880" s="2"/>
+      <c r="D880" s="2"/>
+      <c r="E880" s="2"/>
+      <c r="F880" s="2"/>
+      <c r="G880" s="2"/>
+      <c r="H880" s="2"/>
+      <c r="I880" s="2"/>
+      <c r="J880" s="2"/>
+      <c r="K880" s="2"/>
+      <c r="L880" s="2"/>
+      <c r="M880" s="2"/>
+      <c r="N880" s="2"/>
+      <c r="O880" s="2"/>
+      <c r="P880" s="3"/>
+      <c r="Q880" s="3"/>
+      <c r="R880" s="2"/>
+      <c r="S880" s="2"/>
+      <c r="T880" s="2"/>
+      <c r="U880" s="2"/>
+      <c r="V880" s="2"/>
+      <c r="W880" s="2"/>
+      <c r="X880" s="2"/>
+      <c r="Y880" s="2"/>
+      <c r="Z880" s="2"/>
+    </row>
+    <row r="881" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A881" s="11"/>
+      <c r="B881" s="2"/>
+      <c r="C881" s="2"/>
+      <c r="D881" s="2"/>
+      <c r="E881" s="2"/>
+      <c r="F881" s="2"/>
+      <c r="G881" s="2"/>
+      <c r="H881" s="2"/>
+      <c r="I881" s="2"/>
+      <c r="J881" s="2"/>
+      <c r="K881" s="2"/>
+      <c r="L881" s="2"/>
+      <c r="M881" s="2"/>
+      <c r="N881" s="2"/>
+      <c r="O881" s="2"/>
+      <c r="P881" s="3"/>
+      <c r="Q881" s="3"/>
+      <c r="R881" s="2"/>
+      <c r="S881" s="2"/>
+      <c r="T881" s="2"/>
+      <c r="U881" s="2"/>
+      <c r="V881" s="2"/>
+      <c r="W881" s="2"/>
+      <c r="X881" s="2"/>
+      <c r="Y881" s="2"/>
+      <c r="Z881" s="2"/>
+    </row>
+    <row r="882" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A882" s="11"/>
+      <c r="B882" s="2"/>
+      <c r="C882" s="2"/>
+      <c r="D882" s="2"/>
+      <c r="E882" s="2"/>
+      <c r="F882" s="2"/>
+      <c r="G882" s="2"/>
+      <c r="H882" s="2"/>
+      <c r="I882" s="2"/>
+      <c r="J882" s="2"/>
+      <c r="K882" s="2"/>
+      <c r="L882" s="2"/>
+      <c r="M882" s="2"/>
+      <c r="N882" s="2"/>
+      <c r="O882" s="2"/>
+      <c r="P882" s="3"/>
+      <c r="Q882" s="3"/>
+      <c r="R882" s="2"/>
+      <c r="S882" s="2"/>
+      <c r="T882" s="2"/>
+      <c r="U882" s="2"/>
+      <c r="V882" s="2"/>
+      <c r="W882" s="2"/>
+      <c r="X882" s="2"/>
+      <c r="Y882" s="2"/>
+      <c r="Z882" s="2"/>
+    </row>
+    <row r="883" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A883" s="11"/>
+      <c r="B883" s="2"/>
+      <c r="C883" s="2"/>
+      <c r="D883" s="2"/>
+      <c r="E883" s="2"/>
+      <c r="F883" s="2"/>
+      <c r="G883" s="2"/>
+      <c r="H883" s="2"/>
+      <c r="I883" s="2"/>
+      <c r="J883" s="2"/>
+      <c r="K883" s="2"/>
+      <c r="L883" s="2"/>
+      <c r="M883" s="2"/>
+      <c r="N883" s="2"/>
+      <c r="O883" s="2"/>
+      <c r="P883" s="3"/>
+      <c r="Q883" s="3"/>
+      <c r="R883" s="2"/>
+      <c r="S883" s="2"/>
+      <c r="T883" s="2"/>
+      <c r="U883" s="2"/>
+      <c r="V883" s="2"/>
+      <c r="W883" s="2"/>
+      <c r="X883" s="2"/>
+      <c r="Y883" s="2"/>
+      <c r="Z883" s="2"/>
+    </row>
+    <row r="884" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A884" s="11"/>
+      <c r="B884" s="2"/>
+      <c r="C884" s="2"/>
+      <c r="D884" s="2"/>
+      <c r="E884" s="2"/>
+      <c r="F884" s="2"/>
+      <c r="G884" s="2"/>
+      <c r="H884" s="2"/>
+      <c r="I884" s="2"/>
+      <c r="J884" s="2"/>
+      <c r="K884" s="2"/>
+      <c r="L884" s="2"/>
+      <c r="M884" s="2"/>
+      <c r="N884" s="2"/>
+      <c r="O884" s="2"/>
+      <c r="P884" s="3"/>
+      <c r="Q884" s="3"/>
+      <c r="R884" s="2"/>
+      <c r="S884" s="2"/>
+      <c r="T884" s="2"/>
+      <c r="U884" s="2"/>
+      <c r="V884" s="2"/>
+      <c r="W884" s="2"/>
+      <c r="X884" s="2"/>
+      <c r="Y884" s="2"/>
+      <c r="Z884" s="2"/>
+    </row>
+    <row r="885" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A885" s="11"/>
+      <c r="B885" s="2"/>
+      <c r="C885" s="2"/>
+      <c r="D885" s="2"/>
+      <c r="E885" s="2"/>
+      <c r="F885" s="2"/>
+      <c r="G885" s="2"/>
+      <c r="H885" s="2"/>
+      <c r="I885" s="2"/>
+      <c r="J885" s="2"/>
+      <c r="K885" s="2"/>
+      <c r="L885" s="2"/>
+      <c r="M885" s="2"/>
+      <c r="N885" s="2"/>
+      <c r="O885" s="2"/>
+      <c r="P885" s="3"/>
+      <c r="Q885" s="3"/>
+      <c r="R885" s="2"/>
+      <c r="S885" s="2"/>
+      <c r="T885" s="2"/>
+      <c r="U885" s="2"/>
+      <c r="V885" s="2"/>
+      <c r="W885" s="2"/>
+      <c r="X885" s="2"/>
+      <c r="Y885" s="2"/>
+      <c r="Z885" s="2"/>
+    </row>
+    <row r="886" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A886" s="11"/>
+      <c r="B886" s="2"/>
+      <c r="C886" s="2"/>
+      <c r="D886" s="2"/>
+      <c r="E886" s="2"/>
+      <c r="F886" s="2"/>
+      <c r="G886" s="2"/>
+      <c r="H886" s="2"/>
+      <c r="I886" s="2"/>
+      <c r="J886" s="2"/>
+      <c r="K886" s="2"/>
+      <c r="L886" s="2"/>
+      <c r="M886" s="2"/>
+      <c r="N886" s="2"/>
+      <c r="O886" s="2"/>
+      <c r="P886" s="3"/>
+      <c r="Q886" s="3"/>
+      <c r="R886" s="2"/>
+      <c r="S886" s="2"/>
+      <c r="T886" s="2"/>
+      <c r="U886" s="2"/>
+      <c r="V886" s="2"/>
+      <c r="W886" s="2"/>
+      <c r="X886" s="2"/>
+      <c r="Y886" s="2"/>
+      <c r="Z886" s="2"/>
+    </row>
+    <row r="887" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A887" s="11"/>
+      <c r="B887" s="2"/>
+      <c r="C887" s="2"/>
+      <c r="D887" s="2"/>
+      <c r="E887" s="2"/>
+      <c r="F887" s="2"/>
+      <c r="G887" s="2"/>
+      <c r="H887" s="2"/>
+      <c r="I887" s="2"/>
+      <c r="J887" s="2"/>
+      <c r="K887" s="2"/>
+      <c r="L887" s="2"/>
+      <c r="M887" s="2"/>
+      <c r="N887" s="2"/>
+      <c r="O887" s="2"/>
+      <c r="P887" s="3"/>
+      <c r="Q887" s="3"/>
+      <c r="R887" s="2"/>
+      <c r="S887" s="2"/>
+      <c r="T887" s="2"/>
+      <c r="U887" s="2"/>
+      <c r="V887" s="2"/>
+      <c r="W887" s="2"/>
+      <c r="X887" s="2"/>
+      <c r="Y887" s="2"/>
+      <c r="Z887" s="2"/>
+    </row>
+    <row r="888" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A888" s="11"/>
+      <c r="B888" s="2"/>
+      <c r="C888" s="2"/>
+      <c r="D888" s="2"/>
+      <c r="E888" s="2"/>
+      <c r="F888" s="2"/>
+      <c r="G888" s="2"/>
+      <c r="H888" s="2"/>
+      <c r="I888" s="2"/>
+      <c r="J888" s="2"/>
+      <c r="K888" s="2"/>
+      <c r="L888" s="2"/>
+      <c r="M888" s="2"/>
+      <c r="N888" s="2"/>
+      <c r="O888" s="2"/>
+      <c r="P888" s="3"/>
+      <c r="Q888" s="3"/>
+      <c r="R888" s="2"/>
+      <c r="S888" s="2"/>
+      <c r="T888" s="2"/>
+      <c r="U888" s="2"/>
+      <c r="V888" s="2"/>
+      <c r="W888" s="2"/>
+      <c r="X888" s="2"/>
+      <c r="Y888" s="2"/>
+      <c r="Z888" s="2"/>
+    </row>
+    <row r="889" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A889" s="11"/>
+      <c r="B889" s="2"/>
+      <c r="C889" s="2"/>
+      <c r="D889" s="2"/>
+      <c r="E889" s="2"/>
+      <c r="F889" s="2"/>
+      <c r="G889" s="2"/>
+      <c r="H889" s="2"/>
+      <c r="I889" s="2"/>
+      <c r="J889" s="2"/>
+      <c r="K889" s="2"/>
+      <c r="L889" s="2"/>
+      <c r="M889" s="2"/>
+      <c r="N889" s="2"/>
+      <c r="O889" s="2"/>
+      <c r="P889" s="3"/>
+      <c r="Q889" s="3"/>
+      <c r="R889" s="2"/>
+      <c r="S889" s="2"/>
+      <c r="T889" s="2"/>
+      <c r="U889" s="2"/>
+      <c r="V889" s="2"/>
+      <c r="W889" s="2"/>
+      <c r="X889" s="2"/>
+      <c r="Y889" s="2"/>
+      <c r="Z889" s="2"/>
+    </row>
+    <row r="890" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A890" s="11"/>
+      <c r="B890" s="2"/>
+      <c r="C890" s="2"/>
+      <c r="D890" s="2"/>
+      <c r="E890" s="2"/>
+      <c r="F890" s="2"/>
+      <c r="G890" s="2"/>
+      <c r="H890" s="2"/>
+      <c r="I890" s="2"/>
+      <c r="J890" s="2"/>
+      <c r="K890" s="2"/>
+      <c r="L890" s="2"/>
+      <c r="M890" s="2"/>
+      <c r="N890" s="2"/>
+      <c r="O890" s="2"/>
+      <c r="P890" s="3"/>
+      <c r="Q890" s="3"/>
+      <c r="R890" s="2"/>
+      <c r="S890" s="2"/>
+      <c r="T890" s="2"/>
+      <c r="U890" s="2"/>
+      <c r="V890" s="2"/>
+      <c r="W890" s="2"/>
+      <c r="X890" s="2"/>
+      <c r="Y890" s="2"/>
+      <c r="Z890" s="2"/>
+    </row>
+    <row r="891" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A891" s="11"/>
+      <c r="B891" s="2"/>
+      <c r="C891" s="2"/>
+      <c r="D891" s="2"/>
+      <c r="E891" s="2"/>
+      <c r="F891" s="2"/>
+      <c r="G891" s="2"/>
+      <c r="H891" s="2"/>
+      <c r="I891" s="2"/>
+      <c r="J891" s="2"/>
+      <c r="K891" s="2"/>
+      <c r="L891" s="2"/>
+      <c r="M891" s="2"/>
+      <c r="N891" s="2"/>
+      <c r="O891" s="2"/>
+      <c r="P891" s="3"/>
+      <c r="Q891" s="3"/>
+      <c r="R891" s="2"/>
+      <c r="S891" s="2"/>
+      <c r="T891" s="2"/>
+      <c r="U891" s="2"/>
+      <c r="V891" s="2"/>
+      <c r="W891" s="2"/>
+      <c r="X891" s="2"/>
+      <c r="Y891" s="2"/>
+      <c r="Z891" s="2"/>
+    </row>
+    <row r="892" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A892" s="11"/>
+      <c r="B892" s="2"/>
+      <c r="C892" s="2"/>
+      <c r="D892" s="2"/>
+      <c r="E892" s="2"/>
+      <c r="F892" s="2"/>
+      <c r="G892" s="2"/>
+      <c r="H892" s="2"/>
+      <c r="I892" s="2"/>
+      <c r="J892" s="2"/>
+      <c r="K892" s="2"/>
+      <c r="L892" s="2"/>
+      <c r="M892" s="2"/>
+      <c r="N892" s="2"/>
+      <c r="O892" s="2"/>
+      <c r="P892" s="3"/>
+      <c r="Q892" s="3"/>
+      <c r="R892" s="2"/>
+      <c r="S892" s="2"/>
+      <c r="T892" s="2"/>
+      <c r="U892" s="2"/>
+      <c r="V892" s="2"/>
+      <c r="W892" s="2"/>
+      <c r="X892" s="2"/>
+      <c r="Y892" s="2"/>
+      <c r="Z892" s="2"/>
+    </row>
+    <row r="893" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A893" s="11"/>
+      <c r="B893" s="2"/>
+      <c r="C893" s="2"/>
+      <c r="D893" s="2"/>
+      <c r="E893" s="2"/>
+      <c r="F893" s="2"/>
+      <c r="G893" s="2"/>
+      <c r="H893" s="2"/>
+      <c r="I893" s="2"/>
+      <c r="J893" s="2"/>
+      <c r="K893" s="2"/>
+      <c r="L893" s="2"/>
+      <c r="M893" s="2"/>
+      <c r="N893" s="2"/>
+      <c r="O893" s="2"/>
+      <c r="P893" s="3"/>
+      <c r="Q893" s="3"/>
+      <c r="R893" s="2"/>
+      <c r="S893" s="2"/>
+      <c r="T893" s="2"/>
+      <c r="U893" s="2"/>
+      <c r="V893" s="2"/>
+      <c r="W893" s="2"/>
+      <c r="X893" s="2"/>
+      <c r="Y893" s="2"/>
+      <c r="Z893" s="2"/>
+    </row>
+    <row r="894" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A894" s="11"/>
+      <c r="B894" s="2"/>
+      <c r="C894" s="2"/>
+      <c r="D894" s="2"/>
+      <c r="E894" s="2"/>
+      <c r="F894" s="2"/>
+      <c r="G894" s="2"/>
+      <c r="H894" s="2"/>
+      <c r="I894" s="2"/>
+      <c r="J894" s="2"/>
+      <c r="K894" s="2"/>
+      <c r="L894" s="2"/>
+      <c r="M894" s="2"/>
+      <c r="N894" s="2"/>
+      <c r="O894" s="2"/>
+      <c r="P894" s="3"/>
+      <c r="Q894" s="3"/>
+      <c r="R894" s="2"/>
+      <c r="S894" s="2"/>
+      <c r="T894" s="2"/>
+      <c r="U894" s="2"/>
+      <c r="V894" s="2"/>
+      <c r="W894" s="2"/>
+      <c r="X894" s="2"/>
+      <c r="Y894" s="2"/>
+      <c r="Z894" s="2"/>
+    </row>
+    <row r="895" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A895" s="11"/>
+      <c r="B895" s="2"/>
+      <c r="C895" s="2"/>
+      <c r="D895" s="2"/>
+      <c r="E895" s="2"/>
+      <c r="F895" s="2"/>
+      <c r="G895" s="2"/>
+      <c r="H895" s="2"/>
+      <c r="I895" s="2"/>
+      <c r="J895" s="2"/>
+      <c r="K895" s="2"/>
+      <c r="L895" s="2"/>
+      <c r="M895" s="2"/>
+      <c r="N895" s="2"/>
+      <c r="O895" s="2"/>
+      <c r="P895" s="3"/>
+      <c r="Q895" s="3"/>
+      <c r="R895" s="2"/>
+      <c r="S895" s="2"/>
+      <c r="T895" s="2"/>
+      <c r="U895" s="2"/>
+      <c r="V895" s="2"/>
+      <c r="W895" s="2"/>
+      <c r="X895" s="2"/>
+      <c r="Y895" s="2"/>
+      <c r="Z895" s="2"/>
+    </row>
+    <row r="896" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A896" s="11"/>
+      <c r="B896" s="2"/>
+      <c r="C896" s="2"/>
+      <c r="D896" s="2"/>
+      <c r="E896" s="2"/>
+      <c r="F896" s="2"/>
+      <c r="G896" s="2"/>
+      <c r="H896" s="2"/>
+      <c r="I896" s="2"/>
+      <c r="J896" s="2"/>
+      <c r="K896" s="2"/>
+      <c r="L896" s="2"/>
+      <c r="M896" s="2"/>
+      <c r="N896" s="2"/>
+      <c r="O896" s="2"/>
+      <c r="P896" s="3"/>
+      <c r="Q896" s="3"/>
+      <c r="R896" s="2"/>
+      <c r="S896" s="2"/>
+      <c r="T896" s="2"/>
+      <c r="U896" s="2"/>
+      <c r="V896" s="2"/>
+      <c r="W896" s="2"/>
+      <c r="X896" s="2"/>
+      <c r="Y896" s="2"/>
+      <c r="Z896" s="2"/>
+    </row>
+    <row r="897" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A897" s="11"/>
+      <c r="B897" s="2"/>
+      <c r="C897" s="2"/>
+      <c r="D897" s="2"/>
+      <c r="E897" s="2"/>
+      <c r="F897" s="2"/>
+      <c r="G897" s="2"/>
+      <c r="H897" s="2"/>
+      <c r="I897" s="2"/>
+      <c r="J897" s="2"/>
+      <c r="K897" s="2"/>
+      <c r="L897" s="2"/>
+      <c r="M897" s="2"/>
+      <c r="N897" s="2"/>
+      <c r="O897" s="2"/>
+      <c r="P897" s="3"/>
+      <c r="Q897" s="3"/>
+      <c r="R897" s="2"/>
+      <c r="S897" s="2"/>
+      <c r="T897" s="2"/>
+      <c r="U897" s="2"/>
+      <c r="V897" s="2"/>
+      <c r="W897" s="2"/>
+      <c r="X897" s="2"/>
+      <c r="Y897" s="2"/>
+      <c r="Z897" s="2"/>
+    </row>
+    <row r="898" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A898" s="11"/>
+      <c r="B898" s="2"/>
+      <c r="C898" s="2"/>
+      <c r="D898" s="2"/>
+      <c r="E898" s="2"/>
+      <c r="F898" s="2"/>
+      <c r="G898" s="2"/>
+      <c r="H898" s="2"/>
+      <c r="I898" s="2"/>
+      <c r="J898" s="2"/>
+      <c r="K898" s="2"/>
+      <c r="L898" s="2"/>
+      <c r="M898" s="2"/>
+      <c r="N898" s="2"/>
+      <c r="O898" s="2"/>
+      <c r="P898" s="3"/>
+      <c r="Q898" s="3"/>
+      <c r="R898" s="2"/>
+      <c r="S898" s="2"/>
+      <c r="T898" s="2"/>
+      <c r="U898" s="2"/>
+      <c r="V898" s="2"/>
+      <c r="W898" s="2"/>
+      <c r="X898" s="2"/>
+      <c r="Y898" s="2"/>
+      <c r="Z898" s="2"/>
+    </row>
+    <row r="899" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A899" s="11"/>
+      <c r="B899" s="2"/>
+      <c r="C899" s="2"/>
+      <c r="D899" s="2"/>
+      <c r="E899" s="2"/>
+      <c r="F899" s="2"/>
+      <c r="G899" s="2"/>
+      <c r="H899" s="2"/>
+      <c r="I899" s="2"/>
+      <c r="J899" s="2"/>
+      <c r="K899" s="2"/>
+      <c r="L899" s="2"/>
+      <c r="M899" s="2"/>
+      <c r="N899" s="2"/>
+      <c r="O899" s="2"/>
+      <c r="P899" s="3"/>
+      <c r="Q899" s="3"/>
+      <c r="R899" s="2"/>
+      <c r="S899" s="2"/>
+      <c r="T899" s="2"/>
+      <c r="U899" s="2"/>
+      <c r="V899" s="2"/>
+      <c r="W899" s="2"/>
+      <c r="X899" s="2"/>
+      <c r="Y899" s="2"/>
+      <c r="Z899" s="2"/>
+    </row>
+    <row r="900" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A900" s="11"/>
+      <c r="B900" s="2"/>
+      <c r="C900" s="2"/>
+      <c r="D900" s="2"/>
+      <c r="E900" s="2"/>
+      <c r="F900" s="2"/>
+      <c r="G900" s="2"/>
+      <c r="H900" s="2"/>
+      <c r="I900" s="2"/>
+      <c r="J900" s="2"/>
+      <c r="K900" s="2"/>
+      <c r="L900" s="2"/>
+      <c r="M900" s="2"/>
+      <c r="N900" s="2"/>
+      <c r="O900" s="2"/>
+      <c r="P900" s="3"/>
+      <c r="Q900" s="3"/>
+      <c r="R900" s="2"/>
+      <c r="S900" s="2"/>
+      <c r="T900" s="2"/>
+      <c r="U900" s="2"/>
+      <c r="V900" s="2"/>
+      <c r="W900" s="2"/>
+      <c r="X900" s="2"/>
+      <c r="Y900" s="2"/>
+      <c r="Z900" s="2"/>
+    </row>
+    <row r="901" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A901" s="11"/>
+      <c r="B901" s="2"/>
+      <c r="C901" s="2"/>
+      <c r="D901" s="2"/>
+      <c r="E901" s="2"/>
+      <c r="F901" s="2"/>
+      <c r="G901" s="2"/>
+      <c r="H901" s="2"/>
+      <c r="I901" s="2"/>
+      <c r="J901" s="2"/>
+      <c r="K901" s="2"/>
+      <c r="L901" s="2"/>
+      <c r="M901" s="2"/>
+      <c r="N901" s="2"/>
+      <c r="O901" s="2"/>
+      <c r="P901" s="3"/>
+      <c r="Q901" s="3"/>
+      <c r="R901" s="2"/>
+      <c r="S901" s="2"/>
+      <c r="T901" s="2"/>
+      <c r="U901" s="2"/>
+      <c r="V901" s="2"/>
+      <c r="W901" s="2"/>
+      <c r="X901" s="2"/>
+      <c r="Y901" s="2"/>
+      <c r="Z901" s="2"/>
+    </row>
+    <row r="902" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A902" s="11"/>
+      <c r="B902" s="2"/>
+      <c r="C902" s="2"/>
+      <c r="D902" s="2"/>
+      <c r="E902" s="2"/>
+      <c r="F902" s="2"/>
+      <c r="G902" s="2"/>
+      <c r="H902" s="2"/>
+      <c r="I902" s="2"/>
+      <c r="J902" s="2"/>
+      <c r="K902" s="2"/>
+      <c r="L902" s="2"/>
+      <c r="M902" s="2"/>
+      <c r="N902" s="2"/>
+      <c r="O902" s="2"/>
+      <c r="P902" s="3"/>
+      <c r="Q902" s="3"/>
+      <c r="R902" s="2"/>
+      <c r="S902" s="2"/>
+      <c r="T902" s="2"/>
+      <c r="U902" s="2"/>
+      <c r="V902" s="2"/>
+      <c r="W902" s="2"/>
+      <c r="X902" s="2"/>
+      <c r="Y902" s="2"/>
+      <c r="Z902" s="2"/>
+    </row>
+    <row r="903" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A903" s="11"/>
+      <c r="B903" s="2"/>
+      <c r="C903" s="2"/>
+      <c r="D903" s="2"/>
+      <c r="E903" s="2"/>
+      <c r="F903" s="2"/>
+      <c r="G903" s="2"/>
+      <c r="H903" s="2"/>
+      <c r="I903" s="2"/>
+      <c r="J903" s="2"/>
+      <c r="K903" s="2"/>
+      <c r="L903" s="2"/>
+      <c r="M903" s="2"/>
+      <c r="N903" s="2"/>
+      <c r="O903" s="2"/>
+      <c r="P903" s="3"/>
+      <c r="Q903" s="3"/>
+      <c r="R903" s="2"/>
+      <c r="S903" s="2"/>
+      <c r="T903" s="2"/>
+      <c r="U903" s="2"/>
+      <c r="V903" s="2"/>
+      <c r="W903" s="2"/>
+      <c r="X903" s="2"/>
+      <c r="Y903" s="2"/>
+      <c r="Z903" s="2"/>
+    </row>
+    <row r="904" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A904" s="11"/>
+      <c r="B904" s="2"/>
+      <c r="C904" s="2"/>
+      <c r="D904" s="2"/>
+      <c r="E904" s="2"/>
+      <c r="F904" s="2"/>
+      <c r="G904" s="2"/>
+      <c r="H904" s="2"/>
+      <c r="I904" s="2"/>
+      <c r="J904" s="2"/>
+      <c r="K904" s="2"/>
+      <c r="L904" s="2"/>
+      <c r="M904" s="2"/>
+      <c r="N904" s="2"/>
+      <c r="O904" s="2"/>
+      <c r="P904" s="3"/>
+      <c r="Q904" s="3"/>
+      <c r="R904" s="2"/>
+      <c r="S904" s="2"/>
+      <c r="T904" s="2"/>
+      <c r="U904" s="2"/>
+      <c r="V904" s="2"/>
+      <c r="W904" s="2"/>
+      <c r="X904" s="2"/>
+      <c r="Y904" s="2"/>
+      <c r="Z904" s="2"/>
+    </row>
+    <row r="905" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A905" s="11"/>
+      <c r="B905" s="2"/>
+      <c r="C905" s="2"/>
+      <c r="D905" s="2"/>
+      <c r="E905" s="2"/>
+      <c r="F905" s="2"/>
+      <c r="G905" s="2"/>
+      <c r="H905" s="2"/>
+      <c r="I905" s="2"/>
+      <c r="J905" s="2"/>
+      <c r="K905" s="2"/>
+      <c r="L905" s="2"/>
+      <c r="M905" s="2"/>
+      <c r="N905" s="2"/>
+      <c r="O905" s="2"/>
+      <c r="P905" s="3"/>
+      <c r="Q905" s="3"/>
+      <c r="R905" s="2"/>
+      <c r="S905" s="2"/>
+      <c r="T905" s="2"/>
+      <c r="U905" s="2"/>
+      <c r="V905" s="2"/>
+      <c r="W905" s="2"/>
+      <c r="X905" s="2"/>
+      <c r="Y905" s="2"/>
+      <c r="Z905" s="2"/>
+    </row>
+    <row r="906" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A906" s="11"/>
+      <c r="B906" s="2"/>
+      <c r="C906" s="2"/>
+      <c r="D906" s="2"/>
+      <c r="E906" s="2"/>
+      <c r="F906" s="2"/>
+      <c r="G906" s="2"/>
+      <c r="H906" s="2"/>
+      <c r="I906" s="2"/>
+      <c r="J906" s="2"/>
+      <c r="K906" s="2"/>
+      <c r="L906" s="2"/>
+      <c r="M906" s="2"/>
+      <c r="N906" s="2"/>
+      <c r="O906" s="2"/>
+      <c r="P906" s="3"/>
+      <c r="Q906" s="3"/>
+      <c r="R906" s="2"/>
+      <c r="S906" s="2"/>
+      <c r="T906" s="2"/>
+      <c r="U906" s="2"/>
+      <c r="V906" s="2"/>
+      <c r="W906" s="2"/>
+      <c r="X906" s="2"/>
+      <c r="Y906" s="2"/>
+      <c r="Z906" s="2"/>
+    </row>
+    <row r="907" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A907" s="11"/>
+      <c r="B907" s="2"/>
+      <c r="C907" s="2"/>
+      <c r="D907" s="2"/>
+      <c r="E907" s="2"/>
+      <c r="F907" s="2"/>
+      <c r="G907" s="2"/>
+      <c r="H907" s="2"/>
+      <c r="I907" s="2"/>
+      <c r="J907" s="2"/>
+      <c r="K907" s="2"/>
+      <c r="L907" s="2"/>
+      <c r="M907" s="2"/>
+      <c r="N907" s="2"/>
+      <c r="O907" s="2"/>
+      <c r="P907" s="3"/>
+      <c r="Q907" s="3"/>
+      <c r="R907" s="2"/>
+      <c r="S907" s="2"/>
+      <c r="T907" s="2"/>
+      <c r="U907" s="2"/>
+      <c r="V907" s="2"/>
+      <c r="W907" s="2"/>
+      <c r="X907" s="2"/>
+      <c r="Y907" s="2"/>
+      <c r="Z907" s="2"/>
+    </row>
+    <row r="908" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A908" s="11"/>
+      <c r="B908" s="2"/>
+      <c r="C908" s="2"/>
+      <c r="D908" s="2"/>
+      <c r="E908" s="2"/>
+      <c r="F908" s="2"/>
+      <c r="G908" s="2"/>
+      <c r="H908" s="2"/>
+      <c r="I908" s="2"/>
+      <c r="J908" s="2"/>
+      <c r="K908" s="2"/>
+      <c r="L908" s="2"/>
+      <c r="M908" s="2"/>
+      <c r="N908" s="2"/>
+      <c r="O908" s="2"/>
+      <c r="P908" s="3"/>
+      <c r="Q908" s="3"/>
+      <c r="R908" s="2"/>
+      <c r="S908" s="2"/>
+      <c r="T908" s="2"/>
+      <c r="U908" s="2"/>
+      <c r="V908" s="2"/>
+      <c r="W908" s="2"/>
+      <c r="X908" s="2"/>
+      <c r="Y908" s="2"/>
+      <c r="Z908" s="2"/>
+    </row>
+    <row r="909" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A909" s="11"/>
+      <c r="B909" s="2"/>
+      <c r="C909" s="2"/>
+      <c r="D909" s="2"/>
+      <c r="E909" s="2"/>
+      <c r="F909" s="2"/>
+      <c r="G909" s="2"/>
+      <c r="H909" s="2"/>
+      <c r="I909" s="2"/>
+      <c r="J909" s="2"/>
+      <c r="K909" s="2"/>
+      <c r="L909" s="2"/>
+      <c r="M909" s="2"/>
+      <c r="N909" s="2"/>
+      <c r="O909" s="2"/>
+      <c r="P909" s="3"/>
+      <c r="Q909" s="3"/>
+      <c r="R909" s="2"/>
+      <c r="S909" s="2"/>
+      <c r="T909" s="2"/>
+      <c r="U909" s="2"/>
+      <c r="V909" s="2"/>
+      <c r="W909" s="2"/>
+      <c r="X909" s="2"/>
+      <c r="Y909" s="2"/>
+      <c r="Z909" s="2"/>
+    </row>
+    <row r="910" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A910" s="11"/>
+      <c r="B910" s="2"/>
+      <c r="C910" s="2"/>
+      <c r="D910" s="2"/>
+      <c r="E910" s="2"/>
+      <c r="F910" s="2"/>
+      <c r="G910" s="2"/>
+      <c r="H910" s="2"/>
+      <c r="I910" s="2"/>
+      <c r="J910" s="2"/>
+      <c r="K910" s="2"/>
+      <c r="L910" s="2"/>
+      <c r="M910" s="2"/>
+      <c r="N910" s="2"/>
+      <c r="O910" s="2"/>
+      <c r="P910" s="3"/>
+      <c r="Q910" s="3"/>
+      <c r="R910" s="2"/>
+      <c r="S910" s="2"/>
+      <c r="T910" s="2"/>
+      <c r="U910" s="2"/>
+      <c r="V910" s="2"/>
+      <c r="W910" s="2"/>
+      <c r="X910" s="2"/>
+      <c r="Y910" s="2"/>
+      <c r="Z910" s="2"/>
+    </row>
+    <row r="911" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A911" s="11"/>
+      <c r="B911" s="2"/>
+      <c r="C911" s="2"/>
+      <c r="D911" s="2"/>
+      <c r="E911" s="2"/>
+      <c r="F911" s="2"/>
+      <c r="G911" s="2"/>
+      <c r="H911" s="2"/>
+      <c r="I911" s="2"/>
+      <c r="J911" s="2"/>
+      <c r="K911" s="2"/>
+      <c r="L911" s="2"/>
+      <c r="M911" s="2"/>
+      <c r="N911" s="2"/>
+      <c r="O911" s="2"/>
+      <c r="P911" s="3"/>
+      <c r="Q911" s="3"/>
+      <c r="R911" s="2"/>
+      <c r="S911" s="2"/>
+      <c r="T911" s="2"/>
+      <c r="U911" s="2"/>
+      <c r="V911" s="2"/>
+      <c r="W911" s="2"/>
+      <c r="X911" s="2"/>
+      <c r="Y911" s="2"/>
+      <c r="Z911" s="2"/>
+    </row>
+    <row r="912" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A912" s="11"/>
+      <c r="B912" s="2"/>
+      <c r="C912" s="2"/>
+      <c r="D912" s="2"/>
+      <c r="E912" s="2"/>
+      <c r="F912" s="2"/>
+      <c r="G912" s="2"/>
+      <c r="H912" s="2"/>
+      <c r="I912" s="2"/>
+      <c r="J912" s="2"/>
+      <c r="K912" s="2"/>
+      <c r="L912" s="2"/>
+      <c r="M912" s="2"/>
+      <c r="N912" s="2"/>
+      <c r="O912" s="2"/>
+      <c r="P912" s="3"/>
+      <c r="Q912" s="3"/>
+      <c r="R912" s="2"/>
+      <c r="S912" s="2"/>
+      <c r="T912" s="2"/>
+      <c r="U912" s="2"/>
+      <c r="V912" s="2"/>
+      <c r="W912" s="2"/>
+      <c r="X912" s="2"/>
+      <c r="Y912" s="2"/>
+      <c r="Z912" s="2"/>
+    </row>
+    <row r="913" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A913" s="11"/>
+      <c r="B913" s="2"/>
+      <c r="C913" s="2"/>
+      <c r="D913" s="2"/>
+      <c r="E913" s="2"/>
+      <c r="F913" s="2"/>
+      <c r="G913" s="2"/>
+      <c r="H913" s="2"/>
+      <c r="I913" s="2"/>
+      <c r="J913" s="2"/>
+      <c r="K913" s="2"/>
+      <c r="L913" s="2"/>
+      <c r="M913" s="2"/>
+      <c r="N913" s="2"/>
+      <c r="O913" s="2"/>
+      <c r="P913" s="3"/>
+      <c r="Q913" s="3"/>
+      <c r="R913" s="2"/>
+      <c r="S913" s="2"/>
+      <c r="T913" s="2"/>
+      <c r="U913" s="2"/>
+      <c r="V913" s="2"/>
+      <c r="W913" s="2"/>
+      <c r="X913" s="2"/>
+      <c r="Y913" s="2"/>
+      <c r="Z913" s="2"/>
+    </row>
+    <row r="914" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A914" s="11"/>
+      <c r="B914" s="2"/>
+      <c r="C914" s="2"/>
+      <c r="D914" s="2"/>
+      <c r="E914" s="2"/>
+      <c r="F914" s="2"/>
+      <c r="G914" s="2"/>
+      <c r="H914" s="2"/>
+      <c r="I914" s="2"/>
+      <c r="J914" s="2"/>
+      <c r="K914" s="2"/>
+      <c r="L914" s="2"/>
+      <c r="M914" s="2"/>
+      <c r="N914" s="2"/>
+      <c r="O914" s="2"/>
+      <c r="P914" s="3"/>
+      <c r="Q914" s="3"/>
+      <c r="R914" s="2"/>
+      <c r="S914" s="2"/>
+      <c r="T914" s="2"/>
+      <c r="U914" s="2"/>
+      <c r="V914" s="2"/>
+      <c r="W914" s="2"/>
+      <c r="X914" s="2"/>
+      <c r="Y914" s="2"/>
+      <c r="Z914" s="2"/>
+    </row>
+    <row r="915" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A915" s="11"/>
+      <c r="B915" s="2"/>
+      <c r="C915" s="2"/>
+      <c r="D915" s="2"/>
+      <c r="E915" s="2"/>
+      <c r="F915" s="2"/>
+      <c r="G915" s="2"/>
+      <c r="H915" s="2"/>
+      <c r="I915" s="2"/>
+      <c r="J915" s="2"/>
+      <c r="K915" s="2"/>
+      <c r="L915" s="2"/>
+      <c r="M915" s="2"/>
+      <c r="N915" s="2"/>
+      <c r="O915" s="2"/>
+      <c r="P915" s="3"/>
+      <c r="Q915" s="3"/>
+      <c r="R915" s="2"/>
+      <c r="S915" s="2"/>
+      <c r="T915" s="2"/>
+      <c r="U915" s="2"/>
+      <c r="V915" s="2"/>
+      <c r="W915" s="2"/>
+      <c r="X915" s="2"/>
+      <c r="Y915" s="2"/>
+      <c r="Z915" s="2"/>
+    </row>
+    <row r="916" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A916" s="11"/>
+      <c r="B916" s="2"/>
+      <c r="C916" s="2"/>
+      <c r="D916" s="2"/>
+      <c r="E916" s="2"/>
+      <c r="F916" s="2"/>
+      <c r="G916" s="2"/>
+      <c r="H916" s="2"/>
+      <c r="I916" s="2"/>
+      <c r="J916" s="2"/>
+      <c r="K916" s="2"/>
+      <c r="L916" s="2"/>
+      <c r="M916" s="2"/>
+      <c r="N916" s="2"/>
+      <c r="O916" s="2"/>
+      <c r="P916" s="3"/>
+      <c r="Q916" s="3"/>
+      <c r="R916" s="2"/>
+      <c r="S916" s="2"/>
+      <c r="T916" s="2"/>
+      <c r="U916" s="2"/>
+      <c r="V916" s="2"/>
+      <c r="W916" s="2"/>
+      <c r="X916" s="2"/>
+      <c r="Y916" s="2"/>
+      <c r="Z916" s="2"/>
+    </row>
+    <row r="917" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A917" s="11"/>
+      <c r="B917" s="2"/>
+      <c r="C917" s="2"/>
+      <c r="D917" s="2"/>
+      <c r="E917" s="2"/>
+      <c r="F917" s="2"/>
+      <c r="G917" s="2"/>
+      <c r="H917" s="2"/>
+      <c r="I917" s="2"/>
+      <c r="J917" s="2"/>
+      <c r="K917" s="2"/>
+      <c r="L917" s="2"/>
+      <c r="M917" s="2"/>
+      <c r="N917" s="2"/>
+      <c r="O917" s="2"/>
+      <c r="P917" s="3"/>
+      <c r="Q917" s="3"/>
+      <c r="R917" s="2"/>
+      <c r="S917" s="2"/>
+      <c r="T917" s="2"/>
+      <c r="U917" s="2"/>
+      <c r="V917" s="2"/>
+      <c r="W917" s="2"/>
+      <c r="X917" s="2"/>
+      <c r="Y917" s="2"/>
+      <c r="Z917" s="2"/>
+    </row>
+    <row r="918" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A918" s="11"/>
+      <c r="B918" s="2"/>
+      <c r="C918" s="2"/>
+      <c r="D918" s="2"/>
+      <c r="E918" s="2"/>
+      <c r="F918" s="2"/>
+      <c r="G918" s="2"/>
+      <c r="H918" s="2"/>
+      <c r="I918" s="2"/>
+      <c r="J918" s="2"/>
+      <c r="K918" s="2"/>
+      <c r="L918" s="2"/>
+      <c r="M918" s="2"/>
+      <c r="N918" s="2"/>
+      <c r="O918" s="2"/>
+      <c r="P918" s="3"/>
+      <c r="Q918" s="3"/>
+      <c r="R918" s="2"/>
+      <c r="S918" s="2"/>
+      <c r="T918" s="2"/>
+      <c r="U918" s="2"/>
+      <c r="V918" s="2"/>
+      <c r="W918" s="2"/>
+      <c r="X918" s="2"/>
+      <c r="Y918" s="2"/>
+      <c r="Z918" s="2"/>
+    </row>
+    <row r="919" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A919" s="11"/>
+      <c r="B919" s="2"/>
+      <c r="C919" s="2"/>
+      <c r="D919" s="2"/>
+      <c r="E919" s="2"/>
+      <c r="F919" s="2"/>
+      <c r="G919" s="2"/>
+      <c r="H919" s="2"/>
+      <c r="I919" s="2"/>
+      <c r="J919" s="2"/>
+      <c r="K919" s="2"/>
+      <c r="L919" s="2"/>
+      <c r="M919" s="2"/>
+      <c r="N919" s="2"/>
+      <c r="O919" s="2"/>
+      <c r="P919" s="3"/>
+      <c r="Q919" s="3"/>
+      <c r="R919" s="2"/>
+      <c r="S919" s="2"/>
+      <c r="T919" s="2"/>
+      <c r="U919" s="2"/>
+      <c r="V919" s="2"/>
+      <c r="W919" s="2"/>
+      <c r="X919" s="2"/>
+      <c r="Y919" s="2"/>
+      <c r="Z919" s="2"/>
+    </row>
+    <row r="920" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A920" s="11"/>
+      <c r="B920" s="2"/>
+      <c r="C920" s="2"/>
+      <c r="D920" s="2"/>
+      <c r="E920" s="2"/>
+      <c r="F920" s="2"/>
+      <c r="G920" s="2"/>
+      <c r="H920" s="2"/>
+      <c r="I920" s="2"/>
+      <c r="J920" s="2"/>
+      <c r="K920" s="2"/>
+      <c r="L920" s="2"/>
+      <c r="M920" s="2"/>
+      <c r="N920" s="2"/>
+      <c r="O920" s="2"/>
+      <c r="P920" s="3"/>
+      <c r="Q920" s="3"/>
+      <c r="R920" s="2"/>
+      <c r="S920" s="2"/>
+      <c r="T920" s="2"/>
+      <c r="U920" s="2"/>
+      <c r="V920" s="2"/>
+      <c r="W920" s="2"/>
+      <c r="X920" s="2"/>
+      <c r="Y920" s="2"/>
+      <c r="Z920" s="2"/>
+    </row>
+    <row r="921" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A921" s="11"/>
+      <c r="B921" s="2"/>
+      <c r="C921" s="2"/>
+      <c r="D921" s="2"/>
+      <c r="E921" s="2"/>
+      <c r="F921" s="2"/>
+      <c r="G921" s="2"/>
+      <c r="H921" s="2"/>
+      <c r="I921" s="2"/>
+      <c r="J921" s="2"/>
+      <c r="K921" s="2"/>
+      <c r="L921" s="2"/>
+      <c r="M921" s="2"/>
+      <c r="N921" s="2"/>
+      <c r="O921" s="2"/>
+      <c r="P921" s="3"/>
+      <c r="Q921" s="3"/>
+      <c r="R921" s="2"/>
+      <c r="S921" s="2"/>
+      <c r="T921" s="2"/>
+      <c r="U921" s="2"/>
+      <c r="V921" s="2"/>
+      <c r="W921" s="2"/>
+      <c r="X921" s="2"/>
+      <c r="Y921" s="2"/>
+      <c r="Z921" s="2"/>
+    </row>
+    <row r="922" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A922" s="11"/>
+      <c r="B922" s="2"/>
+      <c r="C922" s="2"/>
+      <c r="D922" s="2"/>
+      <c r="E922" s="2"/>
+      <c r="F922" s="2"/>
+      <c r="G922" s="2"/>
+      <c r="H922" s="2"/>
+      <c r="I922" s="2"/>
+      <c r="J922" s="2"/>
+      <c r="K922" s="2"/>
+      <c r="L922" s="2"/>
+      <c r="M922" s="2"/>
+      <c r="N922" s="2"/>
+      <c r="O922" s="2"/>
+      <c r="P922" s="3"/>
+      <c r="Q922" s="3"/>
+      <c r="R922" s="2"/>
+      <c r="S922" s="2"/>
+      <c r="T922" s="2"/>
+      <c r="U922" s="2"/>
+      <c r="V922" s="2"/>
+      <c r="W922" s="2"/>
+      <c r="X922" s="2"/>
+      <c r="Y922" s="2"/>
+      <c r="Z922" s="2"/>
+    </row>
+    <row r="923" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A923" s="11"/>
+      <c r="B923" s="2"/>
+      <c r="C923" s="2"/>
+      <c r="D923" s="2"/>
+      <c r="E923" s="2"/>
+      <c r="F923" s="2"/>
+      <c r="G923" s="2"/>
+      <c r="H923" s="2"/>
+      <c r="I923" s="2"/>
+      <c r="J923" s="2"/>
+      <c r="K923" s="2"/>
+      <c r="L923" s="2"/>
+      <c r="M923" s="2"/>
+      <c r="N923" s="2"/>
+      <c r="O923" s="2"/>
+      <c r="P923" s="3"/>
+      <c r="Q923" s="3"/>
+      <c r="R923" s="2"/>
+      <c r="S923" s="2"/>
+      <c r="T923" s="2"/>
+      <c r="U923" s="2"/>
+      <c r="V923" s="2"/>
+      <c r="W923" s="2"/>
+      <c r="X923" s="2"/>
+      <c r="Y923" s="2"/>
+      <c r="Z923" s="2"/>
+    </row>
+    <row r="924" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A924" s="11"/>
+      <c r="B924" s="2"/>
+      <c r="C924" s="2"/>
+      <c r="D924" s="2"/>
+      <c r="E924" s="2"/>
+      <c r="F924" s="2"/>
+      <c r="G924" s="2"/>
+      <c r="H924" s="2"/>
+      <c r="I924" s="2"/>
+      <c r="J924" s="2"/>
+      <c r="K924" s="2"/>
+      <c r="L924" s="2"/>
+      <c r="M924" s="2"/>
+      <c r="N924" s="2"/>
+      <c r="O924" s="2"/>
+      <c r="P924" s="3"/>
+      <c r="Q924" s="3"/>
+      <c r="R924" s="2"/>
+      <c r="S924" s="2"/>
+      <c r="T924" s="2"/>
+      <c r="U924" s="2"/>
+      <c r="V924" s="2"/>
+      <c r="W924" s="2"/>
+      <c r="X924" s="2"/>
+      <c r="Y924" s="2"/>
+      <c r="Z924" s="2"/>
+    </row>
+    <row r="925" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A925" s="11"/>
+      <c r="B925" s="2"/>
+      <c r="C925" s="2"/>
+      <c r="D925" s="2"/>
+      <c r="E925" s="2"/>
+      <c r="F925" s="2"/>
+      <c r="G925" s="2"/>
+      <c r="H925" s="2"/>
+      <c r="I925" s="2"/>
+      <c r="J925" s="2"/>
+      <c r="K925" s="2"/>
+      <c r="L925" s="2"/>
+      <c r="M925" s="2"/>
+      <c r="N925" s="2"/>
+      <c r="O925" s="2"/>
+      <c r="P925" s="3"/>
+      <c r="Q925" s="3"/>
+      <c r="R925" s="2"/>
+      <c r="S925" s="2"/>
+      <c r="T925" s="2"/>
+      <c r="U925" s="2"/>
+      <c r="V925" s="2"/>
+      <c r="W925" s="2"/>
+      <c r="X925" s="2"/>
+      <c r="Y925" s="2"/>
+      <c r="Z925" s="2"/>
+    </row>
+    <row r="926" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A926" s="11"/>
+      <c r="B926" s="2"/>
+      <c r="C926" s="2"/>
+      <c r="D926" s="2"/>
+      <c r="E926" s="2"/>
+      <c r="F926" s="2"/>
+      <c r="G926" s="2"/>
+      <c r="H926" s="2"/>
+      <c r="I926" s="2"/>
+      <c r="J926" s="2"/>
+      <c r="K926" s="2"/>
+      <c r="L926" s="2"/>
+      <c r="M926" s="2"/>
+      <c r="N926" s="2"/>
+      <c r="O926" s="2"/>
+      <c r="P926" s="3"/>
+      <c r="Q926" s="3"/>
+      <c r="R926" s="2"/>
+      <c r="S926" s="2"/>
+      <c r="T926" s="2"/>
+      <c r="U926" s="2"/>
+      <c r="V926" s="2"/>
+      <c r="W926" s="2"/>
+      <c r="X926" s="2"/>
+      <c r="Y926" s="2"/>
+      <c r="Z926" s="2"/>
+    </row>
+    <row r="927" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A927" s="11"/>
+      <c r="B927" s="2"/>
+      <c r="C927" s="2"/>
+      <c r="D927" s="2"/>
+      <c r="E927" s="2"/>
+      <c r="F927" s="2"/>
+      <c r="G927" s="2"/>
+      <c r="H927" s="2"/>
+      <c r="I927" s="2"/>
+      <c r="J927" s="2"/>
+      <c r="K927" s="2"/>
+      <c r="L927" s="2"/>
+      <c r="M927" s="2"/>
+      <c r="N927" s="2"/>
+      <c r="O927" s="2"/>
+      <c r="P927" s="3"/>
+      <c r="Q927" s="3"/>
+      <c r="R927" s="2"/>
+      <c r="S927" s="2"/>
+      <c r="T927" s="2"/>
+      <c r="U927" s="2"/>
+      <c r="V927" s="2"/>
+      <c r="W927" s="2"/>
+      <c r="X927" s="2"/>
+      <c r="Y927" s="2"/>
+      <c r="Z927" s="2"/>
+    </row>
+    <row r="928" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A928" s="11"/>
+      <c r="B928" s="2"/>
+      <c r="C928" s="2"/>
+      <c r="D928" s="2"/>
+      <c r="E928" s="2"/>
+      <c r="F928" s="2"/>
+      <c r="G928" s="2"/>
+      <c r="H928" s="2"/>
+      <c r="I928" s="2"/>
+      <c r="J928" s="2"/>
+      <c r="K928" s="2"/>
+      <c r="L928" s="2"/>
+      <c r="M928" s="2"/>
+      <c r="N928" s="2"/>
+      <c r="O928" s="2"/>
+      <c r="P928" s="3"/>
+      <c r="Q928" s="3"/>
+      <c r="R928" s="2"/>
+      <c r="S928" s="2"/>
+      <c r="T928" s="2"/>
+      <c r="U928" s="2"/>
+      <c r="V928" s="2"/>
+      <c r="W928" s="2"/>
+      <c r="X928" s="2"/>
+      <c r="Y928" s="2"/>
+      <c r="Z928" s="2"/>
+    </row>
+    <row r="929" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A929" s="11"/>
+      <c r="B929" s="2"/>
+      <c r="C929" s="2"/>
+      <c r="D929" s="2"/>
+      <c r="E929" s="2"/>
+      <c r="F929" s="2"/>
+      <c r="G929" s="2"/>
+      <c r="H929" s="2"/>
+      <c r="I929" s="2"/>
+      <c r="J929" s="2"/>
+      <c r="K929" s="2"/>
+      <c r="L929" s="2"/>
+      <c r="M929" s="2"/>
+      <c r="N929" s="2"/>
+      <c r="O929" s="2"/>
+      <c r="P929" s="3"/>
+      <c r="Q929" s="3"/>
+      <c r="R929" s="2"/>
+      <c r="S929" s="2"/>
+      <c r="T929" s="2"/>
+      <c r="U929" s="2"/>
+      <c r="V929" s="2"/>
+      <c r="W929" s="2"/>
+      <c r="X929" s="2"/>
+      <c r="Y929" s="2"/>
+      <c r="Z929" s="2"/>
+    </row>
+    <row r="930" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A930" s="11"/>
+      <c r="B930" s="2"/>
+      <c r="C930" s="2"/>
+      <c r="D930" s="2"/>
+      <c r="E930" s="2"/>
+      <c r="F930" s="2"/>
+      <c r="G930" s="2"/>
+      <c r="H930" s="2"/>
+      <c r="I930" s="2"/>
+      <c r="J930" s="2"/>
+      <c r="K930" s="2"/>
+      <c r="L930" s="2"/>
+      <c r="M930" s="2"/>
+      <c r="N930" s="2"/>
+      <c r="O930" s="2"/>
+      <c r="P930" s="3"/>
+      <c r="Q930" s="3"/>
+      <c r="R930" s="2"/>
+      <c r="S930" s="2"/>
+      <c r="T930" s="2"/>
+      <c r="U930" s="2"/>
+      <c r="V930" s="2"/>
+      <c r="W930" s="2"/>
+      <c r="X930" s="2"/>
+      <c r="Y930" s="2"/>
+      <c r="Z930" s="2"/>
+    </row>
+    <row r="931" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A931" s="11"/>
+      <c r="B931" s="2"/>
+      <c r="C931" s="2"/>
+      <c r="D931" s="2"/>
+      <c r="E931" s="2"/>
+      <c r="F931" s="2"/>
+      <c r="G931" s="2"/>
+      <c r="H931" s="2"/>
+      <c r="I931" s="2"/>
+      <c r="J931" s="2"/>
+      <c r="K931" s="2"/>
+      <c r="L931" s="2"/>
+      <c r="M931" s="2"/>
+      <c r="N931" s="2"/>
+      <c r="O931" s="2"/>
+      <c r="P931" s="3"/>
+      <c r="Q931" s="3"/>
+      <c r="R931" s="2"/>
+      <c r="S931" s="2"/>
+      <c r="T931" s="2"/>
+      <c r="U931" s="2"/>
+      <c r="V931" s="2"/>
+      <c r="W931" s="2"/>
+      <c r="X931" s="2"/>
+      <c r="Y931" s="2"/>
+      <c r="Z931" s="2"/>
+    </row>
+    <row r="932" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A932" s="11"/>
+      <c r="B932" s="2"/>
+      <c r="C932" s="2"/>
+      <c r="D932" s="2"/>
+      <c r="E932" s="2"/>
+      <c r="F932" s="2"/>
+      <c r="G932" s="2"/>
+      <c r="H932" s="2"/>
+      <c r="I932" s="2"/>
+      <c r="J932" s="2"/>
+      <c r="K932" s="2"/>
+      <c r="L932" s="2"/>
+      <c r="M932" s="2"/>
+      <c r="N932" s="2"/>
+      <c r="O932" s="2"/>
+      <c r="P932" s="3"/>
+      <c r="Q932" s="3"/>
+      <c r="R932" s="2"/>
+      <c r="S932" s="2"/>
+      <c r="T932" s="2"/>
+      <c r="U932" s="2"/>
+      <c r="V932" s="2"/>
+      <c r="W932" s="2"/>
+      <c r="X932" s="2"/>
+      <c r="Y932" s="2"/>
+      <c r="Z932" s="2"/>
+    </row>
+    <row r="933" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A933" s="11"/>
+      <c r="B933" s="2"/>
+      <c r="C933" s="2"/>
+      <c r="D933" s="2"/>
+      <c r="E933" s="2"/>
+      <c r="F933" s="2"/>
+      <c r="G933" s="2"/>
+      <c r="H933" s="2"/>
+      <c r="I933" s="2"/>
+      <c r="J933" s="2"/>
+      <c r="K933" s="2"/>
+      <c r="L933" s="2"/>
+      <c r="M933" s="2"/>
+      <c r="N933" s="2"/>
+      <c r="O933" s="2"/>
+      <c r="P933" s="3"/>
+      <c r="Q933" s="3"/>
+      <c r="R933" s="2"/>
+      <c r="S933" s="2"/>
+      <c r="T933" s="2"/>
+      <c r="U933" s="2"/>
+      <c r="V933" s="2"/>
+      <c r="W933" s="2"/>
+      <c r="X933" s="2"/>
+      <c r="Y933" s="2"/>
+      <c r="Z933" s="2"/>
+    </row>
+    <row r="934" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A934" s="11"/>
+      <c r="B934" s="2"/>
+      <c r="C934" s="2"/>
+      <c r="D934" s="2"/>
+      <c r="E934" s="2"/>
+      <c r="F934" s="2"/>
+      <c r="G934" s="2"/>
+      <c r="H934" s="2"/>
+      <c r="I934" s="2"/>
+      <c r="J934" s="2"/>
+      <c r="K934" s="2"/>
+      <c r="L934" s="2"/>
+      <c r="M934" s="2"/>
+      <c r="N934" s="2"/>
+      <c r="O934" s="2"/>
+      <c r="P934" s="3"/>
+      <c r="Q934" s="3"/>
+      <c r="R934" s="2"/>
+      <c r="S934" s="2"/>
+      <c r="T934" s="2"/>
+      <c r="U934" s="2"/>
+      <c r="V934" s="2"/>
+      <c r="W934" s="2"/>
+      <c r="X934" s="2"/>
+      <c r="Y934" s="2"/>
+      <c r="Z934" s="2"/>
+    </row>
+    <row r="935" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A935" s="11"/>
+      <c r="B935" s="2"/>
+      <c r="C935" s="2"/>
+      <c r="D935" s="2"/>
+      <c r="E935" s="2"/>
+      <c r="F935" s="2"/>
+      <c r="G935" s="2"/>
+      <c r="H935" s="2"/>
+      <c r="I935" s="2"/>
+      <c r="J935" s="2"/>
+      <c r="K935" s="2"/>
+      <c r="L935" s="2"/>
+      <c r="M935" s="2"/>
+      <c r="N935" s="2"/>
+      <c r="O935" s="2"/>
+      <c r="P935" s="3"/>
+      <c r="Q935" s="3"/>
+      <c r="R935" s="2"/>
+      <c r="S935" s="2"/>
+      <c r="T935" s="2"/>
+      <c r="U935" s="2"/>
+      <c r="V935" s="2"/>
+      <c r="W935" s="2"/>
+      <c r="X935" s="2"/>
+      <c r="Y935" s="2"/>
+      <c r="Z935" s="2"/>
+    </row>
+    <row r="936" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A936" s="11"/>
+      <c r="B936" s="2"/>
+      <c r="C936" s="2"/>
+      <c r="D936" s="2"/>
+      <c r="E936" s="2"/>
+      <c r="F936" s="2"/>
+      <c r="G936" s="2"/>
+      <c r="H936" s="2"/>
+      <c r="I936" s="2"/>
+      <c r="J936" s="2"/>
+      <c r="K936" s="2"/>
+      <c r="L936" s="2"/>
+      <c r="M936" s="2"/>
+      <c r="N936" s="2"/>
+      <c r="O936" s="2"/>
+      <c r="P936" s="3"/>
+      <c r="Q936" s="3"/>
+      <c r="R936" s="2"/>
+      <c r="S936" s="2"/>
+      <c r="T936" s="2"/>
+      <c r="U936" s="2"/>
+      <c r="V936" s="2"/>
+      <c r="W936" s="2"/>
+      <c r="X936" s="2"/>
+      <c r="Y936" s="2"/>
+      <c r="Z936" s="2"/>
+    </row>
+    <row r="937" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A937" s="11"/>
+      <c r="B937" s="2"/>
+      <c r="C937" s="2"/>
+      <c r="D937" s="2"/>
+      <c r="E937" s="2"/>
+      <c r="F937" s="2"/>
+      <c r="G937" s="2"/>
+      <c r="H937" s="2"/>
+      <c r="I937" s="2"/>
+      <c r="J937" s="2"/>
+      <c r="K937" s="2"/>
+      <c r="L937" s="2"/>
+      <c r="M937" s="2"/>
+      <c r="N937" s="2"/>
+      <c r="O937" s="2"/>
+      <c r="P937" s="3"/>
+      <c r="Q937" s="3"/>
+      <c r="R937" s="2"/>
+      <c r="S937" s="2"/>
+      <c r="T937" s="2"/>
+      <c r="U937" s="2"/>
+      <c r="V937" s="2"/>
+      <c r="W937" s="2"/>
+      <c r="X937" s="2"/>
+      <c r="Y937" s="2"/>
+      <c r="Z937" s="2"/>
+    </row>
+    <row r="938" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A938" s="11"/>
+      <c r="B938" s="2"/>
+      <c r="C938" s="2"/>
+      <c r="D938" s="2"/>
+      <c r="E938" s="2"/>
+      <c r="F938" s="2"/>
+      <c r="G938" s="2"/>
+      <c r="H938" s="2"/>
+      <c r="I938" s="2"/>
+      <c r="J938" s="2"/>
+      <c r="K938" s="2"/>
+      <c r="L938" s="2"/>
+      <c r="M938" s="2"/>
+      <c r="N938" s="2"/>
+      <c r="O938" s="2"/>
+      <c r="P938" s="3"/>
+      <c r="Q938" s="3"/>
+      <c r="R938" s="2"/>
+      <c r="S938" s="2"/>
+      <c r="T938" s="2"/>
+      <c r="U938" s="2"/>
+      <c r="V938" s="2"/>
+      <c r="W938" s="2"/>
+      <c r="X938" s="2"/>
+      <c r="Y938" s="2"/>
+      <c r="Z938" s="2"/>
+    </row>
+    <row r="939" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A939" s="11"/>
+      <c r="B939" s="2"/>
+      <c r="C939" s="2"/>
+      <c r="D939" s="2"/>
+      <c r="E939" s="2"/>
+      <c r="F939" s="2"/>
+      <c r="G939" s="2"/>
+      <c r="H939" s="2"/>
+      <c r="I939" s="2"/>
+      <c r="J939" s="2"/>
+      <c r="K939" s="2"/>
+      <c r="L939" s="2"/>
+      <c r="M939" s="2"/>
+      <c r="N939" s="2"/>
+      <c r="O939" s="2"/>
+      <c r="P939" s="3"/>
+      <c r="Q939" s="3"/>
+      <c r="R939" s="2"/>
+      <c r="S939" s="2"/>
+      <c r="T939" s="2"/>
+      <c r="U939" s="2"/>
+      <c r="V939" s="2"/>
+      <c r="W939" s="2"/>
+      <c r="X939" s="2"/>
+      <c r="Y939" s="2"/>
+      <c r="Z939" s="2"/>
+    </row>
+    <row r="940" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A940" s="11"/>
+      <c r="B940" s="2"/>
+      <c r="C940" s="2"/>
+      <c r="D940" s="2"/>
+      <c r="E940" s="2"/>
+      <c r="F940" s="2"/>
+      <c r="G940" s="2"/>
+      <c r="H940" s="2"/>
+      <c r="I940" s="2"/>
+      <c r="J940" s="2"/>
+      <c r="K940" s="2"/>
+      <c r="L940" s="2"/>
+      <c r="M940" s="2"/>
+      <c r="N940" s="2"/>
+      <c r="O940" s="2"/>
+      <c r="P940" s="3"/>
+      <c r="Q940" s="3"/>
+      <c r="R940" s="2"/>
+      <c r="S940" s="2"/>
+      <c r="T940" s="2"/>
+      <c r="U940" s="2"/>
+      <c r="V940" s="2"/>
+      <c r="W940" s="2"/>
+      <c r="X940" s="2"/>
+      <c r="Y940" s="2"/>
+      <c r="Z940" s="2"/>
+    </row>
+    <row r="941" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A941" s="11"/>
+      <c r="B941" s="2"/>
+      <c r="C941" s="2"/>
+      <c r="D941" s="2"/>
+      <c r="E941" s="2"/>
+      <c r="F941" s="2"/>
+      <c r="G941" s="2"/>
+      <c r="H941" s="2"/>
+      <c r="I941" s="2"/>
+      <c r="J941" s="2"/>
+      <c r="K941" s="2"/>
+      <c r="L941" s="2"/>
+      <c r="M941" s="2"/>
+      <c r="N941" s="2"/>
+      <c r="O941" s="2"/>
+      <c r="P941" s="3"/>
+      <c r="Q941" s="3"/>
+      <c r="R941" s="2"/>
+      <c r="S941" s="2"/>
+      <c r="T941" s="2"/>
+      <c r="U941" s="2"/>
+      <c r="V941" s="2"/>
+      <c r="W941" s="2"/>
+      <c r="X941" s="2"/>
+      <c r="Y941" s="2"/>
+      <c r="Z941" s="2"/>
+    </row>
+    <row r="942" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A942" s="11"/>
+      <c r="B942" s="2"/>
+      <c r="C942" s="2"/>
+      <c r="D942" s="2"/>
+      <c r="E942" s="2"/>
+      <c r="F942" s="2"/>
+      <c r="G942" s="2"/>
+      <c r="H942" s="2"/>
+      <c r="I942" s="2"/>
+      <c r="J942" s="2"/>
+      <c r="K942" s="2"/>
+      <c r="L942" s="2"/>
+      <c r="M942" s="2"/>
+      <c r="N942" s="2"/>
+      <c r="O942" s="2"/>
+      <c r="P942" s="3"/>
+      <c r="Q942" s="3"/>
+      <c r="R942" s="2"/>
+      <c r="S942" s="2"/>
+      <c r="T942" s="2"/>
+      <c r="U942" s="2"/>
+      <c r="V942" s="2"/>
+      <c r="W942" s="2"/>
+      <c r="X942" s="2"/>
+      <c r="Y942" s="2"/>
+      <c r="Z942" s="2"/>
+    </row>
+    <row r="943" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A943" s="11"/>
+      <c r="B943" s="2"/>
+      <c r="C943" s="2"/>
+      <c r="D943" s="2"/>
+      <c r="E943" s="2"/>
+      <c r="F943" s="2"/>
+      <c r="G943" s="2"/>
+      <c r="H943" s="2"/>
+      <c r="I943" s="2"/>
+      <c r="J943" s="2"/>
+      <c r="K943" s="2"/>
+      <c r="L943" s="2"/>
+      <c r="M943" s="2"/>
+      <c r="N943" s="2"/>
+      <c r="O943" s="2"/>
+      <c r="P943" s="3"/>
+      <c r="Q943" s="3"/>
+      <c r="R943" s="2"/>
+      <c r="S943" s="2"/>
+      <c r="T943" s="2"/>
+      <c r="U943" s="2"/>
+      <c r="V943" s="2"/>
+      <c r="W943" s="2"/>
+      <c r="X943" s="2"/>
+      <c r="Y943" s="2"/>
+      <c r="Z943" s="2"/>
+    </row>
+    <row r="944" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A944" s="11"/>
+      <c r="B944" s="2"/>
+      <c r="C944" s="2"/>
+      <c r="D944" s="2"/>
+      <c r="E944" s="2"/>
+      <c r="F944" s="2"/>
+      <c r="G944" s="2"/>
+      <c r="H944" s="2"/>
+      <c r="I944" s="2"/>
+      <c r="J944" s="2"/>
+      <c r="K944" s="2"/>
+      <c r="L944" s="2"/>
+      <c r="M944" s="2"/>
+      <c r="N944" s="2"/>
+      <c r="O944" s="2"/>
+      <c r="P944" s="3"/>
+      <c r="Q944" s="3"/>
+      <c r="R944" s="2"/>
+      <c r="S944" s="2"/>
+      <c r="T944" s="2"/>
+      <c r="U944" s="2"/>
+      <c r="V944" s="2"/>
+      <c r="W944" s="2"/>
+      <c r="X944" s="2"/>
+      <c r="Y944" s="2"/>
+      <c r="Z944" s="2"/>
+    </row>
+    <row r="945" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A945" s="11"/>
+      <c r="B945" s="2"/>
+      <c r="C945" s="2"/>
+      <c r="D945" s="2"/>
+      <c r="E945" s="2"/>
+      <c r="F945" s="2"/>
+      <c r="G945" s="2"/>
+      <c r="H945" s="2"/>
+      <c r="I945" s="2"/>
+      <c r="J945" s="2"/>
+      <c r="K945" s="2"/>
+      <c r="L945" s="2"/>
+      <c r="M945" s="2"/>
+      <c r="N945" s="2"/>
+      <c r="O945" s="2"/>
+      <c r="P945" s="3"/>
+      <c r="Q945" s="3"/>
+      <c r="R945" s="2"/>
+      <c r="S945" s="2"/>
+      <c r="T945" s="2"/>
+      <c r="U945" s="2"/>
+      <c r="V945" s="2"/>
+      <c r="W945" s="2"/>
+      <c r="X945" s="2"/>
+      <c r="Y945" s="2"/>
+      <c r="Z945" s="2"/>
+    </row>
+    <row r="946" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A946" s="11"/>
+      <c r="B946" s="2"/>
+      <c r="C946" s="2"/>
+      <c r="D946" s="2"/>
+      <c r="E946" s="2"/>
+      <c r="F946" s="2"/>
+      <c r="G946" s="2"/>
+      <c r="H946" s="2"/>
+      <c r="I946" s="2"/>
+      <c r="J946" s="2"/>
+      <c r="K946" s="2"/>
+      <c r="L946" s="2"/>
+      <c r="M946" s="2"/>
+      <c r="N946" s="2"/>
+      <c r="O946" s="2"/>
+      <c r="P946" s="3"/>
+      <c r="Q946" s="3"/>
+      <c r="R946" s="2"/>
+      <c r="S946" s="2"/>
+      <c r="T946" s="2"/>
+      <c r="U946" s="2"/>
+      <c r="V946" s="2"/>
+      <c r="W946" s="2"/>
+      <c r="X946" s="2"/>
+      <c r="Y946" s="2"/>
+      <c r="Z946" s="2"/>
+    </row>
+    <row r="947" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A947" s="11"/>
+      <c r="B947" s="2"/>
+      <c r="C947" s="2"/>
+      <c r="D947" s="2"/>
+      <c r="E947" s="2"/>
+      <c r="F947" s="2"/>
+      <c r="G947" s="2"/>
+      <c r="H947" s="2"/>
+      <c r="I947" s="2"/>
+      <c r="J947" s="2"/>
+      <c r="K947" s="2"/>
+      <c r="L947" s="2"/>
+      <c r="M947" s="2"/>
+      <c r="N947" s="2"/>
+      <c r="O947" s="2"/>
+      <c r="P947" s="3"/>
+      <c r="Q947" s="3"/>
+      <c r="R947" s="2"/>
+      <c r="S947" s="2"/>
+      <c r="T947" s="2"/>
+      <c r="U947" s="2"/>
+      <c r="V947" s="2"/>
+      <c r="W947" s="2"/>
+      <c r="X947" s="2"/>
+      <c r="Y947" s="2"/>
+      <c r="Z947" s="2"/>
+    </row>
+    <row r="948" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A948" s="11"/>
+      <c r="B948" s="2"/>
+      <c r="C948" s="2"/>
+      <c r="D948" s="2"/>
+      <c r="E948" s="2"/>
+      <c r="F948" s="2"/>
+      <c r="G948" s="2"/>
+      <c r="H948" s="2"/>
+      <c r="I948" s="2"/>
+      <c r="J948" s="2"/>
+      <c r="K948" s="2"/>
+      <c r="L948" s="2"/>
+      <c r="M948" s="2"/>
+      <c r="N948" s="2"/>
+      <c r="O948" s="2"/>
+      <c r="P948" s="3"/>
+      <c r="Q948" s="3"/>
+      <c r="R948" s="2"/>
+      <c r="S948" s="2"/>
+      <c r="T948" s="2"/>
+      <c r="U948" s="2"/>
+      <c r="V948" s="2"/>
+      <c r="W948" s="2"/>
+      <c r="X948" s="2"/>
+      <c r="Y948" s="2"/>
+      <c r="Z948" s="2"/>
+    </row>
+    <row r="949" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A949" s="11"/>
+      <c r="B949" s="2"/>
+      <c r="C949" s="2"/>
+      <c r="D949" s="2"/>
+      <c r="E949" s="2"/>
+      <c r="F949" s="2"/>
+      <c r="G949" s="2"/>
+      <c r="H949" s="2"/>
+      <c r="I949" s="2"/>
+      <c r="J949" s="2"/>
+      <c r="K949" s="2"/>
+      <c r="L949" s="2"/>
+      <c r="M949" s="2"/>
+      <c r="N949" s="2"/>
+      <c r="O949" s="2"/>
+      <c r="P949" s="3"/>
+      <c r="Q949" s="3"/>
+      <c r="R949" s="2"/>
+      <c r="S949" s="2"/>
+      <c r="T949" s="2"/>
+      <c r="U949" s="2"/>
+      <c r="V949" s="2"/>
+      <c r="W949" s="2"/>
+      <c r="X949" s="2"/>
+      <c r="Y949" s="2"/>
+      <c r="Z949" s="2"/>
+    </row>
+    <row r="950" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A950" s="11"/>
+      <c r="B950" s="2"/>
+      <c r="C950" s="2"/>
+      <c r="D950" s="2"/>
+      <c r="E950" s="2"/>
+      <c r="F950" s="2"/>
+      <c r="G950" s="2"/>
+      <c r="H950" s="2"/>
+      <c r="I950" s="2"/>
+      <c r="J950" s="2"/>
+      <c r="K950" s="2"/>
+      <c r="L950" s="2"/>
+      <c r="M950" s="2"/>
+      <c r="N950" s="2"/>
+      <c r="O950" s="2"/>
+      <c r="P950" s="3"/>
+      <c r="Q950" s="3"/>
+      <c r="R950" s="2"/>
+      <c r="S950" s="2"/>
+      <c r="T950" s="2"/>
+      <c r="U950" s="2"/>
+      <c r="V950" s="2"/>
+      <c r="W950" s="2"/>
+      <c r="X950" s="2"/>
+      <c r="Y950" s="2"/>
+      <c r="Z950" s="2"/>
+    </row>
+    <row r="951" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A951" s="11"/>
+      <c r="B951" s="2"/>
+      <c r="C951" s="2"/>
+      <c r="D951" s="2"/>
+      <c r="E951" s="2"/>
+      <c r="F951" s="2"/>
+      <c r="G951" s="2"/>
+      <c r="H951" s="2"/>
+      <c r="I951" s="2"/>
+      <c r="J951" s="2"/>
+      <c r="K951" s="2"/>
+      <c r="L951" s="2"/>
+      <c r="M951" s="2"/>
+      <c r="N951" s="2"/>
+      <c r="O951" s="2"/>
+      <c r="P951" s="3"/>
+      <c r="Q951" s="3"/>
+      <c r="R951" s="2"/>
+      <c r="S951" s="2"/>
+      <c r="T951" s="2"/>
+      <c r="U951" s="2"/>
+      <c r="V951" s="2"/>
+      <c r="W951" s="2"/>
+      <c r="X951" s="2"/>
+      <c r="Y951" s="2"/>
+      <c r="Z951" s="2"/>
+    </row>
+    <row r="952" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A952" s="11"/>
+      <c r="B952" s="2"/>
+      <c r="C952" s="2"/>
+      <c r="D952" s="2"/>
+      <c r="E952" s="2"/>
+      <c r="F952" s="2"/>
+      <c r="G952" s="2"/>
+      <c r="H952" s="2"/>
+      <c r="I952" s="2"/>
+      <c r="J952" s="2"/>
+      <c r="K952" s="2"/>
+      <c r="L952" s="2"/>
+      <c r="M952" s="2"/>
+      <c r="N952" s="2"/>
+      <c r="O952" s="2"/>
+      <c r="P952" s="3"/>
+      <c r="Q952" s="3"/>
+      <c r="R952" s="2"/>
+      <c r="S952" s="2"/>
+      <c r="T952" s="2"/>
+      <c r="U952" s="2"/>
+      <c r="V952" s="2"/>
+      <c r="W952" s="2"/>
+      <c r="X952" s="2"/>
+      <c r="Y952" s="2"/>
+      <c r="Z952" s="2"/>
+    </row>
+    <row r="953" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A953" s="11"/>
+      <c r="B953" s="2"/>
+      <c r="C953" s="2"/>
+      <c r="D953" s="2"/>
+      <c r="E953" s="2"/>
+      <c r="F953" s="2"/>
+      <c r="G953" s="2"/>
+      <c r="H953" s="2"/>
+      <c r="I953" s="2"/>
+      <c r="J953" s="2"/>
+      <c r="K953" s="2"/>
+      <c r="L953" s="2"/>
+      <c r="M953" s="2"/>
+      <c r="N953" s="2"/>
+      <c r="O953" s="2"/>
+      <c r="P953" s="3"/>
+      <c r="Q953" s="3"/>
+      <c r="R953" s="2"/>
+      <c r="S953" s="2"/>
+      <c r="T953" s="2"/>
+      <c r="U953" s="2"/>
+      <c r="V953" s="2"/>
+      <c r="W953" s="2"/>
+      <c r="X953" s="2"/>
+      <c r="Y953" s="2"/>
+      <c r="Z953" s="2"/>
+    </row>
+    <row r="954" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A954" s="11"/>
+      <c r="B954" s="2"/>
+      <c r="C954" s="2"/>
+      <c r="D954" s="2"/>
+      <c r="E954" s="2"/>
+      <c r="F954" s="2"/>
+      <c r="G954" s="2"/>
+      <c r="H954" s="2"/>
+      <c r="I954" s="2"/>
+      <c r="J954" s="2"/>
+      <c r="K954" s="2"/>
+      <c r="L954" s="2"/>
+      <c r="M954" s="2"/>
+      <c r="N954" s="2"/>
+      <c r="O954" s="2"/>
+      <c r="P954" s="3"/>
+      <c r="Q954" s="3"/>
+      <c r="R954" s="2"/>
+      <c r="S954" s="2"/>
+      <c r="T954" s="2"/>
+      <c r="U954" s="2"/>
+      <c r="V954" s="2"/>
+      <c r="W954" s="2"/>
+      <c r="X954" s="2"/>
+      <c r="Y954" s="2"/>
+      <c r="Z954" s="2"/>
+    </row>
+    <row r="955" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A955" s="11"/>
+      <c r="B955" s="2"/>
+      <c r="C955" s="2"/>
+      <c r="D955" s="2"/>
+      <c r="E955" s="2"/>
+      <c r="F955" s="2"/>
+      <c r="G955" s="2"/>
+      <c r="H955" s="2"/>
+      <c r="I955" s="2"/>
+      <c r="J955" s="2"/>
+      <c r="K955" s="2"/>
+      <c r="L955" s="2"/>
+      <c r="M955" s="2"/>
+      <c r="N955" s="2"/>
+      <c r="O955" s="2"/>
+      <c r="P955" s="3"/>
+      <c r="Q955" s="3"/>
+      <c r="R955" s="2"/>
+      <c r="S955" s="2"/>
+      <c r="T955" s="2"/>
+      <c r="U955" s="2"/>
+      <c r="V955" s="2"/>
+      <c r="W955" s="2"/>
+      <c r="X955" s="2"/>
+      <c r="Y955" s="2"/>
+      <c r="Z955" s="2"/>
+    </row>
+    <row r="956" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A956" s="11"/>
+      <c r="B956" s="2"/>
+      <c r="C956" s="2"/>
+      <c r="D956" s="2"/>
+      <c r="E956" s="2"/>
+      <c r="F956" s="2"/>
+      <c r="G956" s="2"/>
+      <c r="H956" s="2"/>
+      <c r="I956" s="2"/>
+      <c r="J956" s="2"/>
+      <c r="K956" s="2"/>
+      <c r="L956" s="2"/>
+      <c r="M956" s="2"/>
+      <c r="N956" s="2"/>
+      <c r="O956" s="2"/>
+      <c r="P956" s="3"/>
+      <c r="Q956" s="3"/>
+      <c r="R956" s="2"/>
+      <c r="S956" s="2"/>
+      <c r="T956" s="2"/>
+      <c r="U956" s="2"/>
+      <c r="V956" s="2"/>
+      <c r="W956" s="2"/>
+      <c r="X956" s="2"/>
+      <c r="Y956" s="2"/>
+      <c r="Z956" s="2"/>
+    </row>
+    <row r="957" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A957" s="11"/>
+      <c r="B957" s="2"/>
+      <c r="C957" s="2"/>
+      <c r="D957" s="2"/>
+      <c r="E957" s="2"/>
+      <c r="F957" s="2"/>
+      <c r="G957" s="2"/>
+      <c r="H957" s="2"/>
+      <c r="I957" s="2"/>
+      <c r="J957" s="2"/>
+      <c r="K957" s="2"/>
+      <c r="L957" s="2"/>
+      <c r="M957" s="2"/>
+      <c r="N957" s="2"/>
+      <c r="O957" s="2"/>
+      <c r="P957" s="3"/>
+      <c r="Q957" s="3"/>
+      <c r="R957" s="2"/>
+      <c r="S957" s="2"/>
+      <c r="T957" s="2"/>
+      <c r="U957" s="2"/>
+      <c r="V957" s="2"/>
+      <c r="W957" s="2"/>
+      <c r="X957" s="2"/>
+      <c r="Y957" s="2"/>
+      <c r="Z957" s="2"/>
+    </row>
+    <row r="958" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A958" s="11"/>
+      <c r="B958" s="2"/>
+      <c r="C958" s="2"/>
+      <c r="D958" s="2"/>
+      <c r="E958" s="2"/>
+      <c r="F958" s="2"/>
+      <c r="G958" s="2"/>
+      <c r="H958" s="2"/>
+      <c r="I958" s="2"/>
+      <c r="J958" s="2"/>
+      <c r="K958" s="2"/>
+      <c r="L958" s="2"/>
+      <c r="M958" s="2"/>
+      <c r="N958" s="2"/>
+      <c r="O958" s="2"/>
+      <c r="P958" s="3"/>
+      <c r="Q958" s="3"/>
+      <c r="R958" s="2"/>
+      <c r="S958" s="2"/>
+      <c r="T958" s="2"/>
+      <c r="U958" s="2"/>
+      <c r="V958" s="2"/>
+      <c r="W958" s="2"/>
+      <c r="X958" s="2"/>
+      <c r="Y958" s="2"/>
+      <c r="Z958" s="2"/>
+    </row>
+    <row r="959" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A959" s="11"/>
+      <c r="B959" s="2"/>
+      <c r="C959" s="2"/>
+      <c r="D959" s="2"/>
+      <c r="E959" s="2"/>
+      <c r="F959" s="2"/>
+      <c r="G959" s="2"/>
+      <c r="H959" s="2"/>
+      <c r="I959" s="2"/>
+      <c r="J959" s="2"/>
+      <c r="K959" s="2"/>
+      <c r="L959" s="2"/>
+      <c r="M959" s="2"/>
+      <c r="N959" s="2"/>
+      <c r="O959" s="2"/>
+      <c r="P959" s="3"/>
+      <c r="Q959" s="3"/>
+      <c r="R959" s="2"/>
+      <c r="S959" s="2"/>
+      <c r="T959" s="2"/>
+      <c r="U959" s="2"/>
+      <c r="V959" s="2"/>
+      <c r="W959" s="2"/>
+      <c r="X959" s="2"/>
+      <c r="Y959" s="2"/>
+      <c r="Z959" s="2"/>
+    </row>
+    <row r="960" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A960" s="11"/>
+      <c r="B960" s="2"/>
+      <c r="C960" s="2"/>
+      <c r="D960" s="2"/>
+      <c r="E960" s="2"/>
+      <c r="F960" s="2"/>
+      <c r="G960" s="2"/>
+      <c r="H960" s="2"/>
+      <c r="I960" s="2"/>
+      <c r="J960" s="2"/>
+      <c r="K960" s="2"/>
+      <c r="L960" s="2"/>
+      <c r="M960" s="2"/>
+      <c r="N960" s="2"/>
+      <c r="O960" s="2"/>
+      <c r="P960" s="3"/>
+      <c r="Q960" s="3"/>
+      <c r="R960" s="2"/>
+      <c r="S960" s="2"/>
+      <c r="T960" s="2"/>
+      <c r="U960" s="2"/>
+      <c r="V960" s="2"/>
+      <c r="W960" s="2"/>
+      <c r="X960" s="2"/>
+      <c r="Y960" s="2"/>
+      <c r="Z960" s="2"/>
+    </row>
+    <row r="961" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A961" s="11"/>
+      <c r="B961" s="2"/>
+      <c r="C961" s="2"/>
+      <c r="D961" s="2"/>
+      <c r="E961" s="2"/>
+      <c r="F961" s="2"/>
+      <c r="G961" s="2"/>
+      <c r="H961" s="2"/>
+      <c r="I961" s="2"/>
+      <c r="J961" s="2"/>
+      <c r="K961" s="2"/>
+      <c r="L961" s="2"/>
+      <c r="M961" s="2"/>
+      <c r="N961" s="2"/>
+      <c r="O961" s="2"/>
+      <c r="P961" s="3"/>
+      <c r="Q961" s="3"/>
+      <c r="R961" s="2"/>
+      <c r="S961" s="2"/>
+      <c r="T961" s="2"/>
+      <c r="U961" s="2"/>
+      <c r="V961" s="2"/>
+      <c r="W961" s="2"/>
+      <c r="X961" s="2"/>
+      <c r="Y961" s="2"/>
+      <c r="Z961" s="2"/>
+    </row>
+    <row r="962" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A962" s="11"/>
+      <c r="B962" s="2"/>
+      <c r="C962" s="2"/>
+      <c r="D962" s="2"/>
+      <c r="E962" s="2"/>
+      <c r="F962" s="2"/>
+      <c r="G962" s="2"/>
+      <c r="H962" s="2"/>
+      <c r="I962" s="2"/>
+      <c r="J962" s="2"/>
+      <c r="K962" s="2"/>
+      <c r="L962" s="2"/>
+      <c r="M962" s="2"/>
+      <c r="N962" s="2"/>
+      <c r="O962" s="2"/>
+      <c r="P962" s="3"/>
+      <c r="Q962" s="3"/>
+      <c r="R962" s="2"/>
+      <c r="S962" s="2"/>
+      <c r="T962" s="2"/>
+      <c r="U962" s="2"/>
+      <c r="V962" s="2"/>
+      <c r="W962" s="2"/>
+      <c r="X962" s="2"/>
+      <c r="Y962" s="2"/>
+      <c r="Z962" s="2"/>
+    </row>
+    <row r="963" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A963" s="11"/>
+      <c r="B963" s="2"/>
+      <c r="C963" s="2"/>
+      <c r="D963" s="2"/>
+      <c r="E963" s="2"/>
+      <c r="F963" s="2"/>
+      <c r="G963" s="2"/>
+      <c r="H963" s="2"/>
+      <c r="I963" s="2"/>
+      <c r="J963" s="2"/>
+      <c r="K963" s="2"/>
+      <c r="L963" s="2"/>
+      <c r="M963" s="2"/>
+      <c r="N963" s="2"/>
+      <c r="O963" s="2"/>
+      <c r="P963" s="3"/>
+      <c r="Q963" s="3"/>
+      <c r="R963" s="2"/>
+      <c r="S963" s="2"/>
+      <c r="T963" s="2"/>
+      <c r="U963" s="2"/>
+      <c r="V963" s="2"/>
+      <c r="W963" s="2"/>
+      <c r="X963" s="2"/>
+      <c r="Y963" s="2"/>
+      <c r="Z963" s="2"/>
+    </row>
+    <row r="964" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A964" s="11"/>
+      <c r="B964" s="2"/>
+      <c r="C964" s="2"/>
+      <c r="D964" s="2"/>
+      <c r="E964" s="2"/>
+      <c r="F964" s="2"/>
+      <c r="G964" s="2"/>
+      <c r="H964" s="2"/>
+      <c r="I964" s="2"/>
+      <c r="J964" s="2"/>
+      <c r="K964" s="2"/>
+      <c r="L964" s="2"/>
+      <c r="M964" s="2"/>
+      <c r="N964" s="2"/>
+      <c r="O964" s="2"/>
+      <c r="P964" s="3"/>
+      <c r="Q964" s="3"/>
+      <c r="R964" s="2"/>
+      <c r="S964" s="2"/>
+      <c r="T964" s="2"/>
+      <c r="U964" s="2"/>
+      <c r="V964" s="2"/>
+      <c r="W964" s="2"/>
+      <c r="X964" s="2"/>
+      <c r="Y964" s="2"/>
+      <c r="Z964" s="2"/>
+    </row>
+    <row r="965" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A965" s="11"/>
+      <c r="B965" s="2"/>
+      <c r="C965" s="2"/>
+      <c r="D965" s="2"/>
+      <c r="E965" s="2"/>
+      <c r="F965" s="2"/>
+      <c r="G965" s="2"/>
+      <c r="H965" s="2"/>
+      <c r="I965" s="2"/>
+      <c r="J965" s="2"/>
+      <c r="K965" s="2"/>
+      <c r="L965" s="2"/>
+      <c r="M965" s="2"/>
+      <c r="N965" s="2"/>
+      <c r="O965" s="2"/>
+      <c r="P965" s="3"/>
+      <c r="Q965" s="3"/>
+      <c r="R965" s="2"/>
+      <c r="S965" s="2"/>
+      <c r="T965" s="2"/>
+      <c r="U965" s="2"/>
+      <c r="V965" s="2"/>
+      <c r="W965" s="2"/>
+      <c r="X965" s="2"/>
+      <c r="Y965" s="2"/>
+      <c r="Z965" s="2"/>
+    </row>
+    <row r="966" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A966" s="11"/>
+      <c r="B966" s="2"/>
+      <c r="C966" s="2"/>
+      <c r="D966" s="2"/>
+      <c r="E966" s="2"/>
+      <c r="F966" s="2"/>
+      <c r="G966" s="2"/>
+      <c r="H966" s="2"/>
+      <c r="I966" s="2"/>
+      <c r="J966" s="2"/>
+      <c r="K966" s="2"/>
+      <c r="L966" s="2"/>
+      <c r="M966" s="2"/>
+      <c r="N966" s="2"/>
+      <c r="O966" s="2"/>
+      <c r="P966" s="3"/>
+      <c r="Q966" s="3"/>
+      <c r="R966" s="2"/>
+      <c r="S966" s="2"/>
+      <c r="T966" s="2"/>
+      <c r="U966" s="2"/>
+      <c r="V966" s="2"/>
+      <c r="W966" s="2"/>
+      <c r="X966" s="2"/>
+      <c r="Y966" s="2"/>
+      <c r="Z966" s="2"/>
+    </row>
+    <row r="967" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A967" s="11"/>
+      <c r="B967" s="2"/>
+      <c r="C967" s="2"/>
+      <c r="D967" s="2"/>
+      <c r="E967" s="2"/>
+      <c r="F967" s="2"/>
+      <c r="G967" s="2"/>
+      <c r="H967" s="2"/>
+      <c r="I967" s="2"/>
+      <c r="J967" s="2"/>
+      <c r="K967" s="2"/>
+      <c r="L967" s="2"/>
+      <c r="M967" s="2"/>
+      <c r="N967" s="2"/>
+      <c r="O967" s="2"/>
+      <c r="P967" s="3"/>
+      <c r="Q967" s="3"/>
+      <c r="R967" s="2"/>
+      <c r="S967" s="2"/>
+      <c r="T967" s="2"/>
+      <c r="U967" s="2"/>
+      <c r="V967" s="2"/>
+      <c r="W967" s="2"/>
+      <c r="X967" s="2"/>
+      <c r="Y967" s="2"/>
+      <c r="Z967" s="2"/>
+    </row>
+    <row r="968" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A968" s="11"/>
+      <c r="B968" s="2"/>
+      <c r="C968" s="2"/>
+      <c r="D968" s="2"/>
+      <c r="E968" s="2"/>
+      <c r="F968" s="2"/>
+      <c r="G968" s="2"/>
+      <c r="H968" s="2"/>
+      <c r="I968" s="2"/>
+      <c r="J968" s="2"/>
+      <c r="K968" s="2"/>
+      <c r="L968" s="2"/>
+      <c r="M968" s="2"/>
+      <c r="N968" s="2"/>
+      <c r="O968" s="2"/>
+      <c r="P968" s="3"/>
+      <c r="Q968" s="3"/>
+      <c r="R968" s="2"/>
+      <c r="S968" s="2"/>
+      <c r="T968" s="2"/>
+      <c r="U968" s="2"/>
+      <c r="V968" s="2"/>
+      <c r="W968" s="2"/>
+      <c r="X968" s="2"/>
+      <c r="Y968" s="2"/>
+      <c r="Z968" s="2"/>
+    </row>
+    <row r="969" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A969" s="11"/>
+      <c r="B969" s="2"/>
+      <c r="C969" s="2"/>
+      <c r="D969" s="2"/>
+      <c r="E969" s="2"/>
+      <c r="F969" s="2"/>
+      <c r="G969" s="2"/>
+      <c r="H969" s="2"/>
+      <c r="I969" s="2"/>
+      <c r="J969" s="2"/>
+      <c r="K969" s="2"/>
+      <c r="L969" s="2"/>
+      <c r="M969" s="2"/>
+      <c r="N969" s="2"/>
+      <c r="O969" s="2"/>
+      <c r="P969" s="3"/>
+      <c r="Q969" s="3"/>
+      <c r="R969" s="2"/>
+      <c r="S969" s="2"/>
+      <c r="T969" s="2"/>
+      <c r="U969" s="2"/>
+      <c r="V969" s="2"/>
+      <c r="W969" s="2"/>
+      <c r="X969" s="2"/>
+      <c r="Y969" s="2"/>
+      <c r="Z969" s="2"/>
+    </row>
+    <row r="970" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A970" s="11"/>
+      <c r="B970" s="2"/>
+      <c r="C970" s="2"/>
+      <c r="D970" s="2"/>
+      <c r="E970" s="2"/>
+      <c r="F970" s="2"/>
+      <c r="G970" s="2"/>
+      <c r="H970" s="2"/>
+      <c r="I970" s="2"/>
+      <c r="J970" s="2"/>
+      <c r="K970" s="2"/>
+      <c r="L970" s="2"/>
+      <c r="M970" s="2"/>
+      <c r="N970" s="2"/>
+      <c r="O970" s="2"/>
+      <c r="P970" s="3"/>
+      <c r="Q970" s="3"/>
+      <c r="R970" s="2"/>
+      <c r="S970" s="2"/>
+      <c r="T970" s="2"/>
+      <c r="U970" s="2"/>
+      <c r="V970" s="2"/>
+      <c r="W970" s="2"/>
+      <c r="X970" s="2"/>
+      <c r="Y970" s="2"/>
+      <c r="Z970" s="2"/>
+    </row>
+    <row r="971" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A971" s="11"/>
+      <c r="B971" s="2"/>
+      <c r="C971" s="2"/>
+      <c r="D971" s="2"/>
+      <c r="E971" s="2"/>
+      <c r="F971" s="2"/>
+      <c r="G971" s="2"/>
+      <c r="H971" s="2"/>
+      <c r="I971" s="2"/>
+      <c r="J971" s="2"/>
+      <c r="K971" s="2"/>
+      <c r="L971" s="2"/>
+      <c r="M971" s="2"/>
+      <c r="N971" s="2"/>
+      <c r="O971" s="2"/>
+      <c r="P971" s="3"/>
+      <c r="Q971" s="3"/>
+      <c r="R971" s="2"/>
+      <c r="S971" s="2"/>
+      <c r="T971" s="2"/>
+      <c r="U971" s="2"/>
+      <c r="V971" s="2"/>
+      <c r="W971" s="2"/>
+      <c r="X971" s="2"/>
+      <c r="Y971" s="2"/>
+      <c r="Z971" s="2"/>
+    </row>
+    <row r="972" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A972" s="11"/>
+      <c r="B972" s="2"/>
+      <c r="C972" s="2"/>
+      <c r="D972" s="2"/>
+      <c r="E972" s="2"/>
+      <c r="F972" s="2"/>
+      <c r="G972" s="2"/>
+      <c r="H972" s="2"/>
+      <c r="I972" s="2"/>
+      <c r="J972" s="2"/>
+      <c r="K972" s="2"/>
+      <c r="L972" s="2"/>
+      <c r="M972" s="2"/>
+      <c r="N972" s="2"/>
+      <c r="O972" s="2"/>
+      <c r="P972" s="3"/>
+      <c r="Q972" s="3"/>
+      <c r="R972" s="2"/>
+      <c r="S972" s="2"/>
+      <c r="T972" s="2"/>
+      <c r="U972" s="2"/>
+      <c r="V972" s="2"/>
+      <c r="W972" s="2"/>
+      <c r="X972" s="2"/>
+      <c r="Y972" s="2"/>
+      <c r="Z972" s="2"/>
+    </row>
+    <row r="973" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A973" s="11"/>
+      <c r="B973" s="2"/>
+      <c r="C973" s="2"/>
+      <c r="D973" s="2"/>
+      <c r="E973" s="2"/>
+      <c r="F973" s="2"/>
+      <c r="G973" s="2"/>
+      <c r="H973" s="2"/>
+      <c r="I973" s="2"/>
+      <c r="J973" s="2"/>
+      <c r="K973" s="2"/>
+      <c r="L973" s="2"/>
+      <c r="M973" s="2"/>
+      <c r="N973" s="2"/>
+      <c r="O973" s="2"/>
+      <c r="P973" s="3"/>
+      <c r="Q973" s="3"/>
+      <c r="R973" s="2"/>
+      <c r="S973" s="2"/>
+      <c r="T973" s="2"/>
+      <c r="U973" s="2"/>
+      <c r="V973" s="2"/>
+      <c r="W973" s="2"/>
+      <c r="X973" s="2"/>
+      <c r="Y973" s="2"/>
+      <c r="Z973" s="2"/>
+    </row>
+    <row r="974" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A974" s="11"/>
+      <c r="B974" s="2"/>
+      <c r="C974" s="2"/>
+      <c r="D974" s="2"/>
+      <c r="E974" s="2"/>
+      <c r="F974" s="2"/>
+      <c r="G974" s="2"/>
+      <c r="H974" s="2"/>
+      <c r="I974" s="2"/>
+      <c r="J974" s="2"/>
+      <c r="K974" s="2"/>
+      <c r="L974" s="2"/>
+      <c r="M974" s="2"/>
+      <c r="N974" s="2"/>
+      <c r="O974" s="2"/>
+      <c r="P974" s="3"/>
+      <c r="Q974" s="3"/>
+      <c r="R974" s="2"/>
+      <c r="S974" s="2"/>
+      <c r="T974" s="2"/>
+      <c r="U974" s="2"/>
+      <c r="V974" s="2"/>
+      <c r="W974" s="2"/>
+      <c r="X974" s="2"/>
+      <c r="Y974" s="2"/>
+      <c r="Z974" s="2"/>
+    </row>
+    <row r="975" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A975" s="11"/>
+      <c r="B975" s="2"/>
+      <c r="C975" s="2"/>
+      <c r="D975" s="2"/>
+      <c r="E975" s="2"/>
+      <c r="F975" s="2"/>
+      <c r="G975" s="2"/>
+      <c r="H975" s="2"/>
+      <c r="I975" s="2"/>
+      <c r="J975" s="2"/>
+      <c r="K975" s="2"/>
+      <c r="L975" s="2"/>
+      <c r="M975" s="2"/>
+      <c r="N975" s="2"/>
+      <c r="O975" s="2"/>
+      <c r="P975" s="3"/>
+      <c r="Q975" s="3"/>
+      <c r="R975" s="2"/>
+      <c r="S975" s="2"/>
+      <c r="T975" s="2"/>
+      <c r="U975" s="2"/>
+      <c r="V975" s="2"/>
+      <c r="W975" s="2"/>
+      <c r="X975" s="2"/>
+      <c r="Y975" s="2"/>
+      <c r="Z975" s="2"/>
+    </row>
+    <row r="976" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A976" s="11"/>
+      <c r="B976" s="2"/>
+      <c r="C976" s="2"/>
+      <c r="D976" s="2"/>
+      <c r="E976" s="2"/>
+      <c r="F976" s="2"/>
+      <c r="G976" s="2"/>
+      <c r="H976" s="2"/>
+      <c r="I976" s="2"/>
+      <c r="J976" s="2"/>
+      <c r="K976" s="2"/>
+      <c r="L976" s="2"/>
+      <c r="M976" s="2"/>
+      <c r="N976" s="2"/>
+      <c r="O976" s="2"/>
+      <c r="P976" s="3"/>
+      <c r="Q976" s="3"/>
+      <c r="R976" s="2"/>
+      <c r="S976" s="2"/>
+      <c r="T976" s="2"/>
+      <c r="U976" s="2"/>
+      <c r="V976" s="2"/>
+      <c r="W976" s="2"/>
+      <c r="X976" s="2"/>
+      <c r="Y976" s="2"/>
+      <c r="Z976" s="2"/>
+    </row>
+    <row r="977" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A977" s="11"/>
+      <c r="B977" s="2"/>
+      <c r="C977" s="2"/>
+      <c r="D977" s="2"/>
+      <c r="E977" s="2"/>
+      <c r="F977" s="2"/>
+      <c r="G977" s="2"/>
+      <c r="H977" s="2"/>
+      <c r="I977" s="2"/>
+      <c r="J977" s="2"/>
+      <c r="K977" s="2"/>
+      <c r="L977" s="2"/>
+      <c r="M977" s="2"/>
+      <c r="N977" s="2"/>
+      <c r="O977" s="2"/>
+      <c r="P977" s="3"/>
+      <c r="Q977" s="3"/>
+      <c r="R977" s="2"/>
+      <c r="S977" s="2"/>
+      <c r="T977" s="2"/>
+      <c r="U977" s="2"/>
+      <c r="V977" s="2"/>
+      <c r="W977" s="2"/>
+      <c r="X977" s="2"/>
+      <c r="Y977" s="2"/>
+      <c r="Z977" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A12:F12"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D8" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D8:D11" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Fixed Price,OSDC,Bodyshop,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>